<commit_message>
update whisp columns excel file
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnell\Documents\GitHub\whisp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CC6670-3A9C-4E9E-A550-7C0430EE1A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC43A7-E222-4A0F-9D82-753F6C558B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{FC85F32F-3F3C-476F-A445-BF878E774111}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="314">
   <si>
     <t>Column name</t>
   </si>
@@ -281,12 +281,6 @@
     <t>Kalischek 2022</t>
   </si>
   <si>
-    <t>Cocoa_bnetd</t>
-  </si>
-  <si>
-    <t>BNETD 2024</t>
-  </si>
-  <si>
     <t>Rubber_FDaP</t>
   </si>
   <si>
@@ -758,15 +752,6 @@
     <t>RADD_after_2020</t>
   </si>
   <si>
-    <t>DIST_after_2020</t>
-  </si>
-  <si>
-    <t>2023-2025</t>
-  </si>
-  <si>
-    <t>Hansen 2025</t>
-  </si>
-  <si>
     <t>GFT_primary</t>
   </si>
   <si>
@@ -860,9 +845,6 @@
     <t>Various national sources combined, date can vary</t>
   </si>
   <si>
-    <t>geojson</t>
-  </si>
-  <si>
     <t>Coordinates of the geometry</t>
   </si>
   <si>
@@ -993,6 +975,9 @@
   </si>
   <si>
     <t>treecover_after_2020</t>
+  </si>
+  <si>
+    <t>geo</t>
   </si>
 </sst>
 </file>
@@ -1384,11 +1369,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A90905-187C-4727-AD42-76516A57CDD0}">
-  <dimension ref="A1:N198"/>
+  <dimension ref="A1:N196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G155" sqref="G155:M155"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2094,7 +2079,7 @@
         <v>2020</v>
       </c>
       <c r="F17" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
@@ -2258,7 +2243,7 @@
         <v>2020</v>
       </c>
       <c r="F21" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G21" t="s">
         <v>19</v>
@@ -2284,7 +2269,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -2293,13 +2278,13 @@
         <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E22">
         <v>2020</v>
       </c>
       <c r="F22" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G22" t="s">
         <v>19</v>
@@ -2340,7 +2325,7 @@
         <v>2020</v>
       </c>
       <c r="F23" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -2416,13 +2401,13 @@
         <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E25">
         <v>2020</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>301</v>
       </c>
       <c r="G25" t="s">
         <v>19</v>
@@ -2457,13 +2442,13 @@
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E26">
         <v>2020</v>
       </c>
       <c r="F26" t="s">
-        <v>307</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s">
         <v>19</v>
@@ -2498,13 +2483,13 @@
         <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E27">
         <v>2020</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G27" t="s">
         <v>19</v>
@@ -2530,7 +2515,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -2539,34 +2524,24 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28">
-        <v>2020</v>
+        <v>2000</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="H28" s="2">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2">
-        <v>1</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>72</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K28" s="2"/>
       <c r="L28" s="2">
-        <v>1</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -2580,10 +2555,10 @@
         <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E29">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="F29" t="s">
         <v>62</v>
@@ -2602,7 +2577,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
@@ -2611,10 +2586,10 @@
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E30">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F30" t="s">
         <v>62</v>
@@ -2633,7 +2608,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -2642,10 +2617,10 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E31">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F31" t="s">
         <v>62</v>
@@ -2664,7 +2639,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
@@ -2673,10 +2648,10 @@
         <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E32">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F32" t="s">
         <v>62</v>
@@ -2695,7 +2670,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
@@ -2704,10 +2679,10 @@
         <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E33">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F33" t="s">
         <v>62</v>
@@ -2726,7 +2701,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
@@ -2735,10 +2710,10 @@
         <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E34">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F34" t="s">
         <v>62</v>
@@ -2757,7 +2732,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
@@ -2766,10 +2741,10 @@
         <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E35">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="F35" t="s">
         <v>62</v>
@@ -2788,7 +2763,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
@@ -2797,10 +2772,10 @@
         <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E36">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F36" t="s">
         <v>62</v>
@@ -2819,7 +2794,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
@@ -2828,10 +2803,10 @@
         <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E37">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="F37" t="s">
         <v>62</v>
@@ -2850,7 +2825,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
@@ -2859,10 +2834,10 @@
         <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E38">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F38" t="s">
         <v>62</v>
@@ -2881,7 +2856,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -2890,10 +2865,10 @@
         <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E39">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F39" t="s">
         <v>62</v>
@@ -2912,7 +2887,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
@@ -2921,10 +2896,10 @@
         <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E40">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="F40" t="s">
         <v>62</v>
@@ -2943,7 +2918,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
@@ -2952,10 +2927,10 @@
         <v>50</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E41">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="F41" t="s">
         <v>62</v>
@@ -2974,7 +2949,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
         <v>15</v>
@@ -2983,10 +2958,10 @@
         <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E42">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="F42" t="s">
         <v>62</v>
@@ -3005,7 +2980,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
         <v>15</v>
@@ -3014,10 +2989,10 @@
         <v>50</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E43">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F43" t="s">
         <v>62</v>
@@ -3036,7 +3011,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
@@ -3045,10 +3020,10 @@
         <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E44">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="F44" t="s">
         <v>62</v>
@@ -3067,7 +3042,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -3076,10 +3051,10 @@
         <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E45">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F45" t="s">
         <v>62</v>
@@ -3098,7 +3073,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
         <v>15</v>
@@ -3107,10 +3082,10 @@
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E46">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F46" t="s">
         <v>62</v>
@@ -3129,7 +3104,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
         <v>15</v>
@@ -3138,10 +3113,10 @@
         <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E47">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F47" t="s">
         <v>62</v>
@@ -3160,7 +3135,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
         <v>15</v>
@@ -3169,10 +3144,10 @@
         <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E48">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F48" t="s">
         <v>62</v>
@@ -3191,7 +3166,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49" t="s">
         <v>15</v>
@@ -3200,10 +3175,10 @@
         <v>50</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E49">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F49" t="s">
         <v>62</v>
@@ -3222,7 +3197,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
         <v>15</v>
@@ -3231,10 +3206,10 @@
         <v>50</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E50">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F50" t="s">
         <v>62</v>
@@ -3253,7 +3228,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
@@ -3262,10 +3237,10 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E51">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F51" t="s">
         <v>62</v>
@@ -3284,7 +3259,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>300</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
@@ -3293,10 +3268,10 @@
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E52">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F52" t="s">
         <v>62</v>
@@ -3315,7 +3290,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>306</v>
+        <v>113</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
@@ -3324,10 +3299,10 @@
         <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="E53">
-        <v>2024</v>
+        <v>2000</v>
       </c>
       <c r="F53" t="s">
         <v>62</v>
@@ -3355,10 +3330,10 @@
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E54">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="F54" t="s">
         <v>62</v>
@@ -3377,7 +3352,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
@@ -3386,10 +3361,10 @@
         <v>50</v>
       </c>
       <c r="D55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E55">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F55" t="s">
         <v>62</v>
@@ -3408,7 +3383,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" t="s">
         <v>15</v>
@@ -3417,10 +3392,10 @@
         <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E56">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F56" t="s">
         <v>62</v>
@@ -3439,7 +3414,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
@@ -3448,10 +3423,10 @@
         <v>50</v>
       </c>
       <c r="D57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E57">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F57" t="s">
         <v>62</v>
@@ -3470,7 +3445,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
@@ -3479,10 +3454,10 @@
         <v>50</v>
       </c>
       <c r="D58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E58">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F58" t="s">
         <v>62</v>
@@ -3501,7 +3476,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -3510,10 +3485,10 @@
         <v>50</v>
       </c>
       <c r="D59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E59">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F59" t="s">
         <v>62</v>
@@ -3532,7 +3507,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -3541,10 +3516,10 @@
         <v>50</v>
       </c>
       <c r="D60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E60">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="F60" t="s">
         <v>62</v>
@@ -3563,7 +3538,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -3572,10 +3547,10 @@
         <v>50</v>
       </c>
       <c r="D61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E61">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F61" t="s">
         <v>62</v>
@@ -3594,7 +3569,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
@@ -3603,10 +3578,10 @@
         <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E62">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="F62" t="s">
         <v>62</v>
@@ -3625,7 +3600,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
@@ -3634,10 +3609,10 @@
         <v>50</v>
       </c>
       <c r="D63" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E63">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F63" t="s">
         <v>62</v>
@@ -3656,7 +3631,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" t="s">
         <v>15</v>
@@ -3665,10 +3640,10 @@
         <v>50</v>
       </c>
       <c r="D64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E64">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F64" t="s">
         <v>62</v>
@@ -3687,7 +3662,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
@@ -3696,10 +3671,10 @@
         <v>50</v>
       </c>
       <c r="D65" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E65">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="F65" t="s">
         <v>62</v>
@@ -3718,7 +3693,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66" t="s">
         <v>15</v>
@@ -3727,10 +3702,10 @@
         <v>50</v>
       </c>
       <c r="D66" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E66">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="F66" t="s">
         <v>62</v>
@@ -3749,7 +3724,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67" t="s">
         <v>15</v>
@@ -3758,10 +3733,10 @@
         <v>50</v>
       </c>
       <c r="D67" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E67">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="F67" t="s">
         <v>62</v>
@@ -3780,7 +3755,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
         <v>15</v>
@@ -3789,10 +3764,10 @@
         <v>50</v>
       </c>
       <c r="D68" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E68">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F68" t="s">
         <v>62</v>
@@ -3811,7 +3786,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s">
         <v>15</v>
@@ -3820,10 +3795,10 @@
         <v>50</v>
       </c>
       <c r="D69" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E69">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="F69" t="s">
         <v>62</v>
@@ -3842,7 +3817,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
@@ -3851,10 +3826,10 @@
         <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E70">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F70" t="s">
         <v>62</v>
@@ -3873,7 +3848,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" t="s">
         <v>15</v>
@@ -3882,10 +3857,10 @@
         <v>50</v>
       </c>
       <c r="D71" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E71">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F71" t="s">
         <v>62</v>
@@ -3904,7 +3879,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72" t="s">
         <v>15</v>
@@ -3913,10 +3888,10 @@
         <v>50</v>
       </c>
       <c r="D72" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E72">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F72" t="s">
         <v>62</v>
@@ -3935,7 +3910,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
@@ -3944,10 +3919,10 @@
         <v>50</v>
       </c>
       <c r="D73" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E73">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F73" t="s">
         <v>62</v>
@@ -3966,7 +3941,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
         <v>15</v>
@@ -3975,10 +3950,10 @@
         <v>50</v>
       </c>
       <c r="D74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E74">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F74" t="s">
         <v>62</v>
@@ -3997,7 +3972,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
         <v>15</v>
@@ -4006,10 +3981,10 @@
         <v>50</v>
       </c>
       <c r="D75" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E75">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F75" t="s">
         <v>62</v>
@@ -4028,7 +4003,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B76" t="s">
         <v>15</v>
@@ -4037,10 +4012,10 @@
         <v>50</v>
       </c>
       <c r="D76" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E76">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F76" t="s">
         <v>62</v>
@@ -4059,7 +4034,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>299</v>
       </c>
       <c r="B77" t="s">
         <v>15</v>
@@ -4068,10 +4043,10 @@
         <v>50</v>
       </c>
       <c r="D77" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E77">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F77" t="s">
         <v>62</v>
@@ -4090,7 +4065,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>305</v>
+        <v>138</v>
       </c>
       <c r="B78" t="s">
         <v>15</v>
@@ -4099,13 +4074,13 @@
         <v>50</v>
       </c>
       <c r="D78" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="E78">
-        <v>2024</v>
+        <v>2001</v>
       </c>
       <c r="F78" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H78" s="2">
         <v>0</v>
@@ -4130,10 +4105,10 @@
         <v>50</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E79">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F79" t="s">
         <v>65</v>
@@ -4152,7 +4127,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B80" t="s">
         <v>15</v>
@@ -4161,10 +4136,10 @@
         <v>50</v>
       </c>
       <c r="D80" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E80">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F80" t="s">
         <v>65</v>
@@ -4183,7 +4158,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B81" t="s">
         <v>15</v>
@@ -4192,10 +4167,10 @@
         <v>50</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E81">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F81" t="s">
         <v>65</v>
@@ -4214,7 +4189,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B82" t="s">
         <v>15</v>
@@ -4223,10 +4198,10 @@
         <v>50</v>
       </c>
       <c r="D82" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E82">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F82" t="s">
         <v>65</v>
@@ -4245,7 +4220,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B83" t="s">
         <v>15</v>
@@ -4254,10 +4229,10 @@
         <v>50</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E83">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F83" t="s">
         <v>65</v>
@@ -4276,7 +4251,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B84" t="s">
         <v>15</v>
@@ -4285,10 +4260,10 @@
         <v>50</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E84">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="F84" t="s">
         <v>65</v>
@@ -4307,7 +4282,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B85" t="s">
         <v>15</v>
@@ -4316,10 +4291,10 @@
         <v>50</v>
       </c>
       <c r="D85" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E85">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F85" t="s">
         <v>65</v>
@@ -4338,7 +4313,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B86" t="s">
         <v>15</v>
@@ -4347,10 +4322,10 @@
         <v>50</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E86">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="F86" t="s">
         <v>65</v>
@@ -4369,7 +4344,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B87" t="s">
         <v>15</v>
@@ -4378,10 +4353,10 @@
         <v>50</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E87">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F87" t="s">
         <v>65</v>
@@ -4400,7 +4375,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B88" t="s">
         <v>15</v>
@@ -4409,10 +4384,10 @@
         <v>50</v>
       </c>
       <c r="D88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E88">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F88" t="s">
         <v>65</v>
@@ -4431,7 +4406,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
         <v>15</v>
@@ -4440,10 +4415,10 @@
         <v>50</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E89">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="F89" t="s">
         <v>65</v>
@@ -4462,7 +4437,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
         <v>15</v>
@@ -4471,10 +4446,10 @@
         <v>50</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E90">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="F90" t="s">
         <v>65</v>
@@ -4493,7 +4468,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B91" t="s">
         <v>15</v>
@@ -4502,10 +4477,10 @@
         <v>50</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E91">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="F91" t="s">
         <v>65</v>
@@ -4524,7 +4499,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B92" t="s">
         <v>15</v>
@@ -4533,10 +4508,10 @@
         <v>50</v>
       </c>
       <c r="D92" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E92">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F92" t="s">
         <v>65</v>
@@ -4555,7 +4530,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B93" t="s">
         <v>15</v>
@@ -4564,10 +4539,10 @@
         <v>50</v>
       </c>
       <c r="D93" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E93">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="F93" t="s">
         <v>65</v>
@@ -4586,7 +4561,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B94" t="s">
         <v>15</v>
@@ -4595,10 +4570,10 @@
         <v>50</v>
       </c>
       <c r="D94" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E94">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F94" t="s">
         <v>65</v>
@@ -4617,7 +4592,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B95" t="s">
         <v>15</v>
@@ -4626,10 +4601,10 @@
         <v>50</v>
       </c>
       <c r="D95" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E95">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F95" t="s">
         <v>65</v>
@@ -4648,7 +4623,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B96" t="s">
         <v>15</v>
@@ -4657,10 +4632,10 @@
         <v>50</v>
       </c>
       <c r="D96" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E96">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F96" t="s">
         <v>65</v>
@@ -4679,7 +4654,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B97" t="s">
         <v>15</v>
@@ -4688,10 +4663,10 @@
         <v>50</v>
       </c>
       <c r="D97" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E97">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F97" t="s">
         <v>65</v>
@@ -4710,7 +4685,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B98" t="s">
         <v>15</v>
@@ -4719,10 +4694,10 @@
         <v>50</v>
       </c>
       <c r="D98" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E98">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F98" t="s">
         <v>65</v>
@@ -4741,7 +4716,7 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B99" t="s">
         <v>15</v>
@@ -4750,10 +4725,10 @@
         <v>50</v>
       </c>
       <c r="D99" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E99">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F99" t="s">
         <v>65</v>
@@ -4772,7 +4747,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B100" t="s">
         <v>15</v>
@@ -4781,10 +4756,10 @@
         <v>50</v>
       </c>
       <c r="D100" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E100">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F100" t="s">
         <v>65</v>
@@ -4803,7 +4778,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>163</v>
+        <v>298</v>
       </c>
       <c r="B101" t="s">
         <v>15</v>
@@ -4812,10 +4787,10 @@
         <v>50</v>
       </c>
       <c r="D101" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E101">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F101" t="s">
         <v>65</v>
@@ -4834,7 +4809,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>304</v>
+        <v>162</v>
       </c>
       <c r="B102" t="s">
         <v>15</v>
@@ -4843,13 +4818,13 @@
         <v>50</v>
       </c>
       <c r="D102" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E102">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="F102" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="H102" s="2">
         <v>0</v>
@@ -4874,13 +4849,13 @@
         <v>50</v>
       </c>
       <c r="D103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E103">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F103" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H103" s="2">
         <v>0</v>
@@ -4896,7 +4871,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B104" t="s">
         <v>15</v>
@@ -4905,13 +4880,13 @@
         <v>50</v>
       </c>
       <c r="D104" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E104">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F104" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H104" s="2">
         <v>0</v>
@@ -4927,7 +4902,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B105" t="s">
         <v>15</v>
@@ -4936,13 +4911,13 @@
         <v>50</v>
       </c>
       <c r="D105" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E105">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F105" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H105" s="2">
         <v>0</v>
@@ -4958,7 +4933,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B106" t="s">
         <v>15</v>
@@ -4967,13 +4942,13 @@
         <v>50</v>
       </c>
       <c r="D106" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E106">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F106" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H106" s="2">
         <v>0</v>
@@ -4989,7 +4964,7 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B107" t="s">
         <v>15</v>
@@ -4998,13 +4973,13 @@
         <v>50</v>
       </c>
       <c r="D107" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E107">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H107" s="2">
         <v>0</v>
@@ -5020,7 +4995,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B108" t="s">
         <v>15</v>
@@ -5029,13 +5004,13 @@
         <v>50</v>
       </c>
       <c r="D108" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E108">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="F108" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H108" s="2">
         <v>0</v>
@@ -5051,22 +5026,22 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>170</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109" t="s">
+        <v>50</v>
+      </c>
+      <c r="D109" t="s">
         <v>171</v>
       </c>
-      <c r="B109" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109" t="s">
-        <v>50</v>
-      </c>
-      <c r="D109" t="s">
-        <v>141</v>
-      </c>
       <c r="E109">
-        <v>2025</v>
+        <v>2001</v>
       </c>
       <c r="F109" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="H109" s="2">
         <v>0</v>
@@ -5082,22 +5057,22 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" t="s">
+        <v>50</v>
+      </c>
+      <c r="D110" t="s">
+        <v>171</v>
+      </c>
+      <c r="E110">
+        <v>2002</v>
+      </c>
+      <c r="F110" t="s">
         <v>172</v>
-      </c>
-      <c r="B110" t="s">
-        <v>15</v>
-      </c>
-      <c r="C110" t="s">
-        <v>50</v>
-      </c>
-      <c r="D110" t="s">
-        <v>173</v>
-      </c>
-      <c r="E110">
-        <v>2001</v>
-      </c>
-      <c r="F110" t="s">
-        <v>174</v>
       </c>
       <c r="H110" s="2">
         <v>0</v>
@@ -5113,7 +5088,7 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B111" t="s">
         <v>15</v>
@@ -5122,13 +5097,13 @@
         <v>50</v>
       </c>
       <c r="D111" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E111">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F111" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H111" s="2">
         <v>0</v>
@@ -5144,7 +5119,7 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
         <v>15</v>
@@ -5153,13 +5128,13 @@
         <v>50</v>
       </c>
       <c r="D112" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E112">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F112" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H112" s="2">
         <v>0</v>
@@ -5175,7 +5150,7 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B113" t="s">
         <v>15</v>
@@ -5184,13 +5159,13 @@
         <v>50</v>
       </c>
       <c r="D113" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E113">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F113" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H113" s="2">
         <v>0</v>
@@ -5206,7 +5181,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B114" t="s">
         <v>15</v>
@@ -5215,13 +5190,13 @@
         <v>50</v>
       </c>
       <c r="D114" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E114">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F114" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H114" s="2">
         <v>0</v>
@@ -5237,7 +5212,7 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B115" t="s">
         <v>15</v>
@@ -5246,13 +5221,13 @@
         <v>50</v>
       </c>
       <c r="D115" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E115">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="F115" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H115" s="2">
         <v>0</v>
@@ -5268,7 +5243,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B116" t="s">
         <v>15</v>
@@ -5277,13 +5252,13 @@
         <v>50</v>
       </c>
       <c r="D116" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E116">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H116" s="2">
         <v>0</v>
@@ -5299,7 +5274,7 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B117" t="s">
         <v>15</v>
@@ -5308,13 +5283,13 @@
         <v>50</v>
       </c>
       <c r="D117" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E117">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="F117" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H117" s="2">
         <v>0</v>
@@ -5330,7 +5305,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B118" t="s">
         <v>15</v>
@@ -5339,13 +5314,13 @@
         <v>50</v>
       </c>
       <c r="D118" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E118">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F118" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H118" s="2">
         <v>0</v>
@@ -5361,7 +5336,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B119" t="s">
         <v>15</v>
@@ -5370,13 +5345,13 @@
         <v>50</v>
       </c>
       <c r="D119" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E119">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F119" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H119" s="2">
         <v>0</v>
@@ -5392,7 +5367,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B120" t="s">
         <v>15</v>
@@ -5401,13 +5376,13 @@
         <v>50</v>
       </c>
       <c r="D120" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E120">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="F120" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H120" s="2">
         <v>0</v>
@@ -5423,7 +5398,7 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B121" t="s">
         <v>15</v>
@@ -5432,13 +5407,13 @@
         <v>50</v>
       </c>
       <c r="D121" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E121">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="F121" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H121" s="2">
         <v>0</v>
@@ -5454,7 +5429,7 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B122" t="s">
         <v>15</v>
@@ -5463,13 +5438,13 @@
         <v>50</v>
       </c>
       <c r="D122" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E122">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="F122" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H122" s="2">
         <v>0</v>
@@ -5485,7 +5460,7 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B123" t="s">
         <v>15</v>
@@ -5494,13 +5469,13 @@
         <v>50</v>
       </c>
       <c r="D123" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E123">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F123" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H123" s="2">
         <v>0</v>
@@ -5516,7 +5491,7 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B124" t="s">
         <v>15</v>
@@ -5525,13 +5500,13 @@
         <v>50</v>
       </c>
       <c r="D124" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E124">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="F124" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H124" s="2">
         <v>0</v>
@@ -5547,7 +5522,7 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B125" t="s">
         <v>15</v>
@@ -5556,13 +5531,13 @@
         <v>50</v>
       </c>
       <c r="D125" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E125">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F125" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H125" s="2">
         <v>0</v>
@@ -5578,7 +5553,7 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B126" t="s">
         <v>15</v>
@@ -5587,13 +5562,13 @@
         <v>50</v>
       </c>
       <c r="D126" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E126">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F126" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H126" s="2">
         <v>0</v>
@@ -5609,7 +5584,7 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B127" t="s">
         <v>15</v>
@@ -5618,13 +5593,13 @@
         <v>50</v>
       </c>
       <c r="D127" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E127">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F127" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H127" s="2">
         <v>0</v>
@@ -5640,7 +5615,7 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B128" t="s">
         <v>15</v>
@@ -5649,13 +5624,13 @@
         <v>50</v>
       </c>
       <c r="D128" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E128">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F128" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H128" s="2">
         <v>0</v>
@@ -5671,22 +5646,22 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
+        <v>192</v>
+      </c>
+      <c r="B129" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" t="s">
+        <v>50</v>
+      </c>
+      <c r="D129" t="s">
+        <v>171</v>
+      </c>
+      <c r="E129">
+        <v>2000</v>
+      </c>
+      <c r="F129" t="s">
         <v>193</v>
-      </c>
-      <c r="B129" t="s">
-        <v>15</v>
-      </c>
-      <c r="C129" t="s">
-        <v>50</v>
-      </c>
-      <c r="D129" t="s">
-        <v>173</v>
-      </c>
-      <c r="E129">
-        <v>2020</v>
-      </c>
-      <c r="F129" t="s">
-        <v>174</v>
       </c>
       <c r="H129" s="2">
         <v>0</v>
@@ -5711,13 +5686,13 @@
         <v>50</v>
       </c>
       <c r="D130" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E130">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="F130" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H130" s="2">
         <v>0</v>
@@ -5733,7 +5708,7 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B131" t="s">
         <v>15</v>
@@ -5742,13 +5717,13 @@
         <v>50</v>
       </c>
       <c r="D131" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E131">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="F131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H131" s="2">
         <v>0</v>
@@ -5764,7 +5739,7 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B132" t="s">
         <v>15</v>
@@ -5773,13 +5748,13 @@
         <v>50</v>
       </c>
       <c r="D132" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E132">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F132" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H132" s="2">
         <v>0</v>
@@ -5795,7 +5770,7 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B133" t="s">
         <v>15</v>
@@ -5804,13 +5779,13 @@
         <v>50</v>
       </c>
       <c r="D133" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E133">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F133" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H133" s="2">
         <v>0</v>
@@ -5826,7 +5801,7 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B134" t="s">
         <v>15</v>
@@ -5835,13 +5810,13 @@
         <v>50</v>
       </c>
       <c r="D134" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E134">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F134" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H134" s="2">
         <v>0</v>
@@ -5857,7 +5832,7 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B135" t="s">
         <v>15</v>
@@ -5866,13 +5841,13 @@
         <v>50</v>
       </c>
       <c r="D135" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E135">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F135" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H135" s="2">
         <v>0</v>
@@ -5888,7 +5863,7 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B136" t="s">
         <v>15</v>
@@ -5897,13 +5872,13 @@
         <v>50</v>
       </c>
       <c r="D136" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E136">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="F136" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H136" s="2">
         <v>0</v>
@@ -5919,7 +5894,7 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B137" t="s">
         <v>15</v>
@@ -5928,13 +5903,13 @@
         <v>50</v>
       </c>
       <c r="D137" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E137">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F137" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H137" s="2">
         <v>0</v>
@@ -5950,7 +5925,7 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B138" t="s">
         <v>15</v>
@@ -5959,13 +5934,13 @@
         <v>50</v>
       </c>
       <c r="D138" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E138">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="F138" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H138" s="2">
         <v>0</v>
@@ -5981,7 +5956,7 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B139" t="s">
         <v>15</v>
@@ -5990,13 +5965,13 @@
         <v>50</v>
       </c>
       <c r="D139" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E139">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F139" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H139" s="2">
         <v>0</v>
@@ -6012,7 +5987,7 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B140" t="s">
         <v>15</v>
@@ -6021,13 +5996,13 @@
         <v>50</v>
       </c>
       <c r="D140" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E140">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F140" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H140" s="2">
         <v>0</v>
@@ -6043,7 +6018,7 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B141" t="s">
         <v>15</v>
@@ -6052,13 +6027,13 @@
         <v>50</v>
       </c>
       <c r="D141" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E141">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="F141" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H141" s="2">
         <v>0</v>
@@ -6074,7 +6049,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B142" t="s">
         <v>15</v>
@@ -6083,13 +6058,13 @@
         <v>50</v>
       </c>
       <c r="D142" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E142">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="F142" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H142" s="2">
         <v>0</v>
@@ -6105,7 +6080,7 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B143" t="s">
         <v>15</v>
@@ -6114,13 +6089,13 @@
         <v>50</v>
       </c>
       <c r="D143" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E143">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="F143" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H143" s="2">
         <v>0</v>
@@ -6136,7 +6111,7 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B144" t="s">
         <v>15</v>
@@ -6145,13 +6120,13 @@
         <v>50</v>
       </c>
       <c r="D144" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E144">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F144" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H144" s="2">
         <v>0</v>
@@ -6167,7 +6142,7 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B145" t="s">
         <v>15</v>
@@ -6176,13 +6151,13 @@
         <v>50</v>
       </c>
       <c r="D145" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E145">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="F145" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H145" s="2">
         <v>0</v>
@@ -6198,7 +6173,7 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B146" t="s">
         <v>15</v>
@@ -6207,13 +6182,13 @@
         <v>50</v>
       </c>
       <c r="D146" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E146">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F146" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H146" s="2">
         <v>0</v>
@@ -6229,7 +6204,7 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B147" t="s">
         <v>15</v>
@@ -6238,13 +6213,13 @@
         <v>50</v>
       </c>
       <c r="D147" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E147">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F147" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H147" s="2">
         <v>0</v>
@@ -6260,7 +6235,7 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B148" t="s">
         <v>15</v>
@@ -6269,13 +6244,13 @@
         <v>50</v>
       </c>
       <c r="D148" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E148">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F148" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H148" s="2">
         <v>0</v>
@@ -6291,7 +6266,7 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B149" t="s">
         <v>15</v>
@@ -6300,13 +6275,13 @@
         <v>50</v>
       </c>
       <c r="D149" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E149">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F149" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H149" s="2">
         <v>0</v>
@@ -6322,7 +6297,7 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B150" t="s">
         <v>15</v>
@@ -6331,13 +6306,13 @@
         <v>50</v>
       </c>
       <c r="D150" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E150">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F150" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H150" s="2">
         <v>0</v>
@@ -6353,7 +6328,7 @@
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B151" t="s">
         <v>15</v>
@@ -6362,13 +6337,13 @@
         <v>50</v>
       </c>
       <c r="D151" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E151">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F151" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H151" s="2">
         <v>0</v>
@@ -6384,7 +6359,7 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B152" t="s">
         <v>15</v>
@@ -6393,13 +6368,13 @@
         <v>50</v>
       </c>
       <c r="D152" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E152">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F152" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H152" s="2">
         <v>0</v>
@@ -6415,7 +6390,7 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B153" t="s">
         <v>15</v>
@@ -6424,13 +6399,13 @@
         <v>50</v>
       </c>
       <c r="D153" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E153">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F153" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H153" s="2">
         <v>0</v>
@@ -6446,7 +6421,7 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B154" t="s">
         <v>15</v>
@@ -6455,13 +6430,13 @@
         <v>50</v>
       </c>
       <c r="D154" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E154">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="F154" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H154" s="2">
         <v>0</v>
@@ -6477,27 +6452,32 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>219</v>
+      </c>
+      <c r="B155" t="s">
+        <v>15</v>
+      </c>
+      <c r="C155" t="s">
+        <v>50</v>
+      </c>
+      <c r="D155" t="s">
+        <v>114</v>
+      </c>
+      <c r="E155" t="s">
         <v>220</v>
       </c>
-      <c r="B155" t="s">
-        <v>15</v>
-      </c>
-      <c r="C155" t="s">
-        <v>50</v>
-      </c>
-      <c r="D155" t="s">
-        <v>173</v>
-      </c>
-      <c r="E155">
-        <v>2025</v>
-      </c>
       <c r="F155" t="s">
-        <v>195</v>
+        <v>62</v>
+      </c>
+      <c r="G155" t="s">
+        <v>19</v>
       </c>
       <c r="H155" s="2">
-        <v>0</v>
-      </c>
-      <c r="I155" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="I155" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="J155" s="2">
         <v>0</v>
       </c>
@@ -6508,7 +6488,7 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B156" t="s">
         <v>15</v>
@@ -6517,10 +6497,10 @@
         <v>50</v>
       </c>
       <c r="D156" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="E156" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F156" t="s">
         <v>62</v>
@@ -6532,7 +6512,7 @@
         <v>1</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J156" s="2">
         <v>0</v>
@@ -6544,7 +6524,7 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B157" t="s">
         <v>15</v>
@@ -6553,13 +6533,13 @@
         <v>50</v>
       </c>
       <c r="D157" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="E157" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F157" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G157" t="s">
         <v>19</v>
@@ -6568,7 +6548,7 @@
         <v>1</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J157" s="2">
         <v>0</v>
@@ -6580,22 +6560,22 @@
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
+        <v>224</v>
+      </c>
+      <c r="B158" t="s">
+        <v>15</v>
+      </c>
+      <c r="C158" t="s">
+        <v>50</v>
+      </c>
+      <c r="D158" t="s">
         <v>225</v>
       </c>
-      <c r="B158" t="s">
-        <v>15</v>
-      </c>
-      <c r="C158" t="s">
-        <v>50</v>
-      </c>
-      <c r="D158" t="s">
-        <v>141</v>
-      </c>
       <c r="E158" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F158" t="s">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="G158" t="s">
         <v>19</v>
@@ -6604,7 +6584,7 @@
         <v>1</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J158" s="2">
         <v>0</v>
@@ -6625,13 +6605,13 @@
         <v>50</v>
       </c>
       <c r="D159" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E159" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F159" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="G159" t="s">
         <v>19</v>
@@ -6640,7 +6620,7 @@
         <v>1</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J159" s="2">
         <v>0</v>
@@ -6652,22 +6632,22 @@
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>227</v>
+      </c>
+      <c r="B160" t="s">
+        <v>15</v>
+      </c>
+      <c r="C160" t="s">
+        <v>50</v>
+      </c>
+      <c r="D160" t="s">
+        <v>139</v>
+      </c>
+      <c r="E160" t="s">
         <v>228</v>
       </c>
-      <c r="B160" t="s">
-        <v>15</v>
-      </c>
-      <c r="C160" t="s">
-        <v>50</v>
-      </c>
-      <c r="D160" t="s">
-        <v>227</v>
-      </c>
-      <c r="E160" t="s">
-        <v>222</v>
-      </c>
       <c r="F160" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="G160" t="s">
         <v>19</v>
@@ -6676,7 +6656,7 @@
         <v>1</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J160" s="2">
         <v>0</v>
@@ -6697,13 +6677,13 @@
         <v>50</v>
       </c>
       <c r="D161" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="E161" t="s">
         <v>230</v>
       </c>
       <c r="F161" t="s">
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="G161" t="s">
         <v>19</v>
@@ -6712,19 +6692,21 @@
         <v>1</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="J161" s="2">
-        <v>0</v>
-      </c>
-      <c r="K161" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K161" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="L161" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B162" t="s">
         <v>15</v>
@@ -6733,10 +6715,10 @@
         <v>50</v>
       </c>
       <c r="D162" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="E162" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F162" t="s">
         <v>62</v>
@@ -6748,13 +6730,13 @@
         <v>1</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J162" s="2">
         <v>1</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L162" s="2">
         <v>0</v>
@@ -6762,7 +6744,7 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B163" t="s">
         <v>15</v>
@@ -6771,13 +6753,13 @@
         <v>50</v>
       </c>
       <c r="D163" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="E163" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F163" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G163" t="s">
         <v>19</v>
@@ -6786,13 +6768,13 @@
         <v>1</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J163" s="2">
         <v>1</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L163" s="2">
         <v>0</v>
@@ -6800,22 +6782,22 @@
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>234</v>
+      </c>
+      <c r="B164" t="s">
+        <v>15</v>
+      </c>
+      <c r="C164" t="s">
+        <v>50</v>
+      </c>
+      <c r="D164" t="s">
         <v>235</v>
       </c>
-      <c r="B164" t="s">
-        <v>15</v>
-      </c>
-      <c r="C164" t="s">
-        <v>50</v>
-      </c>
-      <c r="D164" t="s">
-        <v>141</v>
-      </c>
       <c r="E164" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F164" t="s">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="G164" t="s">
         <v>19</v>
@@ -6824,13 +6806,13 @@
         <v>1</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J164" s="2">
         <v>1</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L164" s="2">
         <v>0</v>
@@ -6838,7 +6820,7 @@
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B165" t="s">
         <v>15</v>
@@ -6847,13 +6829,13 @@
         <v>50</v>
       </c>
       <c r="D165" t="s">
-        <v>237</v>
+        <v>139</v>
       </c>
       <c r="E165" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F165" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="G165" t="s">
         <v>19</v>
@@ -6862,13 +6844,13 @@
         <v>1</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J165" s="2">
         <v>1</v>
       </c>
       <c r="K165" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L165" s="2">
         <v>0</v>
@@ -6876,7 +6858,7 @@
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B166" t="s">
         <v>15</v>
@@ -6885,74 +6867,72 @@
         <v>50</v>
       </c>
       <c r="D166" t="s">
-        <v>141</v>
-      </c>
-      <c r="E166" t="s">
-        <v>232</v>
+        <v>56</v>
+      </c>
+      <c r="E166">
+        <v>2020</v>
       </c>
       <c r="F166" t="s">
-        <v>195</v>
+        <v>52</v>
       </c>
       <c r="G166" t="s">
         <v>19</v>
       </c>
       <c r="H166" s="2">
+        <v>0</v>
+      </c>
+      <c r="I166" s="2"/>
+      <c r="J166" s="2">
+        <v>0</v>
+      </c>
+      <c r="K166" s="2"/>
+      <c r="L166" s="2">
         <v>1</v>
       </c>
-      <c r="I166" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J166" s="2">
-        <v>1</v>
-      </c>
-      <c r="K166" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="L166" s="2">
-        <v>0</v>
+      <c r="M166" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>239</v>
+      </c>
+      <c r="B167" t="s">
+        <v>15</v>
+      </c>
+      <c r="C167" t="s">
+        <v>50</v>
+      </c>
+      <c r="D167" t="s">
         <v>240</v>
       </c>
-      <c r="B167" t="s">
-        <v>15</v>
-      </c>
-      <c r="C167" t="s">
-        <v>50</v>
-      </c>
-      <c r="D167" t="s">
-        <v>141</v>
-      </c>
-      <c r="E167" t="s">
+      <c r="E167">
+        <v>2020</v>
+      </c>
+      <c r="F167" t="s">
         <v>241</v>
-      </c>
-      <c r="F167" t="s">
-        <v>242</v>
       </c>
       <c r="G167" t="s">
         <v>19</v>
       </c>
       <c r="H167" s="2">
+        <v>0</v>
+      </c>
+      <c r="I167" s="2"/>
+      <c r="J167" s="2">
+        <v>0</v>
+      </c>
+      <c r="K167" s="2"/>
+      <c r="L167" s="2">
         <v>1</v>
       </c>
-      <c r="I167" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J167" s="2">
-        <v>1</v>
-      </c>
-      <c r="K167" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="L167" s="2">
-        <v>0</v>
+      <c r="M167" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B168" t="s">
         <v>15</v>
@@ -6967,7 +6947,7 @@
         <v>2020</v>
       </c>
       <c r="F168" t="s">
-        <v>52</v>
+        <v>243</v>
       </c>
       <c r="G168" t="s">
         <v>19</v>
@@ -7004,7 +6984,7 @@
         <v>2020</v>
       </c>
       <c r="F169" t="s">
-        <v>246</v>
+        <v>52</v>
       </c>
       <c r="G169" t="s">
         <v>19</v>
@@ -7021,27 +7001,27 @@
         <v>1</v>
       </c>
       <c r="M169" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>246</v>
+      </c>
+      <c r="B170" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" t="s">
+        <v>50</v>
+      </c>
+      <c r="D170" t="s">
         <v>247</v>
-      </c>
-      <c r="B170" t="s">
-        <v>15</v>
-      </c>
-      <c r="C170" t="s">
-        <v>50</v>
-      </c>
-      <c r="D170" t="s">
-        <v>56</v>
       </c>
       <c r="E170">
         <v>2020</v>
       </c>
       <c r="F170" t="s">
-        <v>248</v>
+        <v>52</v>
       </c>
       <c r="G170" t="s">
         <v>19</v>
@@ -7058,7 +7038,7 @@
         <v>1</v>
       </c>
       <c r="M170" s="2" t="s">
-        <v>58</v>
+        <v>248</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.35">
@@ -7075,13 +7055,10 @@
         <v>250</v>
       </c>
       <c r="E171">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="F171" t="s">
-        <v>52</v>
-      </c>
-      <c r="G171" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="H171" s="2">
         <v>0</v>
@@ -7095,12 +7072,15 @@
         <v>1</v>
       </c>
       <c r="M171" s="2" t="s">
-        <v>54</v>
+        <v>248</v>
+      </c>
+      <c r="N171" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B172" t="s">
         <v>15</v>
@@ -7109,13 +7089,13 @@
         <v>50</v>
       </c>
       <c r="D172" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E172">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F172" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="G172" t="s">
         <v>19</v>
@@ -7132,12 +7112,12 @@
         <v>1</v>
       </c>
       <c r="M172" s="2" t="s">
-        <v>253</v>
+        <v>312</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B173" t="s">
         <v>15</v>
@@ -7146,13 +7126,13 @@
         <v>50</v>
       </c>
       <c r="D173" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E173">
-        <v>2015</v>
+        <v>2023</v>
       </c>
       <c r="F173" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H173" s="2">
         <v>0</v>
@@ -7166,10 +7146,7 @@
         <v>1</v>
       </c>
       <c r="M173" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="N173" t="s">
-        <v>257</v>
+        <v>312</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.35">
@@ -7183,16 +7160,13 @@
         <v>50</v>
       </c>
       <c r="D174" t="s">
+        <v>256</v>
+      </c>
+      <c r="E174">
+        <v>2022</v>
+      </c>
+      <c r="F174" t="s">
         <v>259</v>
-      </c>
-      <c r="E174">
-        <v>2023</v>
-      </c>
-      <c r="F174" t="s">
-        <v>62</v>
-      </c>
-      <c r="G174" t="s">
-        <v>19</v>
       </c>
       <c r="H174" s="2">
         <v>0</v>
@@ -7206,7 +7180,7 @@
         <v>1</v>
       </c>
       <c r="M174" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.35">
@@ -7220,13 +7194,16 @@
         <v>50</v>
       </c>
       <c r="D175" t="s">
-        <v>261</v>
+        <v>74</v>
       </c>
       <c r="E175">
         <v>2023</v>
       </c>
       <c r="F175" t="s">
-        <v>262</v>
+        <v>301</v>
+      </c>
+      <c r="G175" t="s">
+        <v>19</v>
       </c>
       <c r="H175" s="2">
         <v>0</v>
@@ -7240,12 +7217,12 @@
         <v>1</v>
       </c>
       <c r="M175" s="2" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B176" t="s">
         <v>15</v>
@@ -7254,13 +7231,16 @@
         <v>50</v>
       </c>
       <c r="D176" t="s">
-        <v>261</v>
+        <v>82</v>
       </c>
       <c r="E176">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F176" t="s">
-        <v>264</v>
+        <v>301</v>
+      </c>
+      <c r="G176" t="s">
+        <v>19</v>
       </c>
       <c r="H176" s="2">
         <v>0</v>
@@ -7274,12 +7254,12 @@
         <v>1</v>
       </c>
       <c r="M176" s="2" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>265</v>
+        <v>302</v>
       </c>
       <c r="B177" t="s">
         <v>15</v>
@@ -7288,13 +7268,13 @@
         <v>50</v>
       </c>
       <c r="D177" t="s">
-        <v>74</v>
+        <v>303</v>
       </c>
       <c r="E177">
         <v>2023</v>
       </c>
       <c r="F177" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G177" t="s">
         <v>19</v>
@@ -7311,12 +7291,12 @@
         <v>1</v>
       </c>
       <c r="M177" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B178" t="s">
         <v>15</v>
@@ -7325,13 +7305,13 @@
         <v>50</v>
       </c>
       <c r="D178" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E178">
         <v>2023</v>
       </c>
       <c r="F178" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G178" t="s">
         <v>19</v>
@@ -7348,12 +7328,12 @@
         <v>1</v>
       </c>
       <c r="M178" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>308</v>
+        <v>263</v>
       </c>
       <c r="B179" t="s">
         <v>15</v>
@@ -7362,13 +7342,13 @@
         <v>50</v>
       </c>
       <c r="D179" t="s">
-        <v>309</v>
+        <v>264</v>
       </c>
       <c r="E179">
         <v>2023</v>
       </c>
       <c r="F179" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="G179" t="s">
         <v>19</v>
@@ -7385,12 +7365,12 @@
         <v>1</v>
       </c>
       <c r="M179" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B180" t="s">
         <v>15</v>
@@ -7399,13 +7379,13 @@
         <v>50</v>
       </c>
       <c r="D180" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="E180">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="F180" t="s">
-        <v>307</v>
+        <v>259</v>
       </c>
       <c r="G180" t="s">
         <v>19</v>
@@ -7422,12 +7402,12 @@
         <v>1</v>
       </c>
       <c r="M180" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="B181" t="s">
         <v>15</v>
@@ -7436,13 +7416,13 @@
         <v>50</v>
       </c>
       <c r="D181" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E181">
-        <v>2023</v>
+        <v>2015</v>
       </c>
       <c r="F181" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G181" t="s">
         <v>19</v>
@@ -7459,81 +7439,59 @@
         <v>1</v>
       </c>
       <c r="M181" s="2" t="s">
-        <v>314</v>
+        <v>305</v>
+      </c>
+      <c r="N181" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>270</v>
+        <v>313</v>
       </c>
       <c r="B182" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C182" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D182" t="s">
         <v>269</v>
       </c>
-      <c r="E182">
-        <v>2022</v>
+      <c r="E182" t="s">
+        <v>16</v>
       </c>
       <c r="F182" t="s">
-        <v>264</v>
+        <v>18</v>
       </c>
       <c r="G182" t="s">
         <v>19</v>
       </c>
-      <c r="H182" s="2">
-        <v>0</v>
-      </c>
-      <c r="I182" s="2"/>
-      <c r="J182" s="2">
-        <v>0</v>
-      </c>
-      <c r="K182" s="2"/>
-      <c r="L182" s="2">
-        <v>1</v>
-      </c>
-      <c r="M182" s="2" t="s">
-        <v>314</v>
+      <c r="N182" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="B183" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C183" t="s">
-        <v>50</v>
+        <v>271</v>
       </c>
       <c r="D183" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E183">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="F183" t="s">
-        <v>272</v>
+        <v>18</v>
       </c>
       <c r="G183" t="s">
         <v>19</v>
-      </c>
-      <c r="H183" s="2">
-        <v>0</v>
-      </c>
-      <c r="I183" s="2"/>
-      <c r="J183" s="2">
-        <v>0</v>
-      </c>
-      <c r="K183" s="2"/>
-      <c r="L183" s="2">
-        <v>1</v>
-      </c>
-      <c r="M183" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="N183" t="s">
         <v>273</v>
@@ -7547,13 +7505,13 @@
         <v>21</v>
       </c>
       <c r="C184" t="s">
-        <v>16</v>
+        <v>271</v>
       </c>
       <c r="D184" t="s">
         <v>275</v>
       </c>
-      <c r="E184" t="s">
-        <v>16</v>
+      <c r="E184">
+        <v>2020</v>
       </c>
       <c r="F184" t="s">
         <v>18</v>
@@ -7562,7 +7520,7 @@
         <v>19</v>
       </c>
       <c r="N184" t="s">
-        <v>38</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.35">
@@ -7573,13 +7531,13 @@
         <v>21</v>
       </c>
       <c r="C185" t="s">
+        <v>271</v>
+      </c>
+      <c r="D185" t="s">
         <v>277</v>
       </c>
-      <c r="D185" t="s">
-        <v>278</v>
-      </c>
-      <c r="E185">
-        <v>2020</v>
+      <c r="E185" t="s">
+        <v>220</v>
       </c>
       <c r="F185" t="s">
         <v>18</v>
@@ -7588,24 +7546,24 @@
         <v>19</v>
       </c>
       <c r="N185" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B186" t="s">
         <v>21</v>
       </c>
       <c r="C186" t="s">
+        <v>271</v>
+      </c>
+      <c r="D186" t="s">
         <v>277</v>
       </c>
-      <c r="D186" t="s">
-        <v>281</v>
-      </c>
-      <c r="E186">
-        <v>2020</v>
+      <c r="E186" t="s">
+        <v>279</v>
       </c>
       <c r="F186" t="s">
         <v>18</v>
@@ -7614,24 +7572,24 @@
         <v>19</v>
       </c>
       <c r="N186" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B187" t="s">
         <v>21</v>
       </c>
       <c r="C187" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D187" t="s">
-        <v>283</v>
-      </c>
-      <c r="E187" t="s">
-        <v>222</v>
+        <v>281</v>
+      </c>
+      <c r="E187">
+        <v>2020</v>
       </c>
       <c r="F187" t="s">
         <v>18</v>
@@ -7640,24 +7598,24 @@
         <v>19</v>
       </c>
       <c r="N187" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B188" t="s">
         <v>21</v>
       </c>
       <c r="C188" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D188" t="s">
         <v>283</v>
       </c>
-      <c r="E188" t="s">
-        <v>285</v>
+      <c r="E188">
+        <v>2020</v>
       </c>
       <c r="F188" t="s">
         <v>18</v>
@@ -7666,21 +7624,21 @@
         <v>19</v>
       </c>
       <c r="N188" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B189" t="s">
         <v>21</v>
       </c>
       <c r="C189" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D189" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E189">
         <v>2020</v>
@@ -7692,24 +7650,24 @@
         <v>19</v>
       </c>
       <c r="N189" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="B190" t="s">
         <v>21</v>
       </c>
       <c r="C190" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D190" t="s">
-        <v>289</v>
-      </c>
-      <c r="E190">
-        <v>2020</v>
+        <v>285</v>
+      </c>
+      <c r="E190" t="s">
+        <v>279</v>
       </c>
       <c r="F190" t="s">
         <v>18</v>
@@ -7718,24 +7676,24 @@
         <v>19</v>
       </c>
       <c r="N190" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B191" t="s">
         <v>21</v>
       </c>
       <c r="C191" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D191" t="s">
-        <v>291</v>
-      </c>
-      <c r="E191">
-        <v>2020</v>
+        <v>272</v>
+      </c>
+      <c r="E191" t="s">
+        <v>279</v>
       </c>
       <c r="F191" t="s">
         <v>18</v>
@@ -7744,24 +7702,24 @@
         <v>19</v>
       </c>
       <c r="N191" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B192" t="s">
         <v>21</v>
       </c>
       <c r="C192" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D192" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E192" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F192" t="s">
         <v>18</v>
@@ -7770,24 +7728,24 @@
         <v>19</v>
       </c>
       <c r="N192" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B193" t="s">
         <v>21</v>
       </c>
       <c r="C193" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D193" t="s">
-        <v>278</v>
-      </c>
-      <c r="E193" t="s">
-        <v>285</v>
+        <v>287</v>
+      </c>
+      <c r="E193">
+        <v>2015</v>
       </c>
       <c r="F193" t="s">
         <v>18</v>
@@ -7796,24 +7754,24 @@
         <v>19</v>
       </c>
       <c r="N193" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
       <c r="B194" t="s">
         <v>21</v>
       </c>
       <c r="C194" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="D194" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E194" t="s">
-        <v>285</v>
+        <v>16</v>
       </c>
       <c r="F194" t="s">
         <v>18</v>
@@ -7822,24 +7780,24 @@
         <v>19</v>
       </c>
       <c r="N194" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="B195" t="s">
         <v>21</v>
       </c>
       <c r="C195" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="D195" t="s">
         <v>293</v>
       </c>
-      <c r="E195">
-        <v>2015</v>
+      <c r="E195" t="s">
+        <v>16</v>
       </c>
       <c r="F195" t="s">
         <v>18</v>
@@ -7848,18 +7806,18 @@
         <v>19</v>
       </c>
       <c r="N195" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B196" t="s">
         <v>21</v>
       </c>
       <c r="C196" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D196" t="s">
         <v>296</v>
@@ -7875,58 +7833,6 @@
       </c>
       <c r="N196" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>298</v>
-      </c>
-      <c r="B197" t="s">
-        <v>21</v>
-      </c>
-      <c r="C197" t="s">
-        <v>295</v>
-      </c>
-      <c r="D197" t="s">
-        <v>299</v>
-      </c>
-      <c r="E197" t="s">
-        <v>16</v>
-      </c>
-      <c r="F197" t="s">
-        <v>18</v>
-      </c>
-      <c r="G197" t="s">
-        <v>19</v>
-      </c>
-      <c r="N197" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="198" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>301</v>
-      </c>
-      <c r="B198" t="s">
-        <v>21</v>
-      </c>
-      <c r="C198" t="s">
-        <v>295</v>
-      </c>
-      <c r="D198" t="s">
-        <v>302</v>
-      </c>
-      <c r="E198" t="s">
-        <v>16</v>
-      </c>
-      <c r="F198" t="s">
-        <v>18</v>
-      </c>
-      <c r="G198" t="s">
-        <v>19</v>
-      </c>
-      <c r="N198" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -7937,33 +7843,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <kae7f6409c1a45b5af70ba169c41da0e xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </kae7f6409c1a45b5af70ba169c41da0e>
-    <REDD_x002f_NFM_x0020_category xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003082C08FD3D0614AAB94B75C024070A7" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a4b61487ffa532d49c6719891dd0d2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82302deb-32b0-442b-bedc-ba64a9aa8ccd" xmlns:ns3="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cea40d1c5f6ee0e5ae997cf8704aff88" ns2:_="" ns3:_="">
     <xsd:import namespace="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
@@ -8252,26 +8131,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63A60D8A-7D1B-403D-BB2C-B10CCD11CB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
-    <ds:schemaRef ds:uri="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBDC3B9-24A5-4D52-9DEE-E1BAF29BA53E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <kae7f6409c1a45b5af70ba169c41da0e xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </kae7f6409c1a45b5af70ba169c41da0e>
+    <REDD_x002f_NFM_x0020_category xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE6D2EE7-47BC-4B0F-B98D-543F5E3F8F03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8288,4 +8175,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBDC3B9-24A5-4D52-9DEE-E1BAF29BA53E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63A60D8A-7D1B-403D-BB2C-B10CCD11CB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
+    <ds:schemaRef ds:uri="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added national data to whisp columns: a new tab as not strictly default/core whisp datasets
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnell\Documents\GitHub\whisp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC43A7-E222-4A0F-9D82-753F6C558B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D28990-C9B1-4A71-96CF-8FE5A8DEDD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{FC85F32F-3F3C-476F-A445-BF878E774111}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" activeTab="1" xr2:uid="{FC85F32F-3F3C-476F-A445-BF878E774111}"/>
   </bookViews>
   <sheets>
     <sheet name="Whisp outputs" sheetId="1" r:id="rId1"/>
+    <sheet name="Whisp outputs national" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="357">
   <si>
     <t>Column name</t>
   </si>
@@ -978,6 +979,135 @@
   </si>
   <si>
     <t>geo</t>
+  </si>
+  <si>
+    <t>nCO_ideam_forest_2020</t>
+  </si>
+  <si>
+    <t>IDEAM 2020</t>
+  </si>
+  <si>
+    <t>nCO_ideam_agroforest_2020</t>
+  </si>
+  <si>
+    <t>Area of agroforestry</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TC_primary_forest_Amazon_2020</t>
+  </si>
+  <si>
+    <t>Assis et al,. 2019</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TC_secondary_forest_Amazon_2020</t>
+  </si>
+  <si>
+    <t>nBR_BFS_primary_forest_Pantanal_2020</t>
+  </si>
+  <si>
+    <t>Serviço Florestal Brasileiro, 2024</t>
+  </si>
+  <si>
+    <t>nBR_BFS_primary_forest_Caatinga_2020</t>
+  </si>
+  <si>
+    <t>nBR_BFS_primary_forest_AtlanticForest_2020</t>
+  </si>
+  <si>
+    <t>nBR_BFS_primary_forest_Pampa_2020</t>
+  </si>
+  <si>
+    <t>nBR_BFS_primary&amp;secondary_forest_Cerrado_2020</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_forest_Brazil_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Souza et al., 2020</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TCsilviculture_Amazon_2020</t>
+  </si>
+  <si>
+    <t>TERRACLASS (EMBRAPA) (2023)</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TCsilviculture_Cerrado_2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERRACLASS (INPE/EMBRAPA). </t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_silviculture_Brazil_2020</t>
+  </si>
+  <si>
+    <t>nBR_PRODES_deforestation_Brazil_before_2020</t>
+  </si>
+  <si>
+    <t>1988-2000</t>
+  </si>
+  <si>
+    <t>nBR_DETER_forestdegradation_Amazon_before_2020</t>
+  </si>
+  <si>
+    <t>2016-2000</t>
+  </si>
+  <si>
+    <t>Doblas 2022</t>
+  </si>
+  <si>
+    <t>nBR_PRODES_deforestation_Brazil_after_2020</t>
+  </si>
+  <si>
+    <t>2000-present</t>
+  </si>
+  <si>
+    <t>nBR_DETER_forestdegradation_Amazon_after_2020</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TCamz_cer_perennial_2020</t>
+  </si>
+  <si>
+    <t>Area of Perennial Crops</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_coffee_2020</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_palmoil_2020</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_pc_2020</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TCamz_cer_annual_2020</t>
+  </si>
+  <si>
+    <t>Area of Annual Crops</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_soy_2020</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_annual_crops_2020</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TCamz_pasture_2020</t>
+  </si>
+  <si>
+    <t>Area of Pasture</t>
+  </si>
+  <si>
+    <t>nBR_INPE_TCcer_pasture_2020</t>
+  </si>
+  <si>
+    <t>nBR_MapBiomas_col9_pasture_2020</t>
+  </si>
+  <si>
+    <t>nCI_Cocoa_bnetd</t>
+  </si>
+  <si>
+    <t>BNETD 2020.</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1135,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1015,6 +1145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1031,10 +1167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A90905-187C-4727-AD42-76516A57CDD0}">
   <dimension ref="A1:N196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
     </sheetView>
@@ -7783,7 +7920,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>292</v>
       </c>
@@ -7842,7 +7979,1157 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3BA78D-4BAA-453B-B2F4-F30CD56DAD59}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2">
+        <v>2020</v>
+      </c>
+      <c r="F2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E3">
+        <v>2020</v>
+      </c>
+      <c r="F3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4">
+        <v>2020</v>
+      </c>
+      <c r="F4" t="s">
+        <v>319</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>2020</v>
+      </c>
+      <c r="F5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6">
+        <v>2020</v>
+      </c>
+      <c r="F6" t="s">
+        <v>322</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
+      <c r="F7" t="s">
+        <v>322</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8">
+        <v>2020</v>
+      </c>
+      <c r="F8" t="s">
+        <v>322</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9">
+        <v>2020</v>
+      </c>
+      <c r="F9" t="s">
+        <v>322</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10">
+        <v>2020</v>
+      </c>
+      <c r="F10" t="s">
+        <v>322</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>2020</v>
+      </c>
+      <c r="F11" t="s">
+        <v>328</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12">
+        <v>2020</v>
+      </c>
+      <c r="F12" t="s">
+        <v>330</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13">
+        <v>2020</v>
+      </c>
+      <c r="F13" t="s">
+        <v>332</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>333</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14">
+        <v>2020</v>
+      </c>
+      <c r="F14" t="s">
+        <v>328</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>335</v>
+      </c>
+      <c r="F15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
+        <v>337</v>
+      </c>
+      <c r="F16" t="s">
+        <v>338</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>339</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>340</v>
+      </c>
+      <c r="F17" t="s">
+        <v>319</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>341</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" t="s">
+        <v>340</v>
+      </c>
+      <c r="F18" t="s">
+        <v>338</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>343</v>
+      </c>
+      <c r="E19">
+        <v>2020</v>
+      </c>
+      <c r="F19" t="s">
+        <v>330</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>344</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E20">
+        <v>2020</v>
+      </c>
+      <c r="F20" t="s">
+        <v>328</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21">
+        <v>2020</v>
+      </c>
+      <c r="F21" t="s">
+        <v>328</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>346</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>343</v>
+      </c>
+      <c r="E22">
+        <v>2020</v>
+      </c>
+      <c r="F22" t="s">
+        <v>328</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>347</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>348</v>
+      </c>
+      <c r="E23">
+        <v>2020</v>
+      </c>
+      <c r="F23" t="s">
+        <v>330</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>349</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24">
+        <v>2020</v>
+      </c>
+      <c r="F24" t="s">
+        <v>328</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>348</v>
+      </c>
+      <c r="E25">
+        <v>2020</v>
+      </c>
+      <c r="F25" t="s">
+        <v>328</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>351</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>352</v>
+      </c>
+      <c r="E26">
+        <v>2020</v>
+      </c>
+      <c r="F26" t="s">
+        <v>330</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>353</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>352</v>
+      </c>
+      <c r="E27">
+        <v>2020</v>
+      </c>
+      <c r="F27" t="s">
+        <v>332</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>354</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>352</v>
+      </c>
+      <c r="E28">
+        <v>2020</v>
+      </c>
+      <c r="F28" t="s">
+        <v>328</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>355</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29">
+        <v>2020</v>
+      </c>
+      <c r="F29" t="s">
+        <v>356</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <kae7f6409c1a45b5af70ba169c41da0e xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </kae7f6409c1a45b5af70ba169c41da0e>
+    <REDD_x002f_NFM_x0020_category xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003082C08FD3D0614AAB94B75C024070A7" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a4b61487ffa532d49c6719891dd0d2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82302deb-32b0-442b-bedc-ba64a9aa8ccd" xmlns:ns3="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cea40d1c5f6ee0e5ae997cf8704aff88" ns2:_="" ns3:_="">
     <xsd:import namespace="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
@@ -8131,34 +9418,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63A60D8A-7D1B-403D-BB2C-B10CCD11CB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
+    <ds:schemaRef ds:uri="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <kae7f6409c1a45b5af70ba169c41da0e xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </kae7f6409c1a45b5af70ba169c41da0e>
-    <REDD_x002f_NFM_x0020_category xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82302deb-32b0-442b-bedc-ba64a9aa8ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBDC3B9-24A5-4D52-9DEE-E1BAF29BA53E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE6D2EE7-47BC-4B0F-B98D-543F5E3F8F03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8175,23 +9454,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBDC3B9-24A5-4D52-9DEE-E1BAF29BA53E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63A60D8A-7D1B-403D-BB2C-B10CCD11CB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
-    <ds:schemaRef ds:uri="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
keep ESRI only and gain 2020-2023 crop
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnell\Documents\GitHub\whisp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\astri\Documents\FAO\test_degrad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07598504-323B-44EF-9C81-1DB66198FEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F13A04-E6F9-4BB6-B53D-204FFC390426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Whisp outputs" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="356">
   <si>
     <t>Column name</t>
   </si>
@@ -944,12 +944,6 @@
     <t>Karra 2021</t>
   </si>
   <si>
-    <t>GLC_FCS30D_TC_2022</t>
-  </si>
-  <si>
-    <t>Liangyun 2023</t>
-  </si>
-  <si>
     <t>Oil_palm_2023_FDaP</t>
   </si>
   <si>
@@ -965,15 +959,9 @@
     <t>Cocoa_2023_FDaP</t>
   </si>
   <si>
-    <t>ESRI_2023_crop</t>
-  </si>
-  <si>
     <t>Area of Crop</t>
   </si>
   <si>
-    <t>GLC_FCS30D_crop_2022</t>
-  </si>
-  <si>
     <t>GFW_logging_before_2020</t>
   </si>
   <si>
@@ -1095,6 +1083,12 @@
   </si>
   <si>
     <t>To maintain a consistent output format, numeric values will be converted to strings. Note: any multipolygons in the input will be split into individual parts, which may result in duplicate attribute values in the output.</t>
+  </si>
+  <si>
+    <t>ESRI_crop_gain_2020_2023</t>
+  </si>
+  <si>
+    <t>2020 and 2023</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1195,16 +1189,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1510,20 +1500,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N196"/>
+  <dimension ref="A1:N194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.26953125" style="7" bestFit="1" customWidth="1"/>
@@ -1548,7 +1538,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1592,7 +1582,7 @@
       <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" t="s">
         <v>76</v>
       </c>
       <c r="F2" t="s">
@@ -1633,7 +1623,7 @@
       <c r="D3" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" t="s">
         <v>76</v>
       </c>
       <c r="F3" t="s">
@@ -1661,7 +1651,7 @@
         <v>76</v>
       </c>
       <c r="N3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1677,7 +1667,7 @@
       <c r="D4" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" t="s">
         <v>76</v>
       </c>
       <c r="F4" t="s">
@@ -1718,7 +1708,7 @@
       <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" t="s">
         <v>76</v>
       </c>
       <c r="F5" t="s">
@@ -1759,7 +1749,7 @@
       <c r="D6" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" t="s">
         <v>76</v>
       </c>
       <c r="F6" t="s">
@@ -1800,7 +1790,7 @@
       <c r="D7" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" t="s">
         <v>76</v>
       </c>
       <c r="F7" t="s">
@@ -1841,7 +1831,7 @@
       <c r="D8" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" t="s">
         <v>76</v>
       </c>
       <c r="F8" t="s">
@@ -1882,7 +1872,7 @@
       <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" t="s">
         <v>76</v>
       </c>
       <c r="F9" t="s">
@@ -1926,7 +1916,7 @@
       <c r="D10" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" t="s">
         <v>76</v>
       </c>
       <c r="F10" t="s">
@@ -1970,7 +1960,7 @@
       <c r="D11" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" t="s">
         <v>76</v>
       </c>
       <c r="F11" t="s">
@@ -2011,7 +2001,7 @@
       <c r="D12" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>2020</v>
       </c>
       <c r="F12" t="s">
@@ -2052,7 +2042,7 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>2020</v>
       </c>
       <c r="F13" t="s">
@@ -2093,7 +2083,7 @@
       <c r="D14" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>2000</v>
       </c>
       <c r="F14" t="s">
@@ -2137,7 +2127,7 @@
       <c r="D15" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>2020</v>
       </c>
       <c r="F15" t="s">
@@ -2178,7 +2168,7 @@
       <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>2020</v>
       </c>
       <c r="F16" t="s">
@@ -2219,7 +2209,7 @@
       <c r="D17" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>2020</v>
       </c>
       <c r="F17" t="s">
@@ -2260,7 +2250,7 @@
       <c r="D18" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>2020</v>
       </c>
       <c r="F18" t="s">
@@ -2301,7 +2291,7 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>2020</v>
       </c>
       <c r="F19" t="s">
@@ -2342,7 +2332,7 @@
       <c r="D20" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>2020</v>
       </c>
       <c r="F20" t="s">
@@ -2383,7 +2373,7 @@
       <c r="D21" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>2020</v>
       </c>
       <c r="F21" t="s">
@@ -2424,7 +2414,7 @@
       <c r="D22" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>2020</v>
       </c>
       <c r="F22" t="s">
@@ -2465,7 +2455,7 @@
       <c r="D23" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>2020</v>
       </c>
       <c r="F23" t="s">
@@ -2506,7 +2496,7 @@
       <c r="D24" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>2020</v>
       </c>
       <c r="F24" t="s">
@@ -2547,7 +2537,7 @@
       <c r="D25" t="s">
         <v>133</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>2020</v>
       </c>
       <c r="F25" t="s">
@@ -2588,7 +2578,7 @@
       <c r="D26" t="s">
         <v>133</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>2020</v>
       </c>
       <c r="F26" t="s">
@@ -2629,7 +2619,7 @@
       <c r="D27" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>2020</v>
       </c>
       <c r="F27" t="s">
@@ -2670,7 +2660,7 @@
       <c r="D28" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>2000</v>
       </c>
       <c r="F28" t="s">
@@ -2701,7 +2691,7 @@
       <c r="D29" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>2001</v>
       </c>
       <c r="F29" t="s">
@@ -2732,7 +2722,7 @@
       <c r="D30" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <v>2002</v>
       </c>
       <c r="F30" t="s">
@@ -2763,7 +2753,7 @@
       <c r="D31" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="8">
         <v>2003</v>
       </c>
       <c r="F31" t="s">
@@ -2794,7 +2784,7 @@
       <c r="D32" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>2004</v>
       </c>
       <c r="F32" t="s">
@@ -2825,7 +2815,7 @@
       <c r="D33" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <v>2005</v>
       </c>
       <c r="F33" t="s">
@@ -2856,7 +2846,7 @@
       <c r="D34" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <v>2006</v>
       </c>
       <c r="F34" t="s">
@@ -2887,7 +2877,7 @@
       <c r="D35" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <v>2007</v>
       </c>
       <c r="F35" t="s">
@@ -2918,7 +2908,7 @@
       <c r="D36" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="8">
         <v>2008</v>
       </c>
       <c r="F36" t="s">
@@ -2949,7 +2939,7 @@
       <c r="D37" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="8">
         <v>2009</v>
       </c>
       <c r="F37" t="s">
@@ -2980,7 +2970,7 @@
       <c r="D38" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="8">
         <v>2010</v>
       </c>
       <c r="F38" t="s">
@@ -3011,7 +3001,7 @@
       <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="8">
         <v>2011</v>
       </c>
       <c r="F39" t="s">
@@ -3042,7 +3032,7 @@
       <c r="D40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="8">
         <v>2012</v>
       </c>
       <c r="F40" t="s">
@@ -3073,7 +3063,7 @@
       <c r="D41" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="8">
         <v>2013</v>
       </c>
       <c r="F41" t="s">
@@ -3104,7 +3094,7 @@
       <c r="D42" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="8">
         <v>2014</v>
       </c>
       <c r="F42" t="s">
@@ -3135,7 +3125,7 @@
       <c r="D43" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="8">
         <v>2015</v>
       </c>
       <c r="F43" t="s">
@@ -3166,7 +3156,7 @@
       <c r="D44" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="8">
         <v>2016</v>
       </c>
       <c r="F44" t="s">
@@ -3197,7 +3187,7 @@
       <c r="D45" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="8">
         <v>2017</v>
       </c>
       <c r="F45" t="s">
@@ -3228,7 +3218,7 @@
       <c r="D46" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="8">
         <v>2018</v>
       </c>
       <c r="F46" t="s">
@@ -3259,7 +3249,7 @@
       <c r="D47" t="s">
         <v>45</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="8">
         <v>2019</v>
       </c>
       <c r="F47" t="s">
@@ -3290,7 +3280,7 @@
       <c r="D48" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="8">
         <v>2020</v>
       </c>
       <c r="F48" t="s">
@@ -3321,7 +3311,7 @@
       <c r="D49" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="8">
         <v>2021</v>
       </c>
       <c r="F49" t="s">
@@ -3352,7 +3342,7 @@
       <c r="D50" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="8">
         <v>2022</v>
       </c>
       <c r="F50" t="s">
@@ -3383,7 +3373,7 @@
       <c r="D51" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="8">
         <v>2023</v>
       </c>
       <c r="F51" t="s">
@@ -3414,7 +3404,7 @@
       <c r="D52" t="s">
         <v>45</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="8">
         <v>2024</v>
       </c>
       <c r="F52" t="s">
@@ -3445,7 +3435,7 @@
       <c r="D53" t="s">
         <v>49</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="8">
         <v>2000</v>
       </c>
       <c r="F53" t="s">
@@ -3476,7 +3466,7 @@
       <c r="D54" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="8">
         <v>2001</v>
       </c>
       <c r="F54" t="s">
@@ -3507,7 +3497,7 @@
       <c r="D55" t="s">
         <v>49</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="8">
         <v>2002</v>
       </c>
       <c r="F55" t="s">
@@ -3538,7 +3528,7 @@
       <c r="D56" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="8">
         <v>2003</v>
       </c>
       <c r="F56" t="s">
@@ -3569,7 +3559,7 @@
       <c r="D57" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="8">
         <v>2004</v>
       </c>
       <c r="F57" t="s">
@@ -3600,7 +3590,7 @@
       <c r="D58" t="s">
         <v>49</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="8">
         <v>2005</v>
       </c>
       <c r="F58" t="s">
@@ -3631,7 +3621,7 @@
       <c r="D59" t="s">
         <v>49</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="8">
         <v>2006</v>
       </c>
       <c r="F59" t="s">
@@ -3662,7 +3652,7 @@
       <c r="D60" t="s">
         <v>49</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E60" s="8">
         <v>2007</v>
       </c>
       <c r="F60" t="s">
@@ -3693,7 +3683,7 @@
       <c r="D61" t="s">
         <v>49</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E61" s="8">
         <v>2008</v>
       </c>
       <c r="F61" t="s">
@@ -3724,7 +3714,7 @@
       <c r="D62" t="s">
         <v>49</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E62" s="8">
         <v>2009</v>
       </c>
       <c r="F62" t="s">
@@ -3755,7 +3745,7 @@
       <c r="D63" t="s">
         <v>49</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E63" s="8">
         <v>2010</v>
       </c>
       <c r="F63" t="s">
@@ -3786,7 +3776,7 @@
       <c r="D64" t="s">
         <v>49</v>
       </c>
-      <c r="E64" s="9">
+      <c r="E64" s="8">
         <v>2011</v>
       </c>
       <c r="F64" t="s">
@@ -3817,7 +3807,7 @@
       <c r="D65" t="s">
         <v>49</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E65" s="8">
         <v>2012</v>
       </c>
       <c r="F65" t="s">
@@ -3848,7 +3838,7 @@
       <c r="D66" t="s">
         <v>49</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E66" s="8">
         <v>2013</v>
       </c>
       <c r="F66" t="s">
@@ -3879,7 +3869,7 @@
       <c r="D67" t="s">
         <v>49</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E67" s="8">
         <v>2014</v>
       </c>
       <c r="F67" t="s">
@@ -3910,7 +3900,7 @@
       <c r="D68" t="s">
         <v>49</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E68" s="8">
         <v>2015</v>
       </c>
       <c r="F68" t="s">
@@ -3941,7 +3931,7 @@
       <c r="D69" t="s">
         <v>49</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E69" s="8">
         <v>2016</v>
       </c>
       <c r="F69" t="s">
@@ -3972,7 +3962,7 @@
       <c r="D70" t="s">
         <v>49</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E70" s="8">
         <v>2017</v>
       </c>
       <c r="F70" t="s">
@@ -4003,7 +3993,7 @@
       <c r="D71" t="s">
         <v>49</v>
       </c>
-      <c r="E71" s="9">
+      <c r="E71" s="8">
         <v>2018</v>
       </c>
       <c r="F71" t="s">
@@ -4034,7 +4024,7 @@
       <c r="D72" t="s">
         <v>49</v>
       </c>
-      <c r="E72" s="9">
+      <c r="E72" s="8">
         <v>2019</v>
       </c>
       <c r="F72" t="s">
@@ -4065,7 +4055,7 @@
       <c r="D73" t="s">
         <v>49</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E73" s="8">
         <v>2020</v>
       </c>
       <c r="F73" t="s">
@@ -4096,7 +4086,7 @@
       <c r="D74" t="s">
         <v>49</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E74" s="8">
         <v>2021</v>
       </c>
       <c r="F74" t="s">
@@ -4127,7 +4117,7 @@
       <c r="D75" t="s">
         <v>49</v>
       </c>
-      <c r="E75" s="9">
+      <c r="E75" s="8">
         <v>2022</v>
       </c>
       <c r="F75" t="s">
@@ -4158,7 +4148,7 @@
       <c r="D76" t="s">
         <v>49</v>
       </c>
-      <c r="E76" s="9">
+      <c r="E76" s="8">
         <v>2023</v>
       </c>
       <c r="F76" t="s">
@@ -4189,7 +4179,7 @@
       <c r="D77" t="s">
         <v>49</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E77" s="8">
         <v>2024</v>
       </c>
       <c r="F77" t="s">
@@ -4220,7 +4210,7 @@
       <c r="D78" t="s">
         <v>189</v>
       </c>
-      <c r="E78" s="9">
+      <c r="E78" s="8">
         <v>2001</v>
       </c>
       <c r="F78" t="s">
@@ -4251,7 +4241,7 @@
       <c r="D79" t="s">
         <v>189</v>
       </c>
-      <c r="E79" s="9">
+      <c r="E79" s="8">
         <v>2002</v>
       </c>
       <c r="F79" t="s">
@@ -4282,7 +4272,7 @@
       <c r="D80" t="s">
         <v>189</v>
       </c>
-      <c r="E80" s="9">
+      <c r="E80" s="8">
         <v>2003</v>
       </c>
       <c r="F80" t="s">
@@ -4313,7 +4303,7 @@
       <c r="D81" t="s">
         <v>189</v>
       </c>
-      <c r="E81" s="9">
+      <c r="E81" s="8">
         <v>2004</v>
       </c>
       <c r="F81" t="s">
@@ -4344,7 +4334,7 @@
       <c r="D82" t="s">
         <v>189</v>
       </c>
-      <c r="E82" s="9">
+      <c r="E82" s="8">
         <v>2005</v>
       </c>
       <c r="F82" t="s">
@@ -4375,7 +4365,7 @@
       <c r="D83" t="s">
         <v>189</v>
       </c>
-      <c r="E83" s="9">
+      <c r="E83" s="8">
         <v>2006</v>
       </c>
       <c r="F83" t="s">
@@ -4406,7 +4396,7 @@
       <c r="D84" t="s">
         <v>189</v>
       </c>
-      <c r="E84" s="9">
+      <c r="E84" s="8">
         <v>2007</v>
       </c>
       <c r="F84" t="s">
@@ -4437,7 +4427,7 @@
       <c r="D85" t="s">
         <v>189</v>
       </c>
-      <c r="E85" s="9">
+      <c r="E85" s="8">
         <v>2008</v>
       </c>
       <c r="F85" t="s">
@@ -4468,7 +4458,7 @@
       <c r="D86" t="s">
         <v>189</v>
       </c>
-      <c r="E86" s="9">
+      <c r="E86" s="8">
         <v>2009</v>
       </c>
       <c r="F86" t="s">
@@ -4499,7 +4489,7 @@
       <c r="D87" t="s">
         <v>189</v>
       </c>
-      <c r="E87" s="9">
+      <c r="E87" s="8">
         <v>2010</v>
       </c>
       <c r="F87" t="s">
@@ -4530,7 +4520,7 @@
       <c r="D88" t="s">
         <v>189</v>
       </c>
-      <c r="E88" s="9">
+      <c r="E88" s="8">
         <v>2011</v>
       </c>
       <c r="F88" t="s">
@@ -4561,7 +4551,7 @@
       <c r="D89" t="s">
         <v>189</v>
       </c>
-      <c r="E89" s="9">
+      <c r="E89" s="8">
         <v>2012</v>
       </c>
       <c r="F89" t="s">
@@ -4592,7 +4582,7 @@
       <c r="D90" t="s">
         <v>189</v>
       </c>
-      <c r="E90" s="9">
+      <c r="E90" s="8">
         <v>2013</v>
       </c>
       <c r="F90" t="s">
@@ -4623,7 +4613,7 @@
       <c r="D91" t="s">
         <v>189</v>
       </c>
-      <c r="E91" s="9">
+      <c r="E91" s="8">
         <v>2014</v>
       </c>
       <c r="F91" t="s">
@@ -4654,7 +4644,7 @@
       <c r="D92" t="s">
         <v>189</v>
       </c>
-      <c r="E92" s="9">
+      <c r="E92" s="8">
         <v>2015</v>
       </c>
       <c r="F92" t="s">
@@ -4685,7 +4675,7 @@
       <c r="D93" t="s">
         <v>189</v>
       </c>
-      <c r="E93" s="9">
+      <c r="E93" s="8">
         <v>2016</v>
       </c>
       <c r="F93" t="s">
@@ -4716,7 +4706,7 @@
       <c r="D94" t="s">
         <v>189</v>
       </c>
-      <c r="E94" s="9">
+      <c r="E94" s="8">
         <v>2017</v>
       </c>
       <c r="F94" t="s">
@@ -4747,7 +4737,7 @@
       <c r="D95" t="s">
         <v>189</v>
       </c>
-      <c r="E95" s="9">
+      <c r="E95" s="8">
         <v>2018</v>
       </c>
       <c r="F95" t="s">
@@ -4778,7 +4768,7 @@
       <c r="D96" t="s">
         <v>189</v>
       </c>
-      <c r="E96" s="9">
+      <c r="E96" s="8">
         <v>2019</v>
       </c>
       <c r="F96" t="s">
@@ -4809,7 +4799,7 @@
       <c r="D97" t="s">
         <v>189</v>
       </c>
-      <c r="E97" s="9">
+      <c r="E97" s="8">
         <v>2020</v>
       </c>
       <c r="F97" t="s">
@@ -4840,7 +4830,7 @@
       <c r="D98" t="s">
         <v>189</v>
       </c>
-      <c r="E98" s="9">
+      <c r="E98" s="8">
         <v>2021</v>
       </c>
       <c r="F98" t="s">
@@ -4871,7 +4861,7 @@
       <c r="D99" t="s">
         <v>189</v>
       </c>
-      <c r="E99" s="9">
+      <c r="E99" s="8">
         <v>2022</v>
       </c>
       <c r="F99" t="s">
@@ -4902,7 +4892,7 @@
       <c r="D100" t="s">
         <v>189</v>
       </c>
-      <c r="E100" s="9">
+      <c r="E100" s="8">
         <v>2023</v>
       </c>
       <c r="F100" t="s">
@@ -4933,7 +4923,7 @@
       <c r="D101" t="s">
         <v>189</v>
       </c>
-      <c r="E101" s="9">
+      <c r="E101" s="8">
         <v>2024</v>
       </c>
       <c r="F101" t="s">
@@ -4964,7 +4954,7 @@
       <c r="D102" t="s">
         <v>189</v>
       </c>
-      <c r="E102" s="9">
+      <c r="E102" s="8">
         <v>2019</v>
       </c>
       <c r="F102" t="s">
@@ -4995,7 +4985,7 @@
       <c r="D103" t="s">
         <v>189</v>
       </c>
-      <c r="E103" s="9">
+      <c r="E103" s="8">
         <v>2020</v>
       </c>
       <c r="F103" t="s">
@@ -5026,7 +5016,7 @@
       <c r="D104" t="s">
         <v>189</v>
       </c>
-      <c r="E104" s="9">
+      <c r="E104" s="8">
         <v>2021</v>
       </c>
       <c r="F104" t="s">
@@ -5057,7 +5047,7 @@
       <c r="D105" t="s">
         <v>189</v>
       </c>
-      <c r="E105" s="9">
+      <c r="E105" s="8">
         <v>2022</v>
       </c>
       <c r="F105" t="s">
@@ -5088,7 +5078,7 @@
       <c r="D106" t="s">
         <v>189</v>
       </c>
-      <c r="E106" s="9">
+      <c r="E106" s="8">
         <v>2023</v>
       </c>
       <c r="F106" t="s">
@@ -5119,7 +5109,7 @@
       <c r="D107" t="s">
         <v>189</v>
       </c>
-      <c r="E107" s="9">
+      <c r="E107" s="8">
         <v>2024</v>
       </c>
       <c r="F107" t="s">
@@ -5150,7 +5140,7 @@
       <c r="D108" t="s">
         <v>189</v>
       </c>
-      <c r="E108" s="9">
+      <c r="E108" s="8">
         <v>2025</v>
       </c>
       <c r="F108" t="s">
@@ -5181,7 +5171,7 @@
       <c r="D109" t="s">
         <v>222</v>
       </c>
-      <c r="E109" s="9">
+      <c r="E109" s="8">
         <v>2001</v>
       </c>
       <c r="F109" t="s">
@@ -5212,7 +5202,7 @@
       <c r="D110" t="s">
         <v>222</v>
       </c>
-      <c r="E110" s="9">
+      <c r="E110" s="8">
         <v>2002</v>
       </c>
       <c r="F110" t="s">
@@ -5243,7 +5233,7 @@
       <c r="D111" t="s">
         <v>222</v>
       </c>
-      <c r="E111" s="9">
+      <c r="E111" s="8">
         <v>2003</v>
       </c>
       <c r="F111" t="s">
@@ -5274,7 +5264,7 @@
       <c r="D112" t="s">
         <v>222</v>
       </c>
-      <c r="E112" s="9">
+      <c r="E112" s="8">
         <v>2004</v>
       </c>
       <c r="F112" t="s">
@@ -5305,7 +5295,7 @@
       <c r="D113" t="s">
         <v>222</v>
       </c>
-      <c r="E113" s="9">
+      <c r="E113" s="8">
         <v>2005</v>
       </c>
       <c r="F113" t="s">
@@ -5336,7 +5326,7 @@
       <c r="D114" t="s">
         <v>222</v>
       </c>
-      <c r="E114" s="9">
+      <c r="E114" s="8">
         <v>2006</v>
       </c>
       <c r="F114" t="s">
@@ -5367,7 +5357,7 @@
       <c r="D115" t="s">
         <v>222</v>
       </c>
-      <c r="E115" s="9">
+      <c r="E115" s="8">
         <v>2007</v>
       </c>
       <c r="F115" t="s">
@@ -5398,7 +5388,7 @@
       <c r="D116" t="s">
         <v>222</v>
       </c>
-      <c r="E116" s="9">
+      <c r="E116" s="8">
         <v>2008</v>
       </c>
       <c r="F116" t="s">
@@ -5429,7 +5419,7 @@
       <c r="D117" t="s">
         <v>222</v>
       </c>
-      <c r="E117" s="9">
+      <c r="E117" s="8">
         <v>2009</v>
       </c>
       <c r="F117" t="s">
@@ -5460,7 +5450,7 @@
       <c r="D118" t="s">
         <v>222</v>
       </c>
-      <c r="E118" s="9">
+      <c r="E118" s="8">
         <v>2010</v>
       </c>
       <c r="F118" t="s">
@@ -5491,7 +5481,7 @@
       <c r="D119" t="s">
         <v>222</v>
       </c>
-      <c r="E119" s="9">
+      <c r="E119" s="8">
         <v>2011</v>
       </c>
       <c r="F119" t="s">
@@ -5522,7 +5512,7 @@
       <c r="D120" t="s">
         <v>222</v>
       </c>
-      <c r="E120" s="9">
+      <c r="E120" s="8">
         <v>2012</v>
       </c>
       <c r="F120" t="s">
@@ -5553,7 +5543,7 @@
       <c r="D121" t="s">
         <v>222</v>
       </c>
-      <c r="E121" s="9">
+      <c r="E121" s="8">
         <v>2013</v>
       </c>
       <c r="F121" t="s">
@@ -5584,7 +5574,7 @@
       <c r="D122" t="s">
         <v>222</v>
       </c>
-      <c r="E122" s="9">
+      <c r="E122" s="8">
         <v>2014</v>
       </c>
       <c r="F122" t="s">
@@ -5615,7 +5605,7 @@
       <c r="D123" t="s">
         <v>222</v>
       </c>
-      <c r="E123" s="9">
+      <c r="E123" s="8">
         <v>2015</v>
       </c>
       <c r="F123" t="s">
@@ -5646,7 +5636,7 @@
       <c r="D124" t="s">
         <v>222</v>
       </c>
-      <c r="E124" s="9">
+      <c r="E124" s="8">
         <v>2016</v>
       </c>
       <c r="F124" t="s">
@@ -5677,7 +5667,7 @@
       <c r="D125" t="s">
         <v>222</v>
       </c>
-      <c r="E125" s="9">
+      <c r="E125" s="8">
         <v>2017</v>
       </c>
       <c r="F125" t="s">
@@ -5708,7 +5698,7 @@
       <c r="D126" t="s">
         <v>222</v>
       </c>
-      <c r="E126" s="9">
+      <c r="E126" s="8">
         <v>2018</v>
       </c>
       <c r="F126" t="s">
@@ -5739,7 +5729,7 @@
       <c r="D127" t="s">
         <v>222</v>
       </c>
-      <c r="E127" s="9">
+      <c r="E127" s="8">
         <v>2019</v>
       </c>
       <c r="F127" t="s">
@@ -5770,7 +5760,7 @@
       <c r="D128" t="s">
         <v>222</v>
       </c>
-      <c r="E128" s="9">
+      <c r="E128" s="8">
         <v>2020</v>
       </c>
       <c r="F128" t="s">
@@ -5801,7 +5791,7 @@
       <c r="D129" t="s">
         <v>222</v>
       </c>
-      <c r="E129" s="9">
+      <c r="E129" s="8">
         <v>2000</v>
       </c>
       <c r="F129" t="s">
@@ -5832,7 +5822,7 @@
       <c r="D130" t="s">
         <v>222</v>
       </c>
-      <c r="E130" s="9">
+      <c r="E130" s="8">
         <v>2001</v>
       </c>
       <c r="F130" t="s">
@@ -5863,7 +5853,7 @@
       <c r="D131" t="s">
         <v>222</v>
       </c>
-      <c r="E131" s="9">
+      <c r="E131" s="8">
         <v>2002</v>
       </c>
       <c r="F131" t="s">
@@ -5894,7 +5884,7 @@
       <c r="D132" t="s">
         <v>222</v>
       </c>
-      <c r="E132" s="9">
+      <c r="E132" s="8">
         <v>2003</v>
       </c>
       <c r="F132" t="s">
@@ -5925,7 +5915,7 @@
       <c r="D133" t="s">
         <v>222</v>
       </c>
-      <c r="E133" s="9">
+      <c r="E133" s="8">
         <v>2004</v>
       </c>
       <c r="F133" t="s">
@@ -5956,7 +5946,7 @@
       <c r="D134" t="s">
         <v>222</v>
       </c>
-      <c r="E134" s="9">
+      <c r="E134" s="8">
         <v>2005</v>
       </c>
       <c r="F134" t="s">
@@ -5987,7 +5977,7 @@
       <c r="D135" t="s">
         <v>222</v>
       </c>
-      <c r="E135" s="9">
+      <c r="E135" s="8">
         <v>2006</v>
       </c>
       <c r="F135" t="s">
@@ -6018,7 +6008,7 @@
       <c r="D136" t="s">
         <v>222</v>
       </c>
-      <c r="E136" s="9">
+      <c r="E136" s="8">
         <v>2007</v>
       </c>
       <c r="F136" t="s">
@@ -6049,7 +6039,7 @@
       <c r="D137" t="s">
         <v>222</v>
       </c>
-      <c r="E137" s="9">
+      <c r="E137" s="8">
         <v>2008</v>
       </c>
       <c r="F137" t="s">
@@ -6080,7 +6070,7 @@
       <c r="D138" t="s">
         <v>222</v>
       </c>
-      <c r="E138" s="9">
+      <c r="E138" s="8">
         <v>2009</v>
       </c>
       <c r="F138" t="s">
@@ -6111,7 +6101,7 @@
       <c r="D139" t="s">
         <v>222</v>
       </c>
-      <c r="E139" s="9">
+      <c r="E139" s="8">
         <v>2010</v>
       </c>
       <c r="F139" t="s">
@@ -6142,7 +6132,7 @@
       <c r="D140" t="s">
         <v>222</v>
       </c>
-      <c r="E140" s="9">
+      <c r="E140" s="8">
         <v>2011</v>
       </c>
       <c r="F140" t="s">
@@ -6173,7 +6163,7 @@
       <c r="D141" t="s">
         <v>222</v>
       </c>
-      <c r="E141" s="9">
+      <c r="E141" s="8">
         <v>2012</v>
       </c>
       <c r="F141" t="s">
@@ -6204,7 +6194,7 @@
       <c r="D142" t="s">
         <v>222</v>
       </c>
-      <c r="E142" s="9">
+      <c r="E142" s="8">
         <v>2013</v>
       </c>
       <c r="F142" t="s">
@@ -6235,7 +6225,7 @@
       <c r="D143" t="s">
         <v>222</v>
       </c>
-      <c r="E143" s="9">
+      <c r="E143" s="8">
         <v>2014</v>
       </c>
       <c r="F143" t="s">
@@ -6266,7 +6256,7 @@
       <c r="D144" t="s">
         <v>222</v>
       </c>
-      <c r="E144" s="9">
+      <c r="E144" s="8">
         <v>2015</v>
       </c>
       <c r="F144" t="s">
@@ -6297,7 +6287,7 @@
       <c r="D145" t="s">
         <v>222</v>
       </c>
-      <c r="E145" s="9">
+      <c r="E145" s="8">
         <v>2016</v>
       </c>
       <c r="F145" t="s">
@@ -6328,7 +6318,7 @@
       <c r="D146" t="s">
         <v>222</v>
       </c>
-      <c r="E146" s="9">
+      <c r="E146" s="8">
         <v>2017</v>
       </c>
       <c r="F146" t="s">
@@ -6359,7 +6349,7 @@
       <c r="D147" t="s">
         <v>222</v>
       </c>
-      <c r="E147" s="9">
+      <c r="E147" s="8">
         <v>2018</v>
       </c>
       <c r="F147" t="s">
@@ -6390,7 +6380,7 @@
       <c r="D148" t="s">
         <v>222</v>
       </c>
-      <c r="E148" s="9">
+      <c r="E148" s="8">
         <v>2019</v>
       </c>
       <c r="F148" t="s">
@@ -6421,7 +6411,7 @@
       <c r="D149" t="s">
         <v>222</v>
       </c>
-      <c r="E149" s="9">
+      <c r="E149" s="8">
         <v>2020</v>
       </c>
       <c r="F149" t="s">
@@ -6452,7 +6442,7 @@
       <c r="D150" t="s">
         <v>222</v>
       </c>
-      <c r="E150" s="9">
+      <c r="E150" s="8">
         <v>2021</v>
       </c>
       <c r="F150" t="s">
@@ -6483,7 +6473,7 @@
       <c r="D151" t="s">
         <v>222</v>
       </c>
-      <c r="E151" s="9">
+      <c r="E151" s="8">
         <v>2022</v>
       </c>
       <c r="F151" t="s">
@@ -6514,7 +6504,7 @@
       <c r="D152" t="s">
         <v>222</v>
       </c>
-      <c r="E152" s="9">
+      <c r="E152" s="8">
         <v>2023</v>
       </c>
       <c r="F152" t="s">
@@ -6545,7 +6535,7 @@
       <c r="D153" t="s">
         <v>222</v>
       </c>
-      <c r="E153" s="9">
+      <c r="E153" s="8">
         <v>2024</v>
       </c>
       <c r="F153" t="s">
@@ -6576,7 +6566,7 @@
       <c r="D154" t="s">
         <v>222</v>
       </c>
-      <c r="E154" s="9">
+      <c r="E154" s="8">
         <v>2025</v>
       </c>
       <c r="F154" t="s">
@@ -6607,7 +6597,7 @@
       <c r="D155" t="s">
         <v>49</v>
       </c>
-      <c r="E155" s="11" t="s">
+      <c r="E155" t="s">
         <v>271</v>
       </c>
       <c r="F155" t="s">
@@ -6643,7 +6633,7 @@
       <c r="D156" t="s">
         <v>45</v>
       </c>
-      <c r="E156" s="11" t="s">
+      <c r="E156" t="s">
         <v>271</v>
       </c>
       <c r="F156" t="s">
@@ -6679,7 +6669,7 @@
       <c r="D157" t="s">
         <v>189</v>
       </c>
-      <c r="E157" s="11" t="s">
+      <c r="E157" t="s">
         <v>271</v>
       </c>
       <c r="F157" t="s">
@@ -6715,7 +6705,7 @@
       <c r="D158" t="s">
         <v>275</v>
       </c>
-      <c r="E158" s="11" t="s">
+      <c r="E158" t="s">
         <v>271</v>
       </c>
       <c r="F158" t="s">
@@ -6751,7 +6741,7 @@
       <c r="D159" t="s">
         <v>275</v>
       </c>
-      <c r="E159" s="11" t="s">
+      <c r="E159" t="s">
         <v>271</v>
       </c>
       <c r="F159" t="s">
@@ -6787,7 +6777,7 @@
       <c r="D160" t="s">
         <v>189</v>
       </c>
-      <c r="E160" s="11" t="s">
+      <c r="E160" t="s">
         <v>278</v>
       </c>
       <c r="F160" t="s">
@@ -6823,7 +6813,7 @@
       <c r="D161" t="s">
         <v>49</v>
       </c>
-      <c r="E161" s="11" t="s">
+      <c r="E161" t="s">
         <v>280</v>
       </c>
       <c r="F161" t="s">
@@ -6861,7 +6851,7 @@
       <c r="D162" t="s">
         <v>45</v>
       </c>
-      <c r="E162" s="11" t="s">
+      <c r="E162" t="s">
         <v>280</v>
       </c>
       <c r="F162" t="s">
@@ -6899,7 +6889,7 @@
       <c r="D163" t="s">
         <v>189</v>
       </c>
-      <c r="E163" s="11" t="s">
+      <c r="E163" t="s">
         <v>280</v>
       </c>
       <c r="F163" t="s">
@@ -6937,7 +6927,7 @@
       <c r="D164" t="s">
         <v>284</v>
       </c>
-      <c r="E164" s="11" t="s">
+      <c r="E164" t="s">
         <v>285</v>
       </c>
       <c r="F164" t="s">
@@ -6975,7 +6965,7 @@
       <c r="D165" t="s">
         <v>189</v>
       </c>
-      <c r="E165" s="11" t="s">
+      <c r="E165" t="s">
         <v>280</v>
       </c>
       <c r="F165" t="s">
@@ -7013,7 +7003,7 @@
       <c r="D166" t="s">
         <v>23</v>
       </c>
-      <c r="E166" s="9">
+      <c r="E166" s="8">
         <v>2020</v>
       </c>
       <c r="F166" t="s">
@@ -7050,7 +7040,7 @@
       <c r="D167" t="s">
         <v>289</v>
       </c>
-      <c r="E167" s="9">
+      <c r="E167" s="8">
         <v>2020</v>
       </c>
       <c r="F167" t="s">
@@ -7087,7 +7077,7 @@
       <c r="D168" t="s">
         <v>23</v>
       </c>
-      <c r="E168" s="9">
+      <c r="E168" s="8">
         <v>2020</v>
       </c>
       <c r="F168" t="s">
@@ -7124,7 +7114,7 @@
       <c r="D169" t="s">
         <v>294</v>
       </c>
-      <c r="E169" s="9">
+      <c r="E169" s="8">
         <v>2020</v>
       </c>
       <c r="F169" t="s">
@@ -7161,7 +7151,7 @@
       <c r="D170" t="s">
         <v>296</v>
       </c>
-      <c r="E170" s="9">
+      <c r="E170" s="8">
         <v>2020</v>
       </c>
       <c r="F170" t="s">
@@ -7198,7 +7188,7 @@
       <c r="D171" t="s">
         <v>298</v>
       </c>
-      <c r="E171" s="9">
+      <c r="E171" s="8">
         <v>2015</v>
       </c>
       <c r="F171" t="s">
@@ -7235,7 +7225,7 @@
       <c r="D172" t="s">
         <v>302</v>
       </c>
-      <c r="E172" s="9">
+      <c r="E172" s="8">
         <v>2023</v>
       </c>
       <c r="F172" t="s">
@@ -7272,7 +7262,7 @@
       <c r="D173" t="s">
         <v>305</v>
       </c>
-      <c r="E173" s="9">
+      <c r="E173" s="8">
         <v>2023</v>
       </c>
       <c r="F173" t="s">
@@ -7304,13 +7294,16 @@
         <v>16</v>
       </c>
       <c r="D174" t="s">
-        <v>305</v>
-      </c>
-      <c r="E174" s="9">
-        <v>2022</v>
+        <v>61</v>
+      </c>
+      <c r="E174" s="8">
+        <v>2023</v>
       </c>
       <c r="F174" t="s">
-        <v>308</v>
+        <v>121</v>
+      </c>
+      <c r="G174" t="s">
+        <v>79</v>
       </c>
       <c r="H174" s="3">
         <v>0</v>
@@ -7324,7 +7317,7 @@
         <v>1</v>
       </c>
       <c r="M174" s="4" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="175" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7338,9 +7331,9 @@
         <v>16</v>
       </c>
       <c r="D175" t="s">
-        <v>61</v>
-      </c>
-      <c r="E175" s="9">
+        <v>133</v>
+      </c>
+      <c r="E175" s="8">
         <v>2023</v>
       </c>
       <c r="F175" t="s">
@@ -7361,12 +7354,12 @@
         <v>1</v>
       </c>
       <c r="M175" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B176" t="s">
         <v>15</v>
@@ -7375,9 +7368,9 @@
         <v>16</v>
       </c>
       <c r="D176" t="s">
-        <v>133</v>
-      </c>
-      <c r="E176" s="9">
+        <v>59</v>
+      </c>
+      <c r="E176" s="8">
         <v>2023</v>
       </c>
       <c r="F176" t="s">
@@ -7398,12 +7391,12 @@
         <v>1</v>
       </c>
       <c r="M176" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B177" t="s">
         <v>15</v>
@@ -7412,9 +7405,9 @@
         <v>16</v>
       </c>
       <c r="D177" t="s">
-        <v>59</v>
-      </c>
-      <c r="E177" s="9">
+        <v>73</v>
+      </c>
+      <c r="E177" s="8">
         <v>2023</v>
       </c>
       <c r="F177" t="s">
@@ -7435,12 +7428,12 @@
         <v>1</v>
       </c>
       <c r="M177" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>313</v>
+        <v>354</v>
       </c>
       <c r="B178" t="s">
         <v>15</v>
@@ -7449,13 +7442,13 @@
         <v>16</v>
       </c>
       <c r="D178" t="s">
-        <v>73</v>
-      </c>
-      <c r="E178" s="9">
-        <v>2023</v>
+        <v>312</v>
+      </c>
+      <c r="E178" s="8" t="s">
+        <v>355</v>
       </c>
       <c r="F178" t="s">
-        <v>121</v>
+        <v>306</v>
       </c>
       <c r="G178" t="s">
         <v>79</v>
@@ -7472,27 +7465,27 @@
         <v>1</v>
       </c>
       <c r="M178" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="179" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>313</v>
+      </c>
+      <c r="B179" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" t="s">
+        <v>16</v>
+      </c>
+      <c r="D179" t="s">
         <v>314</v>
       </c>
-      <c r="B179" t="s">
-        <v>15</v>
-      </c>
-      <c r="C179" t="s">
-        <v>16</v>
-      </c>
-      <c r="D179" t="s">
+      <c r="E179" s="8">
+        <v>2015</v>
+      </c>
+      <c r="F179" t="s">
         <v>315</v>
-      </c>
-      <c r="E179" s="9">
-        <v>2023</v>
-      </c>
-      <c r="F179" t="s">
-        <v>306</v>
       </c>
       <c r="G179" t="s">
         <v>79</v>
@@ -7509,101 +7502,79 @@
         <v>1</v>
       </c>
       <c r="M179" s="4" t="s">
-        <v>310</v>
+        <v>316</v>
+      </c>
+      <c r="N179" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="180" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B180" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="C180" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="D180" t="s">
-        <v>315</v>
-      </c>
-      <c r="E180" s="9">
-        <v>2022</v>
+        <v>319</v>
+      </c>
+      <c r="E180" t="s">
+        <v>76</v>
       </c>
       <c r="F180" t="s">
-        <v>308</v>
+        <v>78</v>
       </c>
       <c r="G180" t="s">
         <v>79</v>
       </c>
-      <c r="H180" s="3">
-        <v>0</v>
-      </c>
-      <c r="I180" s="4"/>
-      <c r="J180" s="3">
-        <v>0</v>
-      </c>
-      <c r="K180" s="4"/>
-      <c r="L180" s="3">
-        <v>1</v>
-      </c>
-      <c r="M180" s="4" t="s">
-        <v>310</v>
+      <c r="N180" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="181" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B181" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="C181" t="s">
-        <v>16</v>
+        <v>321</v>
       </c>
       <c r="D181" t="s">
-        <v>318</v>
-      </c>
-      <c r="E181" s="9">
-        <v>2015</v>
+        <v>322</v>
+      </c>
+      <c r="E181" s="8">
+        <v>2020</v>
       </c>
       <c r="F181" t="s">
-        <v>319</v>
+        <v>78</v>
       </c>
       <c r="G181" t="s">
         <v>79</v>
       </c>
-      <c r="H181" s="3">
-        <v>0</v>
-      </c>
-      <c r="I181" s="4"/>
-      <c r="J181" s="3">
-        <v>0</v>
-      </c>
-      <c r="K181" s="4"/>
-      <c r="L181" s="3">
-        <v>1</v>
-      </c>
-      <c r="M181" s="4" t="s">
-        <v>320</v>
-      </c>
       <c r="N181" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="182" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B182" t="s">
         <v>81</v>
       </c>
       <c r="C182" t="s">
-        <v>76</v>
+        <v>321</v>
       </c>
       <c r="D182" t="s">
-        <v>323</v>
-      </c>
-      <c r="E182" s="11" t="s">
-        <v>76</v>
+        <v>325</v>
+      </c>
+      <c r="E182" s="8">
+        <v>2020</v>
       </c>
       <c r="F182" t="s">
         <v>78</v>
@@ -7612,24 +7583,24 @@
         <v>79</v>
       </c>
       <c r="N182" t="s">
-        <v>98</v>
+        <v>323</v>
       </c>
     </row>
     <row r="183" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B183" t="s">
         <v>81</v>
       </c>
       <c r="C183" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D183" t="s">
-        <v>326</v>
-      </c>
-      <c r="E183" s="9">
-        <v>2020</v>
+        <v>327</v>
+      </c>
+      <c r="E183" t="s">
+        <v>271</v>
       </c>
       <c r="F183" t="s">
         <v>78</v>
@@ -7638,7 +7609,7 @@
         <v>79</v>
       </c>
       <c r="N183" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="184" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7649,13 +7620,13 @@
         <v>81</v>
       </c>
       <c r="C184" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D184" t="s">
+        <v>327</v>
+      </c>
+      <c r="E184" t="s">
         <v>329</v>
-      </c>
-      <c r="E184" s="9">
-        <v>2020</v>
       </c>
       <c r="F184" t="s">
         <v>78</v>
@@ -7664,7 +7635,7 @@
         <v>79</v>
       </c>
       <c r="N184" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7675,13 +7646,13 @@
         <v>81</v>
       </c>
       <c r="C185" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D185" t="s">
         <v>331</v>
       </c>
-      <c r="E185" s="11" t="s">
-        <v>271</v>
+      <c r="E185" s="8">
+        <v>2020</v>
       </c>
       <c r="F185" t="s">
         <v>78</v>
@@ -7690,7 +7661,7 @@
         <v>79</v>
       </c>
       <c r="N185" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="186" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7701,13 +7672,13 @@
         <v>81</v>
       </c>
       <c r="C186" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D186" t="s">
-        <v>331</v>
-      </c>
-      <c r="E186" s="11" t="s">
         <v>333</v>
+      </c>
+      <c r="E186" s="8">
+        <v>2020</v>
       </c>
       <c r="F186" t="s">
         <v>78</v>
@@ -7716,7 +7687,7 @@
         <v>79</v>
       </c>
       <c r="N186" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="187" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7727,12 +7698,12 @@
         <v>81</v>
       </c>
       <c r="C187" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D187" t="s">
         <v>335</v>
       </c>
-      <c r="E187" s="9">
+      <c r="E187" s="8">
         <v>2020</v>
       </c>
       <c r="F187" t="s">
@@ -7742,7 +7713,7 @@
         <v>79</v>
       </c>
       <c r="N187" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="188" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7753,13 +7724,13 @@
         <v>81</v>
       </c>
       <c r="C188" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D188" t="s">
-        <v>337</v>
-      </c>
-      <c r="E188" s="9">
-        <v>2020</v>
+        <v>335</v>
+      </c>
+      <c r="E188" t="s">
+        <v>329</v>
       </c>
       <c r="F188" t="s">
         <v>78</v>
@@ -7768,24 +7739,24 @@
         <v>79</v>
       </c>
       <c r="N188" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="189" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B189" t="s">
         <v>81</v>
       </c>
       <c r="C189" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D189" t="s">
-        <v>339</v>
-      </c>
-      <c r="E189" s="9">
-        <v>2020</v>
+        <v>322</v>
+      </c>
+      <c r="E189" t="s">
+        <v>329</v>
       </c>
       <c r="F189" t="s">
         <v>78</v>
@@ -7794,24 +7765,24 @@
         <v>79</v>
       </c>
       <c r="N189" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="190" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B190" t="s">
         <v>81</v>
       </c>
       <c r="C190" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D190" t="s">
         <v>339</v>
       </c>
-      <c r="E190" s="11" t="s">
-        <v>333</v>
+      <c r="E190" t="s">
+        <v>329</v>
       </c>
       <c r="F190" t="s">
         <v>78</v>
@@ -7820,24 +7791,24 @@
         <v>79</v>
       </c>
       <c r="N190" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="191" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B191" t="s">
         <v>81</v>
       </c>
       <c r="C191" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D191" t="s">
-        <v>326</v>
-      </c>
-      <c r="E191" s="11" t="s">
-        <v>333</v>
+        <v>341</v>
+      </c>
+      <c r="E191" s="8">
+        <v>2015</v>
       </c>
       <c r="F191" t="s">
         <v>78</v>
@@ -7846,7 +7817,7 @@
         <v>79</v>
       </c>
       <c r="N191" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="192" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7857,13 +7828,13 @@
         <v>81</v>
       </c>
       <c r="C192" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="D192" t="s">
-        <v>343</v>
-      </c>
-      <c r="E192" s="11" t="s">
-        <v>333</v>
+        <v>344</v>
+      </c>
+      <c r="E192" t="s">
+        <v>76</v>
       </c>
       <c r="F192" t="s">
         <v>78</v>
@@ -7872,24 +7843,24 @@
         <v>79</v>
       </c>
       <c r="N192" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
     </row>
     <row r="193" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B193" t="s">
         <v>81</v>
       </c>
       <c r="C193" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="D193" t="s">
-        <v>345</v>
-      </c>
-      <c r="E193" s="9">
-        <v>2015</v>
+        <v>347</v>
+      </c>
+      <c r="E193" t="s">
+        <v>76</v>
       </c>
       <c r="F193" t="s">
         <v>78</v>
@@ -7898,23 +7869,23 @@
         <v>79</v>
       </c>
       <c r="N193" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="194" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B194" t="s">
         <v>81</v>
       </c>
       <c r="C194" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D194" t="s">
-        <v>348</v>
-      </c>
-      <c r="E194" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="E194" t="s">
         <v>76</v>
       </c>
       <c r="F194" t="s">
@@ -7924,59 +7895,7 @@
         <v>79</v>
       </c>
       <c r="N194" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="195" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
-        <v>350</v>
-      </c>
-      <c r="B195" t="s">
-        <v>81</v>
-      </c>
-      <c r="C195" t="s">
-        <v>347</v>
-      </c>
-      <c r="D195" t="s">
         <v>351</v>
-      </c>
-      <c r="E195" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F195" t="s">
-        <v>78</v>
-      </c>
-      <c r="G195" t="s">
-        <v>79</v>
-      </c>
-      <c r="N195" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="196" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>353</v>
-      </c>
-      <c r="B196" t="s">
-        <v>81</v>
-      </c>
-      <c r="C196" t="s">
-        <v>347</v>
-      </c>
-      <c r="D196" t="s">
-        <v>354</v>
-      </c>
-      <c r="E196" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F196" t="s">
-        <v>78</v>
-      </c>
-      <c r="G196" t="s">
-        <v>79</v>
-      </c>
-      <c r="N196" t="s">
-        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -7995,10 +7914,10 @@
       <selection activeCell="E10" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
@@ -8021,7 +7940,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -8065,7 +7984,7 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>2020</v>
       </c>
       <c r="F2" t="s">
@@ -8103,7 +8022,7 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>2020</v>
       </c>
       <c r="F3" t="s">
@@ -8141,7 +8060,7 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>2020</v>
       </c>
       <c r="F4" t="s">
@@ -8179,7 +8098,7 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>2020</v>
       </c>
       <c r="F5" t="s">
@@ -8217,7 +8136,7 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>2020</v>
       </c>
       <c r="F6" t="s">
@@ -8255,7 +8174,7 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>2020</v>
       </c>
       <c r="F7" t="s">
@@ -8293,7 +8212,7 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>2020</v>
       </c>
       <c r="F8" t="s">
@@ -8331,7 +8250,7 @@
       <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>2020</v>
       </c>
       <c r="F9" t="s">
@@ -8358,7 +8277,7 @@
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -8369,7 +8288,7 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>2020</v>
       </c>
       <c r="F10" t="s">
@@ -8407,7 +8326,7 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>2020</v>
       </c>
       <c r="F11" t="s">
@@ -8445,7 +8364,7 @@
       <c r="D12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>2020</v>
       </c>
       <c r="F12" t="s">
@@ -8483,7 +8402,7 @@
       <c r="D13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>2020</v>
       </c>
       <c r="F13" t="s">
@@ -8521,7 +8440,7 @@
       <c r="D14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>2020</v>
       </c>
       <c r="F14" t="s">
@@ -8559,7 +8478,7 @@
       <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F15" t="s">
@@ -8597,7 +8516,7 @@
       <c r="D16" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="F16" t="s">
@@ -8635,7 +8554,7 @@
       <c r="D17" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F17" t="s">
@@ -8673,7 +8592,7 @@
       <c r="D18" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F18" t="s">
@@ -8711,7 +8630,7 @@
       <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>2020</v>
       </c>
       <c r="F19" t="s">
@@ -8749,7 +8668,7 @@
       <c r="D20" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>2020</v>
       </c>
       <c r="F20" t="s">
@@ -8787,7 +8706,7 @@
       <c r="D21" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>2020</v>
       </c>
       <c r="F21" t="s">
@@ -8825,7 +8744,7 @@
       <c r="D22" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>2020</v>
       </c>
       <c r="F22" t="s">
@@ -8863,7 +8782,7 @@
       <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>2020</v>
       </c>
       <c r="F23" t="s">
@@ -8901,7 +8820,7 @@
       <c r="D24" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>2020</v>
       </c>
       <c r="F24" t="s">
@@ -8939,7 +8858,7 @@
       <c r="D25" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>2020</v>
       </c>
       <c r="F25" t="s">
@@ -8977,7 +8896,7 @@
       <c r="D26" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>2020</v>
       </c>
       <c r="F26" t="s">
@@ -9015,7 +8934,7 @@
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>2020</v>
       </c>
       <c r="F27" t="s">
@@ -9053,7 +8972,7 @@
       <c r="D28" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>2020</v>
       </c>
       <c r="F28" t="s">
@@ -9091,7 +9010,7 @@
       <c r="D29" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>2020</v>
       </c>
       <c r="F29" t="s">

</xml_diff>

<commit_message>
updated risk metrics to not use ESA and GFC (GLAD) treeecover for 2020. Removal rational due to high commission errors for indicator 1 when comparing to 21,752 reference points from JRC (as used in testing the EUFO 2020 map)
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="357">
   <si>
     <t>Column name</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Hansen 2013</t>
+  </si>
+  <si>
+    <t>Removed from standard risk metrics due to commission errors</t>
   </si>
   <si>
     <t>Forest_FDaP</t>
@@ -1192,9 +1195,6 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -1204,11 +1204,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1523,20 +1526,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="31.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="33.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="14" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="14.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="14" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="14" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="18.14785714285714" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="14" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="20.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1596,7 +1599,7 @@
       <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1605,19 +1608,19 @@
       <c r="G2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1625,7 +1628,7 @@
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>81</v>
       </c>
@@ -1638,7 +1641,7 @@
       <c r="D3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1647,19 +1650,19 @@
       <c r="G3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M3" s="3" t="s">
@@ -1669,7 +1672,7 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>85</v>
       </c>
@@ -1682,7 +1685,7 @@
       <c r="D4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -1691,19 +1694,19 @@
       <c r="G4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M4" s="3" t="s">
@@ -1711,7 +1714,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>88</v>
       </c>
@@ -1724,7 +1727,7 @@
       <c r="D5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1733,19 +1736,19 @@
       <c r="G5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M5" s="3" t="s">
@@ -1753,7 +1756,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>90</v>
       </c>
@@ -1766,7 +1769,7 @@
       <c r="D6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1775,19 +1778,19 @@
       <c r="G6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M6" s="3" t="s">
@@ -1795,7 +1798,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>93</v>
       </c>
@@ -1808,7 +1811,7 @@
       <c r="D7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1817,19 +1820,19 @@
       <c r="G7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M7" s="3" t="s">
@@ -1837,7 +1840,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
@@ -1850,7 +1853,7 @@
       <c r="D8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1859,19 +1862,19 @@
       <c r="G8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M8" s="3" t="s">
@@ -1879,7 +1882,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>97</v>
       </c>
@@ -1892,7 +1895,7 @@
       <c r="D9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1901,19 +1904,19 @@
       <c r="G9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M9" s="3" t="s">
@@ -1923,7 +1926,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>101</v>
       </c>
@@ -1936,7 +1939,7 @@
       <c r="D10" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1945,19 +1948,19 @@
       <c r="G10" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1967,7 +1970,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>103</v>
       </c>
@@ -1980,7 +1983,7 @@
       <c r="D11" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1989,19 +1992,19 @@
       <c r="G11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M11" s="3" t="s">
@@ -2009,7 +2012,7 @@
       </c>
       <c r="N11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>106</v>
       </c>
@@ -2031,19 +2034,19 @@
       <c r="G12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>77</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>77</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>77</v>
       </c>
       <c r="M12" s="3" t="s">
@@ -2051,7 +2054,7 @@
       </c>
       <c r="N12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>111</v>
       </c>
@@ -2093,7 +2096,7 @@
       </c>
       <c r="N13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>113</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>116</v>
       </c>
@@ -2202,28 +2205,30 @@
         <v>80</v>
       </c>
       <c r="H16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>15</v>
@@ -2232,13 +2237,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E17" s="4">
         <v>2020</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>80</v>
@@ -2265,7 +2270,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
@@ -2280,34 +2285,36 @@
         <v>2020</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="L18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>15</v>
@@ -2349,7 +2356,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
@@ -2364,7 +2371,7 @@
         <v>2020</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>80</v>
@@ -2391,7 +2398,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>15</v>
@@ -2406,7 +2413,7 @@
         <v>2020</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>80</v>
@@ -2433,7 +2440,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>15</v>
@@ -2448,7 +2455,7 @@
         <v>2020</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>80</v>
@@ -2475,7 +2482,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>15</v>
@@ -2490,7 +2497,7 @@
         <v>2020</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>80</v>
@@ -2517,7 +2524,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>15</v>
@@ -2532,7 +2539,7 @@
         <v>2020</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>80</v>
@@ -2559,7 +2566,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>15</v>
@@ -2568,13 +2575,13 @@
         <v>16</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E25" s="4">
         <v>2020</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>80</v>
@@ -2601,22 +2608,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="E26" s="4">
         <v>2020</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>80</v>
@@ -2643,7 +2650,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>15</v>
@@ -2658,7 +2665,7 @@
         <v>2020</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>80</v>
@@ -2685,7 +2692,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>15</v>
@@ -2719,7 +2726,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>15</v>
@@ -2753,7 +2760,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>15</v>
@@ -2787,7 +2794,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>15</v>
@@ -2821,7 +2828,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>15</v>
@@ -2855,7 +2862,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>15</v>
@@ -2889,7 +2896,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>15</v>
@@ -2923,7 +2930,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>15</v>
@@ -2957,7 +2964,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>15</v>
@@ -2991,7 +2998,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>15</v>
@@ -3025,7 +3032,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>15</v>
@@ -3059,7 +3066,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>15</v>
@@ -3093,7 +3100,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>15</v>
@@ -3127,7 +3134,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>15</v>
@@ -3161,7 +3168,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>15</v>
@@ -3195,7 +3202,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>15</v>
@@ -3229,7 +3236,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
@@ -3263,7 +3270,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>15</v>
@@ -3297,7 +3304,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>15</v>
@@ -3331,7 +3338,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>15</v>
@@ -3365,7 +3372,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>15</v>
@@ -3399,7 +3406,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>15</v>
@@ -3433,7 +3440,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>15</v>
@@ -3467,7 +3474,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>15</v>
@@ -3501,7 +3508,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>15</v>
@@ -3535,7 +3542,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>15</v>
@@ -3569,7 +3576,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>15</v>
@@ -3603,7 +3610,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>15</v>
@@ -3637,7 +3644,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>15</v>
@@ -3671,7 +3678,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>15</v>
@@ -3705,7 +3712,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>15</v>
@@ -3739,7 +3746,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>15</v>
@@ -3773,7 +3780,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>15</v>
@@ -3807,7 +3814,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>15</v>
@@ -3841,7 +3848,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>15</v>
@@ -3875,7 +3882,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>15</v>
@@ -3909,7 +3916,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>15</v>
@@ -3943,7 +3950,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>15</v>
@@ -3977,7 +3984,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>15</v>
@@ -4011,7 +4018,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>15</v>
@@ -4045,7 +4052,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>15</v>
@@ -4079,7 +4086,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>15</v>
@@ -4113,7 +4120,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>15</v>
@@ -4147,7 +4154,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>15</v>
@@ -4181,7 +4188,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>15</v>
@@ -4215,7 +4222,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>15</v>
@@ -4249,7 +4256,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>15</v>
@@ -4283,7 +4290,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>15</v>
@@ -4317,7 +4324,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>15</v>
@@ -4351,7 +4358,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>15</v>
@@ -4385,7 +4392,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>15</v>
@@ -4394,7 +4401,7 @@
         <v>16</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E78" s="4">
         <v>2001</v>
@@ -4419,16 +4426,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="E79" s="4">
         <v>2002</v>
@@ -4453,7 +4460,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>15</v>
@@ -4462,7 +4469,7 @@
         <v>16</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E80" s="4">
         <v>2003</v>
@@ -4487,7 +4494,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>15</v>
@@ -4496,7 +4503,7 @@
         <v>16</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E81" s="4">
         <v>2004</v>
@@ -4521,7 +4528,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>15</v>
@@ -4530,7 +4537,7 @@
         <v>16</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E82" s="4">
         <v>2005</v>
@@ -4555,7 +4562,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>15</v>
@@ -4564,7 +4571,7 @@
         <v>16</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E83" s="4">
         <v>2006</v>
@@ -4589,7 +4596,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>15</v>
@@ -4598,7 +4605,7 @@
         <v>16</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E84" s="4">
         <v>2007</v>
@@ -4623,7 +4630,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>15</v>
@@ -4632,7 +4639,7 @@
         <v>16</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E85" s="4">
         <v>2008</v>
@@ -4657,7 +4664,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>15</v>
@@ -4666,7 +4673,7 @@
         <v>16</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E86" s="4">
         <v>2009</v>
@@ -4691,7 +4698,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>15</v>
@@ -4700,7 +4707,7 @@
         <v>16</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E87" s="4">
         <v>2010</v>
@@ -4725,7 +4732,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>15</v>
@@ -4734,7 +4741,7 @@
         <v>16</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E88" s="4">
         <v>2011</v>
@@ -4759,7 +4766,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>15</v>
@@ -4768,7 +4775,7 @@
         <v>16</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E89" s="4">
         <v>2012</v>
@@ -4793,7 +4800,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>15</v>
@@ -4802,7 +4809,7 @@
         <v>16</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E90" s="4">
         <v>2013</v>
@@ -4827,7 +4834,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>15</v>
@@ -4836,7 +4843,7 @@
         <v>16</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E91" s="4">
         <v>2014</v>
@@ -4861,7 +4868,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>15</v>
@@ -4870,7 +4877,7 @@
         <v>16</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E92" s="4">
         <v>2015</v>
@@ -4895,7 +4902,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>15</v>
@@ -4904,7 +4911,7 @@
         <v>16</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E93" s="4">
         <v>2016</v>
@@ -4929,7 +4936,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>15</v>
@@ -4938,7 +4945,7 @@
         <v>16</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E94" s="4">
         <v>2017</v>
@@ -4963,7 +4970,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>15</v>
@@ -4972,7 +4979,7 @@
         <v>16</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E95" s="4">
         <v>2018</v>
@@ -4997,7 +5004,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>15</v>
@@ -5006,7 +5013,7 @@
         <v>16</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E96" s="4">
         <v>2019</v>
@@ -5031,7 +5038,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>15</v>
@@ -5040,7 +5047,7 @@
         <v>16</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E97" s="4">
         <v>2020</v>
@@ -5065,7 +5072,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>15</v>
@@ -5074,7 +5081,7 @@
         <v>16</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E98" s="4">
         <v>2021</v>
@@ -5099,7 +5106,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>15</v>
@@ -5108,7 +5115,7 @@
         <v>16</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E99" s="4">
         <v>2022</v>
@@ -5133,7 +5140,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>15</v>
@@ -5142,7 +5149,7 @@
         <v>16</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E100" s="4">
         <v>2023</v>
@@ -5167,7 +5174,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>15</v>
@@ -5176,7 +5183,7 @@
         <v>16</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E101" s="4">
         <v>2024</v>
@@ -5201,7 +5208,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>15</v>
@@ -5210,13 +5217,13 @@
         <v>16</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E102" s="4">
         <v>2019</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G102" s="3"/>
       <c r="H102" s="5">
@@ -5235,7 +5242,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>15</v>
@@ -5244,13 +5251,13 @@
         <v>16</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E103" s="4">
         <v>2020</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G103" s="3"/>
       <c r="H103" s="5">
@@ -5269,7 +5276,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>15</v>
@@ -5278,13 +5285,13 @@
         <v>16</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E104" s="4">
         <v>2021</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G104" s="3"/>
       <c r="H104" s="5">
@@ -5303,7 +5310,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>15</v>
@@ -5312,13 +5319,13 @@
         <v>16</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E105" s="4">
         <v>2022</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G105" s="3"/>
       <c r="H105" s="5">
@@ -5337,7 +5344,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>15</v>
@@ -5346,13 +5353,13 @@
         <v>16</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E106" s="4">
         <v>2023</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G106" s="3"/>
       <c r="H106" s="5">
@@ -5371,7 +5378,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>15</v>
@@ -5380,13 +5387,13 @@
         <v>16</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E107" s="4">
         <v>2024</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G107" s="3"/>
       <c r="H107" s="5">
@@ -5405,7 +5412,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>15</v>
@@ -5414,13 +5421,13 @@
         <v>16</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E108" s="4">
         <v>2025</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G108" s="3"/>
       <c r="H108" s="5">
@@ -5439,7 +5446,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>15</v>
@@ -5448,13 +5455,13 @@
         <v>16</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E109" s="4">
         <v>2001</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G109" s="3"/>
       <c r="H109" s="5">
@@ -5473,7 +5480,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>15</v>
@@ -5482,13 +5489,13 @@
         <v>16</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E110" s="4">
         <v>2002</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G110" s="3"/>
       <c r="H110" s="5">
@@ -5507,7 +5514,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>15</v>
@@ -5516,13 +5523,13 @@
         <v>16</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E111" s="4">
         <v>2003</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G111" s="3"/>
       <c r="H111" s="5">
@@ -5541,7 +5548,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>15</v>
@@ -5550,13 +5557,13 @@
         <v>16</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E112" s="4">
         <v>2004</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G112" s="3"/>
       <c r="H112" s="5">
@@ -5575,7 +5582,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>15</v>
@@ -5584,13 +5591,13 @@
         <v>16</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E113" s="4">
         <v>2005</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G113" s="3"/>
       <c r="H113" s="5">
@@ -5609,7 +5616,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>15</v>
@@ -5618,13 +5625,13 @@
         <v>16</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E114" s="4">
         <v>2006</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G114" s="3"/>
       <c r="H114" s="5">
@@ -5643,7 +5650,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>15</v>
@@ -5652,13 +5659,13 @@
         <v>16</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E115" s="4">
         <v>2007</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G115" s="3"/>
       <c r="H115" s="5">
@@ -5677,7 +5684,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>15</v>
@@ -5686,13 +5693,13 @@
         <v>16</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E116" s="4">
         <v>2008</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G116" s="3"/>
       <c r="H116" s="5">
@@ -5711,7 +5718,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>15</v>
@@ -5720,13 +5727,13 @@
         <v>16</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E117" s="4">
         <v>2009</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G117" s="3"/>
       <c r="H117" s="5">
@@ -5745,7 +5752,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>15</v>
@@ -5754,13 +5761,13 @@
         <v>16</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E118" s="4">
         <v>2010</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G118" s="3"/>
       <c r="H118" s="5">
@@ -5779,7 +5786,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>15</v>
@@ -5788,13 +5795,13 @@
         <v>16</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E119" s="4">
         <v>2011</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G119" s="3"/>
       <c r="H119" s="5">
@@ -5813,7 +5820,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>15</v>
@@ -5822,13 +5829,13 @@
         <v>16</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E120" s="4">
         <v>2012</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G120" s="3"/>
       <c r="H120" s="5">
@@ -5847,7 +5854,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>15</v>
@@ -5856,13 +5863,13 @@
         <v>16</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E121" s="4">
         <v>2013</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G121" s="3"/>
       <c r="H121" s="5">
@@ -5881,7 +5888,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>15</v>
@@ -5890,13 +5897,13 @@
         <v>16</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E122" s="4">
         <v>2014</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G122" s="3"/>
       <c r="H122" s="5">
@@ -5915,7 +5922,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>15</v>
@@ -5924,13 +5931,13 @@
         <v>16</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E123" s="4">
         <v>2015</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G123" s="3"/>
       <c r="H123" s="5">
@@ -5949,7 +5956,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>15</v>
@@ -5958,13 +5965,13 @@
         <v>16</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E124" s="4">
         <v>2016</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G124" s="3"/>
       <c r="H124" s="5">
@@ -5983,7 +5990,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>15</v>
@@ -5992,13 +5999,13 @@
         <v>16</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E125" s="4">
         <v>2017</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="5">
@@ -6017,7 +6024,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>15</v>
@@ -6026,13 +6033,13 @@
         <v>16</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E126" s="4">
         <v>2018</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="5">
@@ -6051,7 +6058,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>15</v>
@@ -6060,13 +6067,13 @@
         <v>16</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E127" s="4">
         <v>2019</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G127" s="3"/>
       <c r="H127" s="5">
@@ -6085,7 +6092,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>15</v>
@@ -6094,13 +6101,13 @@
         <v>16</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E128" s="4">
         <v>2020</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G128" s="3"/>
       <c r="H128" s="5">
@@ -6119,7 +6126,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>15</v>
@@ -6128,13 +6135,13 @@
         <v>16</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E129" s="4">
         <v>2000</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G129" s="3"/>
       <c r="H129" s="5">
@@ -6153,7 +6160,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>15</v>
@@ -6162,13 +6169,13 @@
         <v>16</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E130" s="4">
         <v>2001</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G130" s="3"/>
       <c r="H130" s="5">
@@ -6187,7 +6194,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>15</v>
@@ -6196,13 +6203,13 @@
         <v>16</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E131" s="4">
         <v>2002</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G131" s="3"/>
       <c r="H131" s="5">
@@ -6221,7 +6228,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>15</v>
@@ -6230,13 +6237,13 @@
         <v>16</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E132" s="4">
         <v>2003</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G132" s="3"/>
       <c r="H132" s="5">
@@ -6255,7 +6262,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>15</v>
@@ -6264,13 +6271,13 @@
         <v>16</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E133" s="4">
         <v>2004</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G133" s="3"/>
       <c r="H133" s="5">
@@ -6289,7 +6296,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>15</v>
@@ -6298,13 +6305,13 @@
         <v>16</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E134" s="4">
         <v>2005</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G134" s="3"/>
       <c r="H134" s="5">
@@ -6323,7 +6330,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>15</v>
@@ -6332,13 +6339,13 @@
         <v>16</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E135" s="4">
         <v>2006</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G135" s="3"/>
       <c r="H135" s="5">
@@ -6357,7 +6364,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>15</v>
@@ -6366,13 +6373,13 @@
         <v>16</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E136" s="4">
         <v>2007</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G136" s="3"/>
       <c r="H136" s="5">
@@ -6391,7 +6398,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>15</v>
@@ -6400,13 +6407,13 @@
         <v>16</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E137" s="4">
         <v>2008</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G137" s="3"/>
       <c r="H137" s="5">
@@ -6425,7 +6432,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>15</v>
@@ -6434,13 +6441,13 @@
         <v>16</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E138" s="4">
         <v>2009</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G138" s="3"/>
       <c r="H138" s="5">
@@ -6459,7 +6466,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>15</v>
@@ -6468,13 +6475,13 @@
         <v>16</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E139" s="4">
         <v>2010</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="5">
@@ -6493,7 +6500,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>15</v>
@@ -6502,13 +6509,13 @@
         <v>16</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E140" s="4">
         <v>2011</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G140" s="3"/>
       <c r="H140" s="5">
@@ -6527,7 +6534,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>15</v>
@@ -6536,13 +6543,13 @@
         <v>16</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E141" s="4">
         <v>2012</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="5">
@@ -6561,7 +6568,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>15</v>
@@ -6570,13 +6577,13 @@
         <v>16</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E142" s="4">
         <v>2013</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G142" s="3"/>
       <c r="H142" s="5">
@@ -6595,7 +6602,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>15</v>
@@ -6604,13 +6611,13 @@
         <v>16</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E143" s="4">
         <v>2014</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G143" s="3"/>
       <c r="H143" s="5">
@@ -6629,7 +6636,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>15</v>
@@ -6638,13 +6645,13 @@
         <v>16</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E144" s="4">
         <v>2015</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G144" s="3"/>
       <c r="H144" s="5">
@@ -6663,7 +6670,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>15</v>
@@ -6672,13 +6679,13 @@
         <v>16</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E145" s="4">
         <v>2016</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G145" s="3"/>
       <c r="H145" s="5">
@@ -6697,7 +6704,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>15</v>
@@ -6706,13 +6713,13 @@
         <v>16</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E146" s="4">
         <v>2017</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G146" s="3"/>
       <c r="H146" s="5">
@@ -6731,7 +6738,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>15</v>
@@ -6740,13 +6747,13 @@
         <v>16</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E147" s="4">
         <v>2018</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G147" s="3"/>
       <c r="H147" s="5">
@@ -6765,7 +6772,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>15</v>
@@ -6774,13 +6781,13 @@
         <v>16</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E148" s="4">
         <v>2019</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G148" s="3"/>
       <c r="H148" s="5">
@@ -6799,7 +6806,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>15</v>
@@ -6808,13 +6815,13 @@
         <v>16</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E149" s="4">
         <v>2020</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G149" s="3"/>
       <c r="H149" s="5">
@@ -6833,7 +6840,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>15</v>
@@ -6842,13 +6849,13 @@
         <v>16</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E150" s="4">
         <v>2021</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G150" s="3"/>
       <c r="H150" s="5">
@@ -6867,7 +6874,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>15</v>
@@ -6876,13 +6883,13 @@
         <v>16</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E151" s="4">
         <v>2022</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G151" s="3"/>
       <c r="H151" s="5">
@@ -6901,7 +6908,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>15</v>
@@ -6910,13 +6917,13 @@
         <v>16</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E152" s="4">
         <v>2023</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G152" s="3"/>
       <c r="H152" s="5">
@@ -6935,7 +6942,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>15</v>
@@ -6944,13 +6951,13 @@
         <v>16</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E153" s="4">
         <v>2024</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G153" s="3"/>
       <c r="H153" s="5">
@@ -6969,7 +6976,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>15</v>
@@ -6978,13 +6985,13 @@
         <v>16</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E154" s="4">
         <v>2025</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G154" s="3"/>
       <c r="H154" s="5">
@@ -7003,7 +7010,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>15</v>
@@ -7014,8 +7021,8 @@
       <c r="D155" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E155" s="12" t="s">
-        <v>273</v>
+      <c r="E155" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>118</v>
@@ -7041,7 +7048,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>15</v>
@@ -7052,8 +7059,8 @@
       <c r="D156" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E156" s="12" t="s">
-        <v>273</v>
+      <c r="E156" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="F156" s="3" t="s">
         <v>118</v>
@@ -7079,7 +7086,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>15</v>
@@ -7088,10 +7095,10 @@
         <v>16</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E157" s="12" t="s">
-        <v>273</v>
+        <v>192</v>
+      </c>
+      <c r="E157" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="F157" s="3" t="s">
         <v>120</v>
@@ -7117,7 +7124,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>15</v>
@@ -7126,13 +7133,13 @@
         <v>16</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="E158" s="12" t="s">
-        <v>273</v>
+        <v>278</v>
+      </c>
+      <c r="E158" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G158" s="3" t="s">
         <v>80</v>
@@ -7155,22 +7162,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D159" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B159" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="E159" s="12" t="s">
-        <v>273</v>
+      <c r="E159" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G159" s="3" t="s">
         <v>80</v>
@@ -7193,7 +7200,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>15</v>
@@ -7202,13 +7209,13 @@
         <v>16</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E160" s="12" t="s">
-        <v>280</v>
+        <v>192</v>
+      </c>
+      <c r="E160" s="11" t="s">
+        <v>281</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G160" s="3" t="s">
         <v>80</v>
@@ -7231,7 +7238,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>15</v>
@@ -7242,8 +7249,8 @@
       <c r="D161" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E161" s="12" t="s">
-        <v>282</v>
+      <c r="E161" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="F161" s="3" t="s">
         <v>118</v>
@@ -7271,7 +7278,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>15</v>
@@ -7282,8 +7289,8 @@
       <c r="D162" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E162" s="12" t="s">
-        <v>282</v>
+      <c r="E162" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>118</v>
@@ -7311,7 +7318,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>15</v>
@@ -7320,10 +7327,10 @@
         <v>16</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E163" s="12" t="s">
-        <v>282</v>
+        <v>192</v>
+      </c>
+      <c r="E163" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="F163" s="3" t="s">
         <v>120</v>
@@ -7351,7 +7358,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>15</v>
@@ -7360,13 +7367,13 @@
         <v>16</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="E164" s="12" t="s">
         <v>287</v>
       </c>
+      <c r="E164" s="11" t="s">
+        <v>288</v>
+      </c>
       <c r="F164" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>80</v>
@@ -7391,7 +7398,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>15</v>
@@ -7400,13 +7407,13 @@
         <v>16</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E165" s="12" t="s">
-        <v>282</v>
+        <v>192</v>
+      </c>
+      <c r="E165" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>80</v>
@@ -7431,7 +7438,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>15</v>
@@ -7469,7 +7476,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>15</v>
@@ -7478,13 +7485,13 @@
         <v>16</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E167" s="4">
         <v>2020</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>80</v>
@@ -7507,7 +7514,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>15</v>
@@ -7522,7 +7529,7 @@
         <v>2020</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>80</v>
@@ -7545,7 +7552,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>15</v>
@@ -7554,7 +7561,7 @@
         <v>16</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E169" s="4">
         <v>2020</v>
@@ -7583,7 +7590,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>15</v>
@@ -7592,7 +7599,7 @@
         <v>16</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E170" s="4">
         <v>2020</v>
@@ -7621,7 +7628,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>15</v>
@@ -7630,13 +7637,13 @@
         <v>16</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E171" s="4">
         <v>2015</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G171" s="3"/>
       <c r="H171" s="5">
@@ -7654,12 +7661,12 @@
         <v>41</v>
       </c>
       <c r="N171" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>15</v>
@@ -7668,7 +7675,7 @@
         <v>16</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E172" s="4">
         <v>2023</v>
@@ -7691,13 +7698,13 @@
         <v>1</v>
       </c>
       <c r="M172" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N172" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>15</v>
@@ -7706,13 +7713,13 @@
         <v>16</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E173" s="4">
         <v>2023</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G173" s="3"/>
       <c r="H173" s="5">
@@ -7727,13 +7734,13 @@
         <v>1</v>
       </c>
       <c r="M173" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N173" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>15</v>
@@ -7748,7 +7755,7 @@
         <v>2023</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>80</v>
@@ -7765,13 +7772,13 @@
         <v>1</v>
       </c>
       <c r="M174" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N174" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>15</v>
@@ -7780,13 +7787,13 @@
         <v>16</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E175" s="4">
         <v>2023</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G175" s="3" t="s">
         <v>80</v>
@@ -7803,13 +7810,13 @@
         <v>1</v>
       </c>
       <c r="M175" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N175" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>15</v>
@@ -7824,7 +7831,7 @@
         <v>2023</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>80</v>
@@ -7841,13 +7848,13 @@
         <v>1</v>
       </c>
       <c r="M176" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N176" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
       <c r="A177" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>15</v>
@@ -7862,7 +7869,7 @@
         <v>2023</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>80</v>
@@ -7879,13 +7886,13 @@
         <v>1</v>
       </c>
       <c r="M177" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N177" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
       <c r="A178" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>15</v>
@@ -7894,13 +7901,13 @@
         <v>16</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>80</v>
@@ -7917,13 +7924,13 @@
         <v>1</v>
       </c>
       <c r="M178" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="N178" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
       <c r="A179" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>15</v>
@@ -7932,13 +7939,13 @@
         <v>16</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E179" s="4">
         <v>2015</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>80</v>
@@ -7955,15 +7962,15 @@
         <v>1</v>
       </c>
       <c r="M179" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N179" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>82</v>
@@ -7972,9 +7979,9 @@
         <v>77</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="E180" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="E180" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F180" s="3" t="s">
@@ -7983,11 +7990,11 @@
       <c r="G180" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H180" s="12"/>
+      <c r="H180" s="13"/>
       <c r="I180" s="3"/>
-      <c r="J180" s="12"/>
+      <c r="J180" s="13"/>
       <c r="K180" s="3"/>
-      <c r="L180" s="12"/>
+      <c r="L180" s="13"/>
       <c r="M180" s="3"/>
       <c r="N180" s="3" t="s">
         <v>100</v>
@@ -7995,16 +8002,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
       <c r="A181" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E181" s="4">
         <v>2020</v>
@@ -8015,28 +8022,28 @@
       <c r="G181" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H181" s="12"/>
+      <c r="H181" s="13"/>
       <c r="I181" s="3"/>
-      <c r="J181" s="12"/>
+      <c r="J181" s="13"/>
       <c r="K181" s="3"/>
-      <c r="L181" s="12"/>
+      <c r="L181" s="13"/>
       <c r="M181" s="3"/>
       <c r="N181" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
       <c r="A182" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E182" s="4">
         <v>2020</v>
@@ -8047,31 +8054,31 @@
       <c r="G182" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H182" s="12"/>
+      <c r="H182" s="13"/>
       <c r="I182" s="3"/>
-      <c r="J182" s="12"/>
+      <c r="J182" s="13"/>
       <c r="K182" s="3"/>
-      <c r="L182" s="12"/>
+      <c r="L182" s="13"/>
       <c r="M182" s="3"/>
       <c r="N182" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
       <c r="A183" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E183" s="12" t="s">
-        <v>273</v>
+        <v>332</v>
+      </c>
+      <c r="E183" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>79</v>
@@ -8079,31 +8086,31 @@
       <c r="G183" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H183" s="12"/>
+      <c r="H183" s="13"/>
       <c r="I183" s="3"/>
-      <c r="J183" s="12"/>
+      <c r="J183" s="13"/>
       <c r="K183" s="3"/>
-      <c r="L183" s="12"/>
+      <c r="L183" s="13"/>
       <c r="M183" s="3"/>
       <c r="N183" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
       <c r="A184" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E184" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
+      </c>
+      <c r="E184" s="11" t="s">
+        <v>334</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>79</v>
@@ -8111,28 +8118,28 @@
       <c r="G184" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H184" s="12"/>
+      <c r="H184" s="13"/>
       <c r="I184" s="3"/>
-      <c r="J184" s="12"/>
+      <c r="J184" s="13"/>
       <c r="K184" s="3"/>
-      <c r="L184" s="12"/>
+      <c r="L184" s="13"/>
       <c r="M184" s="3"/>
       <c r="N184" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
       <c r="A185" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E185" s="4">
         <v>2020</v>
@@ -8143,28 +8150,28 @@
       <c r="G185" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H185" s="12"/>
+      <c r="H185" s="13"/>
       <c r="I185" s="3"/>
-      <c r="J185" s="12"/>
+      <c r="J185" s="13"/>
       <c r="K185" s="3"/>
-      <c r="L185" s="12"/>
+      <c r="L185" s="13"/>
       <c r="M185" s="3"/>
       <c r="N185" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E186" s="4">
         <v>2020</v>
@@ -8175,28 +8182,28 @@
       <c r="G186" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H186" s="12"/>
+      <c r="H186" s="13"/>
       <c r="I186" s="3"/>
-      <c r="J186" s="12"/>
+      <c r="J186" s="13"/>
       <c r="K186" s="3"/>
-      <c r="L186" s="12"/>
+      <c r="L186" s="13"/>
       <c r="M186" s="3"/>
       <c r="N186" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E187" s="4">
         <v>2020</v>
@@ -8207,31 +8214,31 @@
       <c r="G187" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H187" s="12"/>
+      <c r="H187" s="13"/>
       <c r="I187" s="3"/>
-      <c r="J187" s="12"/>
+      <c r="J187" s="13"/>
       <c r="K187" s="3"/>
-      <c r="L187" s="12"/>
+      <c r="L187" s="13"/>
       <c r="M187" s="3"/>
       <c r="N187" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
       <c r="A188" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="E188" s="12" t="s">
-        <v>333</v>
+        <v>340</v>
+      </c>
+      <c r="E188" s="11" t="s">
+        <v>334</v>
       </c>
       <c r="F188" s="3" t="s">
         <v>79</v>
@@ -8239,31 +8246,31 @@
       <c r="G188" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H188" s="12"/>
+      <c r="H188" s="13"/>
       <c r="I188" s="3"/>
-      <c r="J188" s="12"/>
+      <c r="J188" s="13"/>
       <c r="K188" s="3"/>
-      <c r="L188" s="12"/>
+      <c r="L188" s="13"/>
       <c r="M188" s="3"/>
       <c r="N188" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
       <c r="A189" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E189" s="12" t="s">
-        <v>333</v>
+        <v>327</v>
+      </c>
+      <c r="E189" s="11" t="s">
+        <v>334</v>
       </c>
       <c r="F189" s="3" t="s">
         <v>79</v>
@@ -8271,31 +8278,31 @@
       <c r="G189" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H189" s="12"/>
+      <c r="H189" s="13"/>
       <c r="I189" s="3"/>
-      <c r="J189" s="12"/>
+      <c r="J189" s="13"/>
       <c r="K189" s="3"/>
-      <c r="L189" s="12"/>
+      <c r="L189" s="13"/>
       <c r="M189" s="3"/>
       <c r="N189" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E190" s="12" t="s">
-        <v>333</v>
+        <v>344</v>
+      </c>
+      <c r="E190" s="11" t="s">
+        <v>334</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>79</v>
@@ -8303,28 +8310,28 @@
       <c r="G190" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H190" s="12"/>
+      <c r="H190" s="13"/>
       <c r="I190" s="3"/>
-      <c r="J190" s="12"/>
+      <c r="J190" s="13"/>
       <c r="K190" s="3"/>
-      <c r="L190" s="12"/>
+      <c r="L190" s="13"/>
       <c r="M190" s="3"/>
       <c r="N190" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E191" s="4">
         <v>2015</v>
@@ -8335,30 +8342,30 @@
       <c r="G191" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H191" s="12"/>
+      <c r="H191" s="13"/>
       <c r="I191" s="3"/>
-      <c r="J191" s="12"/>
+      <c r="J191" s="13"/>
       <c r="K191" s="3"/>
-      <c r="L191" s="12"/>
+      <c r="L191" s="13"/>
       <c r="M191" s="3"/>
       <c r="N191" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E192" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="E192" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F192" s="3" t="s">
@@ -8367,30 +8374,30 @@
       <c r="G192" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H192" s="12"/>
+      <c r="H192" s="13"/>
       <c r="I192" s="3"/>
-      <c r="J192" s="12"/>
+      <c r="J192" s="13"/>
       <c r="K192" s="3"/>
-      <c r="L192" s="12"/>
+      <c r="L192" s="13"/>
       <c r="M192" s="3"/>
       <c r="N192" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
       <c r="A193" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E193" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E193" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F193" s="3" t="s">
@@ -8399,30 +8406,30 @@
       <c r="G193" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H193" s="12"/>
+      <c r="H193" s="13"/>
       <c r="I193" s="3"/>
-      <c r="J193" s="12"/>
+      <c r="J193" s="13"/>
       <c r="K193" s="3"/>
-      <c r="L193" s="12"/>
+      <c r="L193" s="13"/>
       <c r="M193" s="3"/>
       <c r="N193" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="15">
       <c r="A194" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="E194" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="E194" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F194" s="3" t="s">
@@ -8431,14 +8438,14 @@
       <c r="G194" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H194" s="12"/>
+      <c r="H194" s="13"/>
       <c r="I194" s="3"/>
-      <c r="J194" s="12"/>
+      <c r="J194" s="13"/>
       <c r="K194" s="3"/>
-      <c r="L194" s="12"/>
+      <c r="L194" s="13"/>
       <c r="M194" s="3"/>
       <c r="N194" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -8457,20 +8464,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -9050,7 +9057,7 @@
       <c r="D15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -9090,7 +9097,7 @@
       <c r="D16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -9130,7 +9137,7 @@
       <c r="D17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -9170,7 +9177,7 @@
       <c r="D18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F18" s="3" t="s">

</xml_diff>

<commit_message>
updated doc for dataset
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnell\Documents\GitHub\whisp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3CC688-2526-4953-8A57-48845E86BC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73BD1CF-3F80-4868-A3BF-967D1406E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="364">
   <si>
     <t>Column name</t>
   </si>
@@ -1104,6 +1104,15 @@
   </si>
   <si>
     <t>Processing info in dictionary format: whisp_version (python package release), processing_timestamp_utc (in ISO 8601 standard and set to UTC)</t>
+  </si>
+  <si>
+    <t>DIST_after_2020</t>
+  </si>
+  <si>
+    <t>2023-2026</t>
+  </si>
+  <si>
+    <t>Pickens 2025</t>
   </si>
 </sst>
 </file>
@@ -1520,11 +1529,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N195"/>
+  <dimension ref="A1:N196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7018,7 +7027,7 @@
     </row>
     <row r="166" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>292</v>
+        <v>361</v>
       </c>
       <c r="B166" t="s">
         <v>15</v>
@@ -7027,35 +7036,33 @@
         <v>16</v>
       </c>
       <c r="D166" t="s">
-        <v>24</v>
-      </c>
-      <c r="E166" s="3">
-        <v>2020</v>
+        <v>194</v>
+      </c>
+      <c r="E166" s="9" t="s">
+        <v>362</v>
       </c>
       <c r="F166" t="s">
-        <v>114</v>
-      </c>
-      <c r="G166" t="s">
-        <v>82</v>
+        <v>363</v>
       </c>
       <c r="H166" s="4">
-        <v>0</v>
-      </c>
-      <c r="I166" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J166" s="4">
-        <v>0</v>
-      </c>
-      <c r="K166" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K166" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L166" s="4">
-        <v>1</v>
-      </c>
-      <c r="M166" s="5" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B167" t="s">
         <v>15</v>
@@ -7064,13 +7071,13 @@
         <v>16</v>
       </c>
       <c r="D167" t="s">
-        <v>294</v>
+        <v>24</v>
       </c>
       <c r="E167" s="3">
         <v>2020</v>
       </c>
       <c r="F167" t="s">
-        <v>295</v>
+        <v>114</v>
       </c>
       <c r="G167" t="s">
         <v>82</v>
@@ -7092,7 +7099,7 @@
     </row>
     <row r="168" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B168" t="s">
         <v>15</v>
@@ -7101,13 +7108,13 @@
         <v>16</v>
       </c>
       <c r="D168" t="s">
-        <v>24</v>
+        <v>294</v>
       </c>
       <c r="E168" s="3">
         <v>2020</v>
       </c>
       <c r="F168" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G168" t="s">
         <v>82</v>
@@ -7129,7 +7136,7 @@
     </row>
     <row r="169" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B169" t="s">
         <v>15</v>
@@ -7138,13 +7145,13 @@
         <v>16</v>
       </c>
       <c r="D169" t="s">
-        <v>299</v>
+        <v>24</v>
       </c>
       <c r="E169" s="3">
         <v>2020</v>
       </c>
       <c r="F169" t="s">
-        <v>114</v>
+        <v>297</v>
       </c>
       <c r="G169" t="s">
         <v>82</v>
@@ -7161,12 +7168,12 @@
         <v>1</v>
       </c>
       <c r="M169" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="170" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B170" t="s">
         <v>15</v>
@@ -7175,7 +7182,7 @@
         <v>16</v>
       </c>
       <c r="D170" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E170" s="3">
         <v>2020</v>
@@ -7198,12 +7205,12 @@
         <v>1</v>
       </c>
       <c r="M170" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="171" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B171" t="s">
         <v>15</v>
@@ -7212,13 +7219,16 @@
         <v>16</v>
       </c>
       <c r="D171" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E171" s="3">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="F171" t="s">
-        <v>304</v>
+        <v>114</v>
+      </c>
+      <c r="G171" t="s">
+        <v>82</v>
       </c>
       <c r="H171" s="4">
         <v>0</v>
@@ -7234,13 +7244,10 @@
       <c r="M171" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N171" t="s">
-        <v>305</v>
-      </c>
     </row>
     <row r="172" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B172" t="s">
         <v>15</v>
@@ -7249,16 +7256,13 @@
         <v>16</v>
       </c>
       <c r="D172" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E172" s="3">
-        <v>2023</v>
+        <v>2015</v>
       </c>
       <c r="F172" t="s">
-        <v>120</v>
-      </c>
-      <c r="G172" t="s">
-        <v>82</v>
+        <v>304</v>
       </c>
       <c r="H172" s="4">
         <v>0</v>
@@ -7272,12 +7276,15 @@
         <v>1</v>
       </c>
       <c r="M172" s="5" t="s">
-        <v>308</v>
+        <v>41</v>
+      </c>
+      <c r="N172" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="173" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B173" t="s">
         <v>15</v>
@@ -7286,13 +7293,16 @@
         <v>16</v>
       </c>
       <c r="D173" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E173" s="3">
         <v>2023</v>
       </c>
       <c r="F173" t="s">
-        <v>311</v>
+        <v>120</v>
+      </c>
+      <c r="G173" t="s">
+        <v>82</v>
       </c>
       <c r="H173" s="4">
         <v>0</v>
@@ -7311,7 +7321,7 @@
     </row>
     <row r="174" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B174" t="s">
         <v>15</v>
@@ -7320,16 +7330,13 @@
         <v>16</v>
       </c>
       <c r="D174" t="s">
-        <v>62</v>
+        <v>310</v>
       </c>
       <c r="E174" s="3">
         <v>2023</v>
       </c>
       <c r="F174" t="s">
-        <v>126</v>
-      </c>
-      <c r="G174" t="s">
-        <v>82</v>
+        <v>311</v>
       </c>
       <c r="H174" s="4">
         <v>0</v>
@@ -7343,12 +7350,12 @@
         <v>1</v>
       </c>
       <c r="M174" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="175" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B175" t="s">
         <v>15</v>
@@ -7357,7 +7364,7 @@
         <v>16</v>
       </c>
       <c r="D175" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="E175" s="3">
         <v>2023</v>
@@ -7385,7 +7392,7 @@
     </row>
     <row r="176" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B176" t="s">
         <v>15</v>
@@ -7394,7 +7401,7 @@
         <v>16</v>
       </c>
       <c r="D176" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="E176" s="3">
         <v>2023</v>
@@ -7422,7 +7429,7 @@
     </row>
     <row r="177" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B177" t="s">
         <v>15</v>
@@ -7431,7 +7438,7 @@
         <v>16</v>
       </c>
       <c r="D177" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E177" s="3">
         <v>2023</v>
@@ -7459,7 +7466,7 @@
     </row>
     <row r="178" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B178" t="s">
         <v>15</v>
@@ -7468,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="D178" t="s">
-        <v>318</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>319</v>
+        <v>74</v>
+      </c>
+      <c r="E178" s="3">
+        <v>2023</v>
       </c>
       <c r="F178" t="s">
-        <v>311</v>
+        <v>126</v>
       </c>
       <c r="G178" t="s">
         <v>82</v>
@@ -7496,7 +7503,7 @@
     </row>
     <row r="179" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B179" t="s">
         <v>15</v>
@@ -7505,13 +7512,13 @@
         <v>16</v>
       </c>
       <c r="D179" t="s">
-        <v>321</v>
-      </c>
-      <c r="E179" s="3">
-        <v>2015</v>
+        <v>318</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>319</v>
       </c>
       <c r="F179" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="G179" t="s">
         <v>82</v>
@@ -7528,44 +7535,52 @@
         <v>1</v>
       </c>
       <c r="M179" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="N179" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="180" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B180" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C180" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="D180" t="s">
-        <v>326</v>
-      </c>
-      <c r="E180" s="9" t="s">
-        <v>79</v>
+        <v>321</v>
+      </c>
+      <c r="E180" s="3">
+        <v>2015</v>
       </c>
       <c r="F180" t="s">
-        <v>81</v>
+        <v>322</v>
       </c>
       <c r="G180" t="s">
         <v>82</v>
       </c>
-      <c r="H180" s="3"/>
-      <c r="J180" s="3"/>
-      <c r="L180" s="3"/>
+      <c r="H180" s="4">
+        <v>0</v>
+      </c>
+      <c r="I180" s="5"/>
+      <c r="J180" s="4">
+        <v>0</v>
+      </c>
+      <c r="K180" s="5"/>
+      <c r="L180" s="4">
+        <v>1</v>
+      </c>
+      <c r="M180" s="5" t="s">
+        <v>323</v>
+      </c>
       <c r="N180" t="s">
-        <v>102</v>
+        <v>324</v>
       </c>
     </row>
     <row r="181" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
       <c r="B181" t="s">
         <v>84</v>
@@ -7574,53 +7589,53 @@
         <v>79</v>
       </c>
       <c r="D181" t="s">
-        <v>360</v>
-      </c>
-      <c r="E181" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E181" s="9" t="s">
         <v>79</v>
       </c>
       <c r="F181" t="s">
         <v>81</v>
       </c>
-      <c r="H181" s="4"/>
-      <c r="I181" s="5"/>
-      <c r="J181" s="4"/>
-      <c r="K181" s="5"/>
-      <c r="L181" s="4"/>
-      <c r="M181" s="5"/>
+      <c r="G181" t="s">
+        <v>82</v>
+      </c>
+      <c r="H181" s="3"/>
+      <c r="J181" s="3"/>
+      <c r="L181" s="3"/>
+      <c r="N181" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="182" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c r="B182" t="s">
         <v>84</v>
       </c>
       <c r="C182" t="s">
-        <v>328</v>
+        <v>79</v>
       </c>
       <c r="D182" t="s">
-        <v>329</v>
-      </c>
-      <c r="E182" s="3">
-        <v>2020</v>
+        <v>360</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F182" t="s">
         <v>81</v>
       </c>
-      <c r="G182" t="s">
-        <v>82</v>
-      </c>
-      <c r="H182" s="3"/>
-      <c r="J182" s="3"/>
-      <c r="L182" s="3"/>
-      <c r="N182" t="s">
-        <v>330</v>
-      </c>
+      <c r="H182" s="4"/>
+      <c r="I182" s="5"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="5"/>
+      <c r="L182" s="4"/>
+      <c r="M182" s="5"/>
     </row>
     <row r="183" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B183" t="s">
         <v>84</v>
@@ -7629,7 +7644,7 @@
         <v>328</v>
       </c>
       <c r="D183" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E183" s="3">
         <v>2020</v>
@@ -7649,7 +7664,7 @@
     </row>
     <row r="184" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B184" t="s">
         <v>84</v>
@@ -7658,10 +7673,10 @@
         <v>328</v>
       </c>
       <c r="D184" t="s">
-        <v>334</v>
-      </c>
-      <c r="E184" s="9" t="s">
-        <v>276</v>
+        <v>332</v>
+      </c>
+      <c r="E184" s="3">
+        <v>2020</v>
       </c>
       <c r="F184" t="s">
         <v>81</v>
@@ -7678,7 +7693,7 @@
     </row>
     <row r="185" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B185" t="s">
         <v>84</v>
@@ -7690,7 +7705,7 @@
         <v>334</v>
       </c>
       <c r="E185" s="9" t="s">
-        <v>336</v>
+        <v>276</v>
       </c>
       <c r="F185" t="s">
         <v>81</v>
@@ -7707,7 +7722,7 @@
     </row>
     <row r="186" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B186" t="s">
         <v>84</v>
@@ -7716,10 +7731,10 @@
         <v>328</v>
       </c>
       <c r="D186" t="s">
-        <v>338</v>
-      </c>
-      <c r="E186" s="3">
-        <v>2020</v>
+        <v>334</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>336</v>
       </c>
       <c r="F186" t="s">
         <v>81</v>
@@ -7736,7 +7751,7 @@
     </row>
     <row r="187" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B187" t="s">
         <v>84</v>
@@ -7745,7 +7760,7 @@
         <v>328</v>
       </c>
       <c r="D187" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E187" s="3">
         <v>2020</v>
@@ -7765,7 +7780,7 @@
     </row>
     <row r="188" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B188" t="s">
         <v>84</v>
@@ -7774,7 +7789,7 @@
         <v>328</v>
       </c>
       <c r="D188" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E188" s="3">
         <v>2020</v>
@@ -7794,7 +7809,7 @@
     </row>
     <row r="189" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B189" t="s">
         <v>84</v>
@@ -7805,8 +7820,8 @@
       <c r="D189" t="s">
         <v>342</v>
       </c>
-      <c r="E189" s="9" t="s">
-        <v>336</v>
+      <c r="E189" s="3">
+        <v>2020</v>
       </c>
       <c r="F189" t="s">
         <v>81</v>
@@ -7823,7 +7838,7 @@
     </row>
     <row r="190" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B190" t="s">
         <v>84</v>
@@ -7832,7 +7847,7 @@
         <v>328</v>
       </c>
       <c r="D190" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="E190" s="9" t="s">
         <v>336</v>
@@ -7852,7 +7867,7 @@
     </row>
     <row r="191" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B191" t="s">
         <v>84</v>
@@ -7861,7 +7876,7 @@
         <v>328</v>
       </c>
       <c r="D191" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="E191" s="9" t="s">
         <v>336</v>
@@ -7881,7 +7896,7 @@
     </row>
     <row r="192" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B192" t="s">
         <v>84</v>
@@ -7890,10 +7905,10 @@
         <v>328</v>
       </c>
       <c r="D192" t="s">
-        <v>348</v>
-      </c>
-      <c r="E192" s="3">
-        <v>2015</v>
+        <v>346</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>336</v>
       </c>
       <c r="F192" t="s">
         <v>81</v>
@@ -7910,19 +7925,19 @@
     </row>
     <row r="193" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B193" t="s">
         <v>84</v>
       </c>
       <c r="C193" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D193" t="s">
-        <v>351</v>
-      </c>
-      <c r="E193" s="9" t="s">
-        <v>79</v>
+        <v>348</v>
+      </c>
+      <c r="E193" s="3">
+        <v>2015</v>
       </c>
       <c r="F193" t="s">
         <v>81</v>
@@ -7934,12 +7949,12 @@
       <c r="J193" s="3"/>
       <c r="L193" s="3"/>
       <c r="N193" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
     </row>
     <row r="194" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B194" t="s">
         <v>84</v>
@@ -7948,7 +7963,7 @@
         <v>350</v>
       </c>
       <c r="D194" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E194" s="9" t="s">
         <v>79</v>
@@ -7963,12 +7978,12 @@
       <c r="J194" s="3"/>
       <c r="L194" s="3"/>
       <c r="N194" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="195" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B195" t="s">
         <v>84</v>
@@ -7977,7 +7992,7 @@
         <v>350</v>
       </c>
       <c r="D195" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E195" s="9" t="s">
         <v>79</v>
@@ -7992,6 +8007,35 @@
       <c r="J195" s="3"/>
       <c r="L195" s="3"/>
       <c r="N195" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>356</v>
+      </c>
+      <c r="B196" t="s">
+        <v>84</v>
+      </c>
+      <c r="C196" t="s">
+        <v>350</v>
+      </c>
+      <c r="D196" t="s">
+        <v>357</v>
+      </c>
+      <c r="E196" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F196" t="s">
+        <v>81</v>
+      </c>
+      <c r="G196" t="s">
+        <v>82</v>
+      </c>
+      <c r="H196" s="3"/>
+      <c r="J196" s="3"/>
+      <c r="L196" s="3"/>
+      <c r="N196" t="s">
         <v>358</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added in GLAD Landsat (GLAD-L) alerts for after 2020 combined, and each annual time step; added in annual timesteps for DIST alerts for 2024-2026
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnell\Documents\GitHub\whisp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73BD1CF-3F80-4868-A3BF-967D1406E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2483E82-E14A-4683-A9FE-C0501ACEAFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="376">
   <si>
     <t>Column name</t>
   </si>
@@ -1109,17 +1109,53 @@
     <t>DIST_after_2020</t>
   </si>
   <si>
-    <t>2023-2026</t>
-  </si>
-  <si>
     <t>Pickens 2025</t>
+  </si>
+  <si>
+    <t>2024-2026</t>
+  </si>
+  <si>
+    <t>DIST_year_2024</t>
+  </si>
+  <si>
+    <t>DIST_year_2025</t>
+  </si>
+  <si>
+    <t>DIST_year_2026</t>
+  </si>
+  <si>
+    <t>GLAD-L_year_2001</t>
+  </si>
+  <si>
+    <t>GLAD-L_year_2002</t>
+  </si>
+  <si>
+    <t>GLAD-L_year_2003</t>
+  </si>
+  <si>
+    <t>GLAD-L_year_2004</t>
+  </si>
+  <si>
+    <t>GLAD-L_year_2005</t>
+  </si>
+  <si>
+    <t>GLAD-L_year_2006</t>
+  </si>
+  <si>
+    <t>Hansen 2016</t>
+  </si>
+  <si>
+    <t>GLAD-L_after_2020</t>
+  </si>
+  <si>
+    <t>2021-2026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1137,6 +1173,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1192,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1224,6 +1272,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1529,11 +1578,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N196"/>
+  <dimension ref="A1:N206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5195,7 +5244,7 @@
     </row>
     <row r="109" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>226</v>
+        <v>364</v>
       </c>
       <c r="B109" t="s">
         <v>15</v>
@@ -5204,13 +5253,13 @@
         <v>16</v>
       </c>
       <c r="D109" t="s">
-        <v>227</v>
-      </c>
-      <c r="E109" s="3">
-        <v>2001</v>
+        <v>194</v>
+      </c>
+      <c r="E109" s="9">
+        <v>2024</v>
       </c>
       <c r="F109" t="s">
-        <v>228</v>
+        <v>362</v>
       </c>
       <c r="H109" s="4">
         <v>0</v>
@@ -5226,7 +5275,7 @@
     </row>
     <row r="110" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>229</v>
+        <v>365</v>
       </c>
       <c r="B110" t="s">
         <v>15</v>
@@ -5235,13 +5284,13 @@
         <v>16</v>
       </c>
       <c r="D110" t="s">
-        <v>227</v>
-      </c>
-      <c r="E110" s="3">
-        <v>2002</v>
+        <v>194</v>
+      </c>
+      <c r="E110" s="9">
+        <v>2025</v>
       </c>
       <c r="F110" t="s">
-        <v>228</v>
+        <v>362</v>
       </c>
       <c r="H110" s="4">
         <v>0</v>
@@ -5257,7 +5306,7 @@
     </row>
     <row r="111" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>230</v>
+        <v>366</v>
       </c>
       <c r="B111" t="s">
         <v>15</v>
@@ -5266,13 +5315,13 @@
         <v>16</v>
       </c>
       <c r="D111" t="s">
-        <v>227</v>
-      </c>
-      <c r="E111" s="3">
-        <v>2003</v>
+        <v>194</v>
+      </c>
+      <c r="E111" s="9">
+        <v>2026</v>
       </c>
       <c r="F111" t="s">
-        <v>228</v>
+        <v>362</v>
       </c>
       <c r="H111" s="4">
         <v>0</v>
@@ -5288,7 +5337,7 @@
     </row>
     <row r="112" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>231</v>
+        <v>367</v>
       </c>
       <c r="B112" t="s">
         <v>15</v>
@@ -5297,14 +5346,15 @@
         <v>16</v>
       </c>
       <c r="D112" t="s">
-        <v>227</v>
-      </c>
-      <c r="E112" s="3">
-        <v>2004</v>
+        <v>194</v>
+      </c>
+      <c r="E112" s="9">
+        <v>2021</v>
       </c>
       <c r="F112" t="s">
-        <v>228</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="G112" s="11"/>
       <c r="H112" s="4">
         <v>0</v>
       </c>
@@ -5319,7 +5369,7 @@
     </row>
     <row r="113" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>232</v>
+        <v>368</v>
       </c>
       <c r="B113" t="s">
         <v>15</v>
@@ -5328,13 +5378,13 @@
         <v>16</v>
       </c>
       <c r="D113" t="s">
-        <v>227</v>
-      </c>
-      <c r="E113" s="3">
-        <v>2005</v>
+        <v>194</v>
+      </c>
+      <c r="E113" s="9">
+        <v>2022</v>
       </c>
       <c r="F113" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="H113" s="4">
         <v>0</v>
@@ -5350,7 +5400,7 @@
     </row>
     <row r="114" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>233</v>
+        <v>369</v>
       </c>
       <c r="B114" t="s">
         <v>15</v>
@@ -5359,13 +5409,13 @@
         <v>16</v>
       </c>
       <c r="D114" t="s">
-        <v>227</v>
-      </c>
-      <c r="E114" s="3">
-        <v>2006</v>
+        <v>194</v>
+      </c>
+      <c r="E114" s="9">
+        <v>2023</v>
       </c>
       <c r="F114" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="H114" s="4">
         <v>0</v>
@@ -5381,7 +5431,7 @@
     </row>
     <row r="115" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>234</v>
+        <v>370</v>
       </c>
       <c r="B115" t="s">
         <v>15</v>
@@ -5390,13 +5440,13 @@
         <v>16</v>
       </c>
       <c r="D115" t="s">
-        <v>227</v>
-      </c>
-      <c r="E115" s="3">
-        <v>2007</v>
+        <v>194</v>
+      </c>
+      <c r="E115" s="9">
+        <v>2024</v>
       </c>
       <c r="F115" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="H115" s="4">
         <v>0</v>
@@ -5412,7 +5462,7 @@
     </row>
     <row r="116" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>235</v>
+        <v>371</v>
       </c>
       <c r="B116" t="s">
         <v>15</v>
@@ -5421,13 +5471,13 @@
         <v>16</v>
       </c>
       <c r="D116" t="s">
-        <v>227</v>
-      </c>
-      <c r="E116" s="3">
-        <v>2008</v>
+        <v>194</v>
+      </c>
+      <c r="E116" s="9">
+        <v>2025</v>
       </c>
       <c r="F116" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="H116" s="4">
         <v>0</v>
@@ -5443,7 +5493,7 @@
     </row>
     <row r="117" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>236</v>
+        <v>372</v>
       </c>
       <c r="B117" t="s">
         <v>15</v>
@@ -5452,13 +5502,13 @@
         <v>16</v>
       </c>
       <c r="D117" t="s">
-        <v>227</v>
-      </c>
-      <c r="E117" s="3">
-        <v>2009</v>
+        <v>194</v>
+      </c>
+      <c r="E117" s="9">
+        <v>2026</v>
       </c>
       <c r="F117" t="s">
-        <v>228</v>
+        <v>373</v>
       </c>
       <c r="H117" s="4">
         <v>0</v>
@@ -5474,7 +5524,7 @@
     </row>
     <row r="118" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B118" t="s">
         <v>15</v>
@@ -5486,7 +5536,7 @@
         <v>227</v>
       </c>
       <c r="E118" s="3">
-        <v>2010</v>
+        <v>2001</v>
       </c>
       <c r="F118" t="s">
         <v>228</v>
@@ -5505,7 +5555,7 @@
     </row>
     <row r="119" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B119" t="s">
         <v>15</v>
@@ -5517,7 +5567,7 @@
         <v>227</v>
       </c>
       <c r="E119" s="3">
-        <v>2011</v>
+        <v>2002</v>
       </c>
       <c r="F119" t="s">
         <v>228</v>
@@ -5536,7 +5586,7 @@
     </row>
     <row r="120" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B120" t="s">
         <v>15</v>
@@ -5548,7 +5598,7 @@
         <v>227</v>
       </c>
       <c r="E120" s="3">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="F120" t="s">
         <v>228</v>
@@ -5567,7 +5617,7 @@
     </row>
     <row r="121" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B121" t="s">
         <v>15</v>
@@ -5579,7 +5629,7 @@
         <v>227</v>
       </c>
       <c r="E121" s="3">
-        <v>2013</v>
+        <v>2004</v>
       </c>
       <c r="F121" t="s">
         <v>228</v>
@@ -5598,7 +5648,7 @@
     </row>
     <row r="122" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B122" t="s">
         <v>15</v>
@@ -5610,7 +5660,7 @@
         <v>227</v>
       </c>
       <c r="E122" s="3">
-        <v>2014</v>
+        <v>2005</v>
       </c>
       <c r="F122" t="s">
         <v>228</v>
@@ -5629,7 +5679,7 @@
     </row>
     <row r="123" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B123" t="s">
         <v>15</v>
@@ -5641,7 +5691,7 @@
         <v>227</v>
       </c>
       <c r="E123" s="3">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="F123" t="s">
         <v>228</v>
@@ -5660,7 +5710,7 @@
     </row>
     <row r="124" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B124" t="s">
         <v>15</v>
@@ -5672,7 +5722,7 @@
         <v>227</v>
       </c>
       <c r="E124" s="3">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="F124" t="s">
         <v>228</v>
@@ -5691,7 +5741,7 @@
     </row>
     <row r="125" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B125" t="s">
         <v>15</v>
@@ -5703,7 +5753,7 @@
         <v>227</v>
       </c>
       <c r="E125" s="3">
-        <v>2017</v>
+        <v>2008</v>
       </c>
       <c r="F125" t="s">
         <v>228</v>
@@ -5722,7 +5772,7 @@
     </row>
     <row r="126" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B126" t="s">
         <v>15</v>
@@ -5734,7 +5784,7 @@
         <v>227</v>
       </c>
       <c r="E126" s="3">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="F126" t="s">
         <v>228</v>
@@ -5753,7 +5803,7 @@
     </row>
     <row r="127" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B127" t="s">
         <v>15</v>
@@ -5765,7 +5815,7 @@
         <v>227</v>
       </c>
       <c r="E127" s="3">
-        <v>2019</v>
+        <v>2010</v>
       </c>
       <c r="F127" t="s">
         <v>228</v>
@@ -5784,7 +5834,7 @@
     </row>
     <row r="128" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B128" t="s">
         <v>15</v>
@@ -5796,7 +5846,7 @@
         <v>227</v>
       </c>
       <c r="E128" s="3">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="F128" t="s">
         <v>228</v>
@@ -5815,7 +5865,7 @@
     </row>
     <row r="129" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B129" t="s">
         <v>15</v>
@@ -5827,10 +5877,10 @@
         <v>227</v>
       </c>
       <c r="E129" s="3">
-        <v>2000</v>
+        <v>2012</v>
       </c>
       <c r="F129" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H129" s="4">
         <v>0</v>
@@ -5846,7 +5896,7 @@
     </row>
     <row r="130" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B130" t="s">
         <v>15</v>
@@ -5858,10 +5908,10 @@
         <v>227</v>
       </c>
       <c r="E130" s="3">
-        <v>2001</v>
+        <v>2013</v>
       </c>
       <c r="F130" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H130" s="4">
         <v>0</v>
@@ -5877,7 +5927,7 @@
     </row>
     <row r="131" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B131" t="s">
         <v>15</v>
@@ -5889,10 +5939,10 @@
         <v>227</v>
       </c>
       <c r="E131" s="3">
-        <v>2002</v>
+        <v>2014</v>
       </c>
       <c r="F131" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H131" s="4">
         <v>0</v>
@@ -5908,7 +5958,7 @@
     </row>
     <row r="132" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B132" t="s">
         <v>15</v>
@@ -5920,10 +5970,10 @@
         <v>227</v>
       </c>
       <c r="E132" s="3">
-        <v>2003</v>
+        <v>2015</v>
       </c>
       <c r="F132" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H132" s="4">
         <v>0</v>
@@ -5939,7 +5989,7 @@
     </row>
     <row r="133" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B133" t="s">
         <v>15</v>
@@ -5951,10 +6001,10 @@
         <v>227</v>
       </c>
       <c r="E133" s="3">
-        <v>2004</v>
+        <v>2016</v>
       </c>
       <c r="F133" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H133" s="4">
         <v>0</v>
@@ -5970,7 +6020,7 @@
     </row>
     <row r="134" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B134" t="s">
         <v>15</v>
@@ -5982,10 +6032,10 @@
         <v>227</v>
       </c>
       <c r="E134" s="3">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="F134" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H134" s="4">
         <v>0</v>
@@ -6001,7 +6051,7 @@
     </row>
     <row r="135" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B135" t="s">
         <v>15</v>
@@ -6013,10 +6063,10 @@
         <v>227</v>
       </c>
       <c r="E135" s="3">
-        <v>2006</v>
+        <v>2018</v>
       </c>
       <c r="F135" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H135" s="4">
         <v>0</v>
@@ -6032,7 +6082,7 @@
     </row>
     <row r="136" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B136" t="s">
         <v>15</v>
@@ -6044,10 +6094,10 @@
         <v>227</v>
       </c>
       <c r="E136" s="3">
-        <v>2007</v>
+        <v>2019</v>
       </c>
       <c r="F136" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H136" s="4">
         <v>0</v>
@@ -6063,7 +6113,7 @@
     </row>
     <row r="137" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B137" t="s">
         <v>15</v>
@@ -6075,10 +6125,10 @@
         <v>227</v>
       </c>
       <c r="E137" s="3">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="F137" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="H137" s="4">
         <v>0</v>
@@ -6094,7 +6144,7 @@
     </row>
     <row r="138" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B138" t="s">
         <v>15</v>
@@ -6106,7 +6156,7 @@
         <v>227</v>
       </c>
       <c r="E138" s="3">
-        <v>2009</v>
+        <v>2000</v>
       </c>
       <c r="F138" t="s">
         <v>249</v>
@@ -6125,7 +6175,7 @@
     </row>
     <row r="139" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B139" t="s">
         <v>15</v>
@@ -6137,7 +6187,7 @@
         <v>227</v>
       </c>
       <c r="E139" s="3">
-        <v>2010</v>
+        <v>2001</v>
       </c>
       <c r="F139" t="s">
         <v>249</v>
@@ -6156,7 +6206,7 @@
     </row>
     <row r="140" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B140" t="s">
         <v>15</v>
@@ -6168,7 +6218,7 @@
         <v>227</v>
       </c>
       <c r="E140" s="3">
-        <v>2011</v>
+        <v>2002</v>
       </c>
       <c r="F140" t="s">
         <v>249</v>
@@ -6187,7 +6237,7 @@
     </row>
     <row r="141" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B141" t="s">
         <v>15</v>
@@ -6199,7 +6249,7 @@
         <v>227</v>
       </c>
       <c r="E141" s="3">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="F141" t="s">
         <v>249</v>
@@ -6218,7 +6268,7 @@
     </row>
     <row r="142" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B142" t="s">
         <v>15</v>
@@ -6230,7 +6280,7 @@
         <v>227</v>
       </c>
       <c r="E142" s="3">
-        <v>2013</v>
+        <v>2004</v>
       </c>
       <c r="F142" t="s">
         <v>249</v>
@@ -6249,7 +6299,7 @@
     </row>
     <row r="143" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B143" t="s">
         <v>15</v>
@@ -6261,7 +6311,7 @@
         <v>227</v>
       </c>
       <c r="E143" s="3">
-        <v>2014</v>
+        <v>2005</v>
       </c>
       <c r="F143" t="s">
         <v>249</v>
@@ -6280,7 +6330,7 @@
     </row>
     <row r="144" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B144" t="s">
         <v>15</v>
@@ -6292,7 +6342,7 @@
         <v>227</v>
       </c>
       <c r="E144" s="3">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="F144" t="s">
         <v>249</v>
@@ -6311,7 +6361,7 @@
     </row>
     <row r="145" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B145" t="s">
         <v>15</v>
@@ -6323,7 +6373,7 @@
         <v>227</v>
       </c>
       <c r="E145" s="3">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="F145" t="s">
         <v>249</v>
@@ -6342,7 +6392,7 @@
     </row>
     <row r="146" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B146" t="s">
         <v>15</v>
@@ -6354,7 +6404,7 @@
         <v>227</v>
       </c>
       <c r="E146" s="3">
-        <v>2017</v>
+        <v>2008</v>
       </c>
       <c r="F146" t="s">
         <v>249</v>
@@ -6373,7 +6423,7 @@
     </row>
     <row r="147" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B147" t="s">
         <v>15</v>
@@ -6385,7 +6435,7 @@
         <v>227</v>
       </c>
       <c r="E147" s="3">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="F147" t="s">
         <v>249</v>
@@ -6404,7 +6454,7 @@
     </row>
     <row r="148" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B148" t="s">
         <v>15</v>
@@ -6416,7 +6466,7 @@
         <v>227</v>
       </c>
       <c r="E148" s="3">
-        <v>2019</v>
+        <v>2010</v>
       </c>
       <c r="F148" t="s">
         <v>249</v>
@@ -6435,7 +6485,7 @@
     </row>
     <row r="149" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B149" t="s">
         <v>15</v>
@@ -6447,7 +6497,7 @@
         <v>227</v>
       </c>
       <c r="E149" s="3">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="F149" t="s">
         <v>249</v>
@@ -6466,7 +6516,7 @@
     </row>
     <row r="150" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B150" t="s">
         <v>15</v>
@@ -6478,7 +6528,7 @@
         <v>227</v>
       </c>
       <c r="E150" s="3">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="F150" t="s">
         <v>249</v>
@@ -6497,7 +6547,7 @@
     </row>
     <row r="151" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B151" t="s">
         <v>15</v>
@@ -6509,7 +6559,7 @@
         <v>227</v>
       </c>
       <c r="E151" s="3">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="F151" t="s">
         <v>249</v>
@@ -6528,7 +6578,7 @@
     </row>
     <row r="152" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B152" t="s">
         <v>15</v>
@@ -6540,7 +6590,7 @@
         <v>227</v>
       </c>
       <c r="E152" s="3">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="F152" t="s">
         <v>249</v>
@@ -6559,7 +6609,7 @@
     </row>
     <row r="153" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B153" t="s">
         <v>15</v>
@@ -6571,7 +6621,7 @@
         <v>227</v>
       </c>
       <c r="E153" s="3">
-        <v>2024</v>
+        <v>2015</v>
       </c>
       <c r="F153" t="s">
         <v>249</v>
@@ -6590,7 +6640,7 @@
     </row>
     <row r="154" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B154" t="s">
         <v>15</v>
@@ -6602,7 +6652,7 @@
         <v>227</v>
       </c>
       <c r="E154" s="3">
-        <v>2025</v>
+        <v>2016</v>
       </c>
       <c r="F154" t="s">
         <v>249</v>
@@ -6621,7 +6671,7 @@
     </row>
     <row r="155" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B155" t="s">
         <v>15</v>
@@ -6630,23 +6680,18 @@
         <v>16</v>
       </c>
       <c r="D155" t="s">
-        <v>50</v>
-      </c>
-      <c r="E155" s="9" t="s">
-        <v>276</v>
+        <v>227</v>
+      </c>
+      <c r="E155" s="3">
+        <v>2017</v>
       </c>
       <c r="F155" t="s">
-        <v>120</v>
-      </c>
-      <c r="G155" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="H155" s="4">
-        <v>1</v>
-      </c>
-      <c r="I155" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I155" s="5"/>
       <c r="J155" s="4">
         <v>0</v>
       </c>
@@ -6657,7 +6702,7 @@
     </row>
     <row r="156" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B156" t="s">
         <v>15</v>
@@ -6666,23 +6711,18 @@
         <v>16</v>
       </c>
       <c r="D156" t="s">
-        <v>46</v>
-      </c>
-      <c r="E156" s="9" t="s">
-        <v>276</v>
+        <v>227</v>
+      </c>
+      <c r="E156" s="3">
+        <v>2018</v>
       </c>
       <c r="F156" t="s">
-        <v>120</v>
-      </c>
-      <c r="G156" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="H156" s="4">
-        <v>1</v>
-      </c>
-      <c r="I156" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I156" s="5"/>
       <c r="J156" s="4">
         <v>0</v>
       </c>
@@ -6693,7 +6733,7 @@
     </row>
     <row r="157" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B157" t="s">
         <v>15</v>
@@ -6702,23 +6742,18 @@
         <v>16</v>
       </c>
       <c r="D157" t="s">
-        <v>194</v>
-      </c>
-      <c r="E157" s="9" t="s">
-        <v>276</v>
+        <v>227</v>
+      </c>
+      <c r="E157" s="3">
+        <v>2019</v>
       </c>
       <c r="F157" t="s">
-        <v>122</v>
-      </c>
-      <c r="G157" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="H157" s="4">
-        <v>1</v>
-      </c>
-      <c r="I157" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I157" s="5"/>
       <c r="J157" s="4">
         <v>0</v>
       </c>
@@ -6729,7 +6764,7 @@
     </row>
     <row r="158" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B158" t="s">
         <v>15</v>
@@ -6738,23 +6773,18 @@
         <v>16</v>
       </c>
       <c r="D158" t="s">
-        <v>280</v>
-      </c>
-      <c r="E158" s="9" t="s">
-        <v>276</v>
+        <v>227</v>
+      </c>
+      <c r="E158" s="3">
+        <v>2020</v>
       </c>
       <c r="F158" t="s">
-        <v>228</v>
-      </c>
-      <c r="G158" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="H158" s="4">
-        <v>1</v>
-      </c>
-      <c r="I158" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I158" s="5"/>
       <c r="J158" s="4">
         <v>0</v>
       </c>
@@ -6765,7 +6795,7 @@
     </row>
     <row r="159" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B159" t="s">
         <v>15</v>
@@ -6774,23 +6804,18 @@
         <v>16</v>
       </c>
       <c r="D159" t="s">
-        <v>280</v>
-      </c>
-      <c r="E159" s="9" t="s">
-        <v>276</v>
+        <v>227</v>
+      </c>
+      <c r="E159" s="3">
+        <v>2021</v>
       </c>
       <c r="F159" t="s">
         <v>249</v>
       </c>
-      <c r="G159" t="s">
-        <v>82</v>
-      </c>
       <c r="H159" s="4">
-        <v>1</v>
-      </c>
-      <c r="I159" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I159" s="5"/>
       <c r="J159" s="4">
         <v>0</v>
       </c>
@@ -6801,7 +6826,7 @@
     </row>
     <row r="160" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B160" t="s">
         <v>15</v>
@@ -6810,23 +6835,18 @@
         <v>16</v>
       </c>
       <c r="D160" t="s">
-        <v>194</v>
-      </c>
-      <c r="E160" s="9" t="s">
-        <v>283</v>
+        <v>227</v>
+      </c>
+      <c r="E160" s="3">
+        <v>2022</v>
       </c>
       <c r="F160" t="s">
-        <v>219</v>
-      </c>
-      <c r="G160" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="H160" s="4">
-        <v>1</v>
-      </c>
-      <c r="I160" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I160" s="5"/>
       <c r="J160" s="4">
         <v>0</v>
       </c>
@@ -6835,9 +6855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B161" t="s">
         <v>15</v>
@@ -6846,127 +6866,106 @@
         <v>16</v>
       </c>
       <c r="D161" t="s">
+        <v>227</v>
+      </c>
+      <c r="E161" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F161" t="s">
+        <v>249</v>
+      </c>
+      <c r="H161" s="4">
+        <v>0</v>
+      </c>
+      <c r="I161" s="5"/>
+      <c r="J161" s="4">
+        <v>0</v>
+      </c>
+      <c r="K161" s="5"/>
+      <c r="L161" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>273</v>
+      </c>
+      <c r="B162" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" t="s">
+        <v>16</v>
+      </c>
+      <c r="D162" t="s">
+        <v>227</v>
+      </c>
+      <c r="E162" s="3">
+        <v>2024</v>
+      </c>
+      <c r="F162" t="s">
+        <v>249</v>
+      </c>
+      <c r="H162" s="4">
+        <v>0</v>
+      </c>
+      <c r="I162" s="5"/>
+      <c r="J162" s="4">
+        <v>0</v>
+      </c>
+      <c r="K162" s="5"/>
+      <c r="L162" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>274</v>
+      </c>
+      <c r="B163" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" t="s">
+        <v>16</v>
+      </c>
+      <c r="D163" t="s">
+        <v>227</v>
+      </c>
+      <c r="E163" s="3">
+        <v>2025</v>
+      </c>
+      <c r="F163" t="s">
+        <v>249</v>
+      </c>
+      <c r="H163" s="4">
+        <v>0</v>
+      </c>
+      <c r="I163" s="5"/>
+      <c r="J163" s="4">
+        <v>0</v>
+      </c>
+      <c r="K163" s="5"/>
+      <c r="L163" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>275</v>
+      </c>
+      <c r="B164" t="s">
+        <v>15</v>
+      </c>
+      <c r="C164" t="s">
+        <v>16</v>
+      </c>
+      <c r="D164" t="s">
         <v>50</v>
       </c>
-      <c r="E161" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="F161" t="s">
+      <c r="E164" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="F164" t="s">
         <v>120</v>
-      </c>
-      <c r="G161" t="s">
-        <v>82</v>
-      </c>
-      <c r="H161" s="4">
-        <v>1</v>
-      </c>
-      <c r="I161" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J161" s="4">
-        <v>1</v>
-      </c>
-      <c r="K161" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L161" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
-        <v>286</v>
-      </c>
-      <c r="B162" t="s">
-        <v>15</v>
-      </c>
-      <c r="C162" t="s">
-        <v>16</v>
-      </c>
-      <c r="D162" t="s">
-        <v>46</v>
-      </c>
-      <c r="E162" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="F162" t="s">
-        <v>120</v>
-      </c>
-      <c r="G162" t="s">
-        <v>82</v>
-      </c>
-      <c r="H162" s="4">
-        <v>1</v>
-      </c>
-      <c r="I162" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J162" s="4">
-        <v>1</v>
-      </c>
-      <c r="K162" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L162" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
-        <v>287</v>
-      </c>
-      <c r="B163" t="s">
-        <v>15</v>
-      </c>
-      <c r="C163" t="s">
-        <v>16</v>
-      </c>
-      <c r="D163" t="s">
-        <v>194</v>
-      </c>
-      <c r="E163" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="F163" t="s">
-        <v>122</v>
-      </c>
-      <c r="G163" t="s">
-        <v>82</v>
-      </c>
-      <c r="H163" s="4">
-        <v>1</v>
-      </c>
-      <c r="I163" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J163" s="4">
-        <v>1</v>
-      </c>
-      <c r="K163" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L163" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
-        <v>288</v>
-      </c>
-      <c r="B164" t="s">
-        <v>15</v>
-      </c>
-      <c r="C164" t="s">
-        <v>16</v>
-      </c>
-      <c r="D164" t="s">
-        <v>289</v>
-      </c>
-      <c r="E164" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="F164" t="s">
-        <v>228</v>
       </c>
       <c r="G164" t="s">
         <v>82</v>
@@ -6975,21 +6974,19 @@
         <v>1</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J164" s="4">
-        <v>1</v>
-      </c>
-      <c r="K164" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K164" s="5"/>
       <c r="L164" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B165" t="s">
         <v>15</v>
@@ -6998,13 +6995,13 @@
         <v>16</v>
       </c>
       <c r="D165" t="s">
-        <v>194</v>
+        <v>46</v>
       </c>
       <c r="E165" s="9" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="F165" t="s">
-        <v>249</v>
+        <v>120</v>
       </c>
       <c r="G165" t="s">
         <v>82</v>
@@ -7013,21 +7010,19 @@
         <v>1</v>
       </c>
       <c r="I165" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J165" s="4">
-        <v>1</v>
-      </c>
-      <c r="K165" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K165" s="5"/>
       <c r="L165" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>361</v>
+        <v>278</v>
       </c>
       <c r="B166" t="s">
         <v>15</v>
@@ -7039,30 +7034,31 @@
         <v>194</v>
       </c>
       <c r="E166" s="9" t="s">
-        <v>362</v>
+        <v>276</v>
       </c>
       <c r="F166" t="s">
-        <v>363</v>
+        <v>122</v>
+      </c>
+      <c r="G166" t="s">
+        <v>82</v>
       </c>
       <c r="H166" s="4">
         <v>1</v>
       </c>
       <c r="I166" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J166" s="4">
-        <v>1</v>
-      </c>
-      <c r="K166" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K166" s="5"/>
       <c r="L166" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B167" t="s">
         <v>15</v>
@@ -7071,35 +7067,34 @@
         <v>16</v>
       </c>
       <c r="D167" t="s">
-        <v>24</v>
-      </c>
-      <c r="E167" s="3">
-        <v>2020</v>
+        <v>280</v>
+      </c>
+      <c r="E167" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="F167" t="s">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="G167" t="s">
         <v>82</v>
       </c>
       <c r="H167" s="4">
-        <v>0</v>
-      </c>
-      <c r="I167" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="J167" s="4">
         <v>0</v>
       </c>
       <c r="K167" s="5"/>
       <c r="L167" s="4">
-        <v>1</v>
-      </c>
-      <c r="M167" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B168" t="s">
         <v>15</v>
@@ -7108,35 +7103,34 @@
         <v>16</v>
       </c>
       <c r="D168" t="s">
-        <v>294</v>
-      </c>
-      <c r="E168" s="3">
-        <v>2020</v>
+        <v>280</v>
+      </c>
+      <c r="E168" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="F168" t="s">
-        <v>295</v>
+        <v>249</v>
       </c>
       <c r="G168" t="s">
         <v>82</v>
       </c>
       <c r="H168" s="4">
-        <v>0</v>
-      </c>
-      <c r="I168" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="J168" s="4">
         <v>0</v>
       </c>
       <c r="K168" s="5"/>
       <c r="L168" s="4">
-        <v>1</v>
-      </c>
-      <c r="M168" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B169" t="s">
         <v>15</v>
@@ -7145,35 +7139,34 @@
         <v>16</v>
       </c>
       <c r="D169" t="s">
-        <v>24</v>
-      </c>
-      <c r="E169" s="3">
-        <v>2020</v>
+        <v>194</v>
+      </c>
+      <c r="E169" s="9" t="s">
+        <v>283</v>
       </c>
       <c r="F169" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
       <c r="G169" t="s">
         <v>82</v>
       </c>
       <c r="H169" s="4">
-        <v>0</v>
-      </c>
-      <c r="I169" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="J169" s="4">
         <v>0</v>
       </c>
       <c r="K169" s="5"/>
       <c r="L169" s="4">
-        <v>1</v>
-      </c>
-      <c r="M169" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B170" t="s">
         <v>15</v>
@@ -7182,35 +7175,36 @@
         <v>16</v>
       </c>
       <c r="D170" t="s">
-        <v>299</v>
-      </c>
-      <c r="E170" s="3">
-        <v>2020</v>
+        <v>50</v>
+      </c>
+      <c r="E170" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="F170" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="G170" t="s">
         <v>82</v>
       </c>
       <c r="H170" s="4">
-        <v>0</v>
-      </c>
-      <c r="I170" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J170" s="4">
-        <v>0</v>
-      </c>
-      <c r="K170" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K170" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L170" s="4">
-        <v>1</v>
-      </c>
-      <c r="M170" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B171" t="s">
         <v>15</v>
@@ -7219,35 +7213,36 @@
         <v>16</v>
       </c>
       <c r="D171" t="s">
-        <v>301</v>
-      </c>
-      <c r="E171" s="3">
-        <v>2020</v>
+        <v>46</v>
+      </c>
+      <c r="E171" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="F171" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="G171" t="s">
         <v>82</v>
       </c>
       <c r="H171" s="4">
-        <v>0</v>
-      </c>
-      <c r="I171" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I171" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J171" s="4">
-        <v>0</v>
-      </c>
-      <c r="K171" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K171" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L171" s="4">
-        <v>1</v>
-      </c>
-      <c r="M171" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="B172" t="s">
         <v>15</v>
@@ -7256,35 +7251,36 @@
         <v>16</v>
       </c>
       <c r="D172" t="s">
-        <v>303</v>
-      </c>
-      <c r="E172" s="3">
-        <v>2015</v>
+        <v>194</v>
+      </c>
+      <c r="E172" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="F172" t="s">
-        <v>304</v>
+        <v>122</v>
+      </c>
+      <c r="G172" t="s">
+        <v>82</v>
       </c>
       <c r="H172" s="4">
-        <v>0</v>
-      </c>
-      <c r="I172" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I172" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J172" s="4">
-        <v>0</v>
-      </c>
-      <c r="K172" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K172" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L172" s="4">
-        <v>1</v>
-      </c>
-      <c r="M172" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N172" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="B173" t="s">
         <v>15</v>
@@ -7293,35 +7289,36 @@
         <v>16</v>
       </c>
       <c r="D173" t="s">
-        <v>307</v>
-      </c>
-      <c r="E173" s="3">
-        <v>2023</v>
+        <v>289</v>
+      </c>
+      <c r="E173" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="F173" t="s">
-        <v>120</v>
+        <v>228</v>
       </c>
       <c r="G173" t="s">
         <v>82</v>
       </c>
       <c r="H173" s="4">
-        <v>0</v>
-      </c>
-      <c r="I173" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I173" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J173" s="4">
-        <v>0</v>
-      </c>
-      <c r="K173" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K173" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L173" s="4">
-        <v>1</v>
-      </c>
-      <c r="M173" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="B174" t="s">
         <v>15</v>
@@ -7330,32 +7327,36 @@
         <v>16</v>
       </c>
       <c r="D174" t="s">
-        <v>310</v>
-      </c>
-      <c r="E174" s="3">
-        <v>2023</v>
+        <v>194</v>
+      </c>
+      <c r="E174" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="F174" t="s">
-        <v>311</v>
+        <v>249</v>
+      </c>
+      <c r="G174" t="s">
+        <v>82</v>
       </c>
       <c r="H174" s="4">
-        <v>0</v>
-      </c>
-      <c r="I174" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I174" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J174" s="4">
-        <v>0</v>
-      </c>
-      <c r="K174" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K174" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L174" s="4">
-        <v>1</v>
-      </c>
-      <c r="M174" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>312</v>
+        <v>361</v>
       </c>
       <c r="B175" t="s">
         <v>15</v>
@@ -7364,35 +7365,33 @@
         <v>16</v>
       </c>
       <c r="D175" t="s">
-        <v>62</v>
-      </c>
-      <c r="E175" s="3">
-        <v>2023</v>
+        <v>194</v>
+      </c>
+      <c r="E175" s="9" t="s">
+        <v>363</v>
       </c>
       <c r="F175" t="s">
-        <v>126</v>
-      </c>
-      <c r="G175" t="s">
-        <v>82</v>
+        <v>362</v>
       </c>
       <c r="H175" s="4">
-        <v>0</v>
-      </c>
-      <c r="I175" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I175" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J175" s="4">
-        <v>0</v>
-      </c>
-      <c r="K175" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K175" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L175" s="4">
-        <v>1</v>
-      </c>
-      <c r="M175" s="5" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>314</v>
+        <v>374</v>
       </c>
       <c r="B176" t="s">
         <v>15</v>
@@ -7401,35 +7400,33 @@
         <v>16</v>
       </c>
       <c r="D176" t="s">
-        <v>138</v>
-      </c>
-      <c r="E176" s="3">
-        <v>2023</v>
+        <v>194</v>
+      </c>
+      <c r="E176" s="9" t="s">
+        <v>375</v>
       </c>
       <c r="F176" t="s">
-        <v>126</v>
-      </c>
-      <c r="G176" t="s">
-        <v>82</v>
+        <v>373</v>
       </c>
       <c r="H176" s="4">
-        <v>0</v>
-      </c>
-      <c r="I176" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="I176" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="J176" s="4">
-        <v>0</v>
-      </c>
-      <c r="K176" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="K176" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L176" s="4">
-        <v>1</v>
-      </c>
-      <c r="M176" s="5" t="s">
-        <v>313</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="B177" t="s">
         <v>15</v>
@@ -7438,13 +7435,13 @@
         <v>16</v>
       </c>
       <c r="D177" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="E177" s="3">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="F177" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G177" t="s">
         <v>82</v>
@@ -7461,12 +7458,12 @@
         <v>1</v>
       </c>
       <c r="M177" s="5" t="s">
-        <v>313</v>
+        <v>26</v>
       </c>
     </row>
     <row r="178" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="B178" t="s">
         <v>15</v>
@@ -7475,13 +7472,13 @@
         <v>16</v>
       </c>
       <c r="D178" t="s">
-        <v>74</v>
+        <v>294</v>
       </c>
       <c r="E178" s="3">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="F178" t="s">
-        <v>126</v>
+        <v>295</v>
       </c>
       <c r="G178" t="s">
         <v>82</v>
@@ -7498,12 +7495,12 @@
         <v>1</v>
       </c>
       <c r="M178" s="5" t="s">
-        <v>313</v>
+        <v>26</v>
       </c>
     </row>
     <row r="179" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="B179" t="s">
         <v>15</v>
@@ -7512,13 +7509,13 @@
         <v>16</v>
       </c>
       <c r="D179" t="s">
-        <v>318</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>319</v>
+        <v>24</v>
+      </c>
+      <c r="E179" s="3">
+        <v>2020</v>
       </c>
       <c r="F179" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="G179" t="s">
         <v>82</v>
@@ -7535,12 +7532,12 @@
         <v>1</v>
       </c>
       <c r="M179" s="5" t="s">
-        <v>313</v>
+        <v>26</v>
       </c>
     </row>
     <row r="180" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="B180" t="s">
         <v>15</v>
@@ -7549,13 +7546,13 @@
         <v>16</v>
       </c>
       <c r="D180" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="E180" s="3">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="F180" t="s">
-        <v>322</v>
+        <v>114</v>
       </c>
       <c r="G180" t="s">
         <v>82</v>
@@ -7572,314 +7569,394 @@
         <v>1</v>
       </c>
       <c r="M180" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="N180" t="s">
-        <v>324</v>
+        <v>28</v>
       </c>
     </row>
     <row r="181" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="B181" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C181" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="D181" t="s">
-        <v>326</v>
-      </c>
-      <c r="E181" s="9" t="s">
-        <v>79</v>
+        <v>301</v>
+      </c>
+      <c r="E181" s="3">
+        <v>2020</v>
       </c>
       <c r="F181" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="G181" t="s">
         <v>82</v>
       </c>
-      <c r="H181" s="3"/>
-      <c r="J181" s="3"/>
-      <c r="L181" s="3"/>
-      <c r="N181" t="s">
-        <v>102</v>
+      <c r="H181" s="4">
+        <v>0</v>
+      </c>
+      <c r="I181" s="5"/>
+      <c r="J181" s="4">
+        <v>0</v>
+      </c>
+      <c r="K181" s="5"/>
+      <c r="L181" s="4">
+        <v>1</v>
+      </c>
+      <c r="M181" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="182" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>359</v>
+        <v>302</v>
       </c>
       <c r="B182" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C182" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="D182" t="s">
-        <v>360</v>
-      </c>
-      <c r="E182" s="3" t="s">
-        <v>79</v>
+        <v>303</v>
+      </c>
+      <c r="E182" s="3">
+        <v>2015</v>
       </c>
       <c r="F182" t="s">
-        <v>81</v>
-      </c>
-      <c r="H182" s="4"/>
+        <v>304</v>
+      </c>
+      <c r="H182" s="4">
+        <v>0</v>
+      </c>
       <c r="I182" s="5"/>
-      <c r="J182" s="4"/>
+      <c r="J182" s="4">
+        <v>0</v>
+      </c>
       <c r="K182" s="5"/>
-      <c r="L182" s="4"/>
-      <c r="M182" s="5"/>
+      <c r="L182" s="4">
+        <v>1</v>
+      </c>
+      <c r="M182" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N182" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="183" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B183" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C183" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D183" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="E183" s="3">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F183" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="G183" t="s">
         <v>82</v>
       </c>
-      <c r="H183" s="3"/>
-      <c r="J183" s="3"/>
-      <c r="L183" s="3"/>
-      <c r="N183" t="s">
-        <v>330</v>
+      <c r="H183" s="4">
+        <v>0</v>
+      </c>
+      <c r="I183" s="5"/>
+      <c r="J183" s="4">
+        <v>0</v>
+      </c>
+      <c r="K183" s="5"/>
+      <c r="L183" s="4">
+        <v>1</v>
+      </c>
+      <c r="M183" s="5" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="B184" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C184" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D184" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="E184" s="3">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F184" t="s">
-        <v>81</v>
-      </c>
-      <c r="G184" t="s">
-        <v>82</v>
-      </c>
-      <c r="H184" s="3"/>
-      <c r="J184" s="3"/>
-      <c r="L184" s="3"/>
-      <c r="N184" t="s">
-        <v>330</v>
+        <v>311</v>
+      </c>
+      <c r="H184" s="4">
+        <v>0</v>
+      </c>
+      <c r="I184" s="5"/>
+      <c r="J184" s="4">
+        <v>0</v>
+      </c>
+      <c r="K184" s="5"/>
+      <c r="L184" s="4">
+        <v>1</v>
+      </c>
+      <c r="M184" s="5" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="185" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="B185" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C185" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D185" t="s">
-        <v>334</v>
-      </c>
-      <c r="E185" s="9" t="s">
-        <v>276</v>
+        <v>62</v>
+      </c>
+      <c r="E185" s="3">
+        <v>2023</v>
       </c>
       <c r="F185" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="G185" t="s">
         <v>82</v>
       </c>
-      <c r="H185" s="3"/>
-      <c r="J185" s="3"/>
-      <c r="L185" s="3"/>
-      <c r="N185" t="s">
-        <v>330</v>
+      <c r="H185" s="4">
+        <v>0</v>
+      </c>
+      <c r="I185" s="5"/>
+      <c r="J185" s="4">
+        <v>0</v>
+      </c>
+      <c r="K185" s="5"/>
+      <c r="L185" s="4">
+        <v>1</v>
+      </c>
+      <c r="M185" s="5" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="186" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="B186" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C186" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D186" t="s">
-        <v>334</v>
-      </c>
-      <c r="E186" s="9" t="s">
-        <v>336</v>
+        <v>138</v>
+      </c>
+      <c r="E186" s="3">
+        <v>2023</v>
       </c>
       <c r="F186" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="G186" t="s">
         <v>82</v>
       </c>
-      <c r="H186" s="3"/>
-      <c r="J186" s="3"/>
-      <c r="L186" s="3"/>
-      <c r="N186" t="s">
-        <v>330</v>
+      <c r="H186" s="4">
+        <v>0</v>
+      </c>
+      <c r="I186" s="5"/>
+      <c r="J186" s="4">
+        <v>0</v>
+      </c>
+      <c r="K186" s="5"/>
+      <c r="L186" s="4">
+        <v>1</v>
+      </c>
+      <c r="M186" s="5" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="187" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="B187" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C187" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D187" t="s">
-        <v>338</v>
+        <v>60</v>
       </c>
       <c r="E187" s="3">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F187" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="G187" t="s">
         <v>82</v>
       </c>
-      <c r="H187" s="3"/>
-      <c r="J187" s="3"/>
-      <c r="L187" s="3"/>
-      <c r="N187" t="s">
-        <v>330</v>
+      <c r="H187" s="4">
+        <v>0</v>
+      </c>
+      <c r="I187" s="5"/>
+      <c r="J187" s="4">
+        <v>0</v>
+      </c>
+      <c r="K187" s="5"/>
+      <c r="L187" s="4">
+        <v>1</v>
+      </c>
+      <c r="M187" s="5" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="188" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="B188" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C188" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D188" t="s">
-        <v>340</v>
+        <v>74</v>
       </c>
       <c r="E188" s="3">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F188" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="G188" t="s">
         <v>82</v>
       </c>
-      <c r="H188" s="3"/>
-      <c r="J188" s="3"/>
-      <c r="L188" s="3"/>
-      <c r="N188" t="s">
-        <v>330</v>
+      <c r="H188" s="4">
+        <v>0</v>
+      </c>
+      <c r="I188" s="5"/>
+      <c r="J188" s="4">
+        <v>0</v>
+      </c>
+      <c r="K188" s="5"/>
+      <c r="L188" s="4">
+        <v>1</v>
+      </c>
+      <c r="M188" s="5" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="189" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="B189" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C189" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D189" t="s">
-        <v>342</v>
-      </c>
-      <c r="E189" s="3">
-        <v>2020</v>
+        <v>318</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>319</v>
       </c>
       <c r="F189" t="s">
-        <v>81</v>
+        <v>311</v>
       </c>
       <c r="G189" t="s">
         <v>82</v>
       </c>
-      <c r="H189" s="3"/>
-      <c r="J189" s="3"/>
-      <c r="L189" s="3"/>
-      <c r="N189" t="s">
-        <v>330</v>
+      <c r="H189" s="4">
+        <v>0</v>
+      </c>
+      <c r="I189" s="5"/>
+      <c r="J189" s="4">
+        <v>0</v>
+      </c>
+      <c r="K189" s="5"/>
+      <c r="L189" s="4">
+        <v>1</v>
+      </c>
+      <c r="M189" s="5" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="190" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="B190" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="C190" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
       <c r="D190" t="s">
-        <v>342</v>
-      </c>
-      <c r="E190" s="9" t="s">
-        <v>336</v>
+        <v>321</v>
+      </c>
+      <c r="E190" s="3">
+        <v>2015</v>
       </c>
       <c r="F190" t="s">
-        <v>81</v>
+        <v>322</v>
       </c>
       <c r="G190" t="s">
         <v>82</v>
       </c>
-      <c r="H190" s="3"/>
-      <c r="J190" s="3"/>
-      <c r="L190" s="3"/>
+      <c r="H190" s="4">
+        <v>0</v>
+      </c>
+      <c r="I190" s="5"/>
+      <c r="J190" s="4">
+        <v>0</v>
+      </c>
+      <c r="K190" s="5"/>
+      <c r="L190" s="4">
+        <v>1</v>
+      </c>
+      <c r="M190" s="5" t="s">
+        <v>323</v>
+      </c>
       <c r="N190" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="191" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="B191" t="s">
         <v>84</v>
       </c>
       <c r="C191" t="s">
-        <v>328</v>
+        <v>79</v>
       </c>
       <c r="D191" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E191" s="9" t="s">
-        <v>336</v>
+        <v>79</v>
       </c>
       <c r="F191" t="s">
         <v>81</v>
@@ -7891,41 +7968,38 @@
       <c r="J191" s="3"/>
       <c r="L191" s="3"/>
       <c r="N191" t="s">
-        <v>330</v>
+        <v>102</v>
       </c>
     </row>
     <row r="192" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="B192" t="s">
         <v>84</v>
       </c>
       <c r="C192" t="s">
-        <v>328</v>
+        <v>79</v>
       </c>
       <c r="D192" t="s">
-        <v>346</v>
-      </c>
-      <c r="E192" s="9" t="s">
-        <v>336</v>
+        <v>360</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F192" t="s">
         <v>81</v>
       </c>
-      <c r="G192" t="s">
-        <v>82</v>
-      </c>
-      <c r="H192" s="3"/>
-      <c r="J192" s="3"/>
-      <c r="L192" s="3"/>
-      <c r="N192" t="s">
-        <v>330</v>
-      </c>
+      <c r="H192" s="4"/>
+      <c r="I192" s="5"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="5"/>
+      <c r="L192" s="4"/>
+      <c r="M192" s="5"/>
     </row>
     <row r="193" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B193" t="s">
         <v>84</v>
@@ -7934,10 +8008,10 @@
         <v>328</v>
       </c>
       <c r="D193" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="E193" s="3">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="F193" t="s">
         <v>81</v>
@@ -7954,19 +8028,19 @@
     </row>
     <row r="194" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="B194" t="s">
         <v>84</v>
       </c>
       <c r="C194" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D194" t="s">
-        <v>351</v>
-      </c>
-      <c r="E194" s="9" t="s">
-        <v>79</v>
+        <v>332</v>
+      </c>
+      <c r="E194" s="3">
+        <v>2020</v>
       </c>
       <c r="F194" t="s">
         <v>81</v>
@@ -7978,24 +8052,24 @@
       <c r="J194" s="3"/>
       <c r="L194" s="3"/>
       <c r="N194" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
     </row>
     <row r="195" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="B195" t="s">
         <v>84</v>
       </c>
       <c r="C195" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D195" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="E195" s="9" t="s">
-        <v>79</v>
+        <v>276</v>
       </c>
       <c r="F195" t="s">
         <v>81</v>
@@ -8007,24 +8081,24 @@
       <c r="J195" s="3"/>
       <c r="L195" s="3"/>
       <c r="N195" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="196" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="B196" t="s">
         <v>84</v>
       </c>
       <c r="C196" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D196" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="E196" s="9" t="s">
-        <v>79</v>
+        <v>336</v>
       </c>
       <c r="F196" t="s">
         <v>81</v>
@@ -8036,11 +8110,303 @@
       <c r="J196" s="3"/>
       <c r="L196" s="3"/>
       <c r="N196" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>337</v>
+      </c>
+      <c r="B197" t="s">
+        <v>84</v>
+      </c>
+      <c r="C197" t="s">
+        <v>328</v>
+      </c>
+      <c r="D197" t="s">
+        <v>338</v>
+      </c>
+      <c r="E197" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F197" t="s">
+        <v>81</v>
+      </c>
+      <c r="G197" t="s">
+        <v>82</v>
+      </c>
+      <c r="H197" s="3"/>
+      <c r="J197" s="3"/>
+      <c r="L197" s="3"/>
+      <c r="N197" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>339</v>
+      </c>
+      <c r="B198" t="s">
+        <v>84</v>
+      </c>
+      <c r="C198" t="s">
+        <v>328</v>
+      </c>
+      <c r="D198" t="s">
+        <v>340</v>
+      </c>
+      <c r="E198" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F198" t="s">
+        <v>81</v>
+      </c>
+      <c r="G198" t="s">
+        <v>82</v>
+      </c>
+      <c r="H198" s="3"/>
+      <c r="J198" s="3"/>
+      <c r="L198" s="3"/>
+      <c r="N198" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>341</v>
+      </c>
+      <c r="B199" t="s">
+        <v>84</v>
+      </c>
+      <c r="C199" t="s">
+        <v>328</v>
+      </c>
+      <c r="D199" t="s">
+        <v>342</v>
+      </c>
+      <c r="E199" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F199" t="s">
+        <v>81</v>
+      </c>
+      <c r="G199" t="s">
+        <v>82</v>
+      </c>
+      <c r="H199" s="3"/>
+      <c r="J199" s="3"/>
+      <c r="L199" s="3"/>
+      <c r="N199" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>343</v>
+      </c>
+      <c r="B200" t="s">
+        <v>84</v>
+      </c>
+      <c r="C200" t="s">
+        <v>328</v>
+      </c>
+      <c r="D200" t="s">
+        <v>342</v>
+      </c>
+      <c r="E200" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="F200" t="s">
+        <v>81</v>
+      </c>
+      <c r="G200" t="s">
+        <v>82</v>
+      </c>
+      <c r="H200" s="3"/>
+      <c r="J200" s="3"/>
+      <c r="L200" s="3"/>
+      <c r="N200" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>344</v>
+      </c>
+      <c r="B201" t="s">
+        <v>84</v>
+      </c>
+      <c r="C201" t="s">
+        <v>328</v>
+      </c>
+      <c r="D201" t="s">
+        <v>329</v>
+      </c>
+      <c r="E201" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="F201" t="s">
+        <v>81</v>
+      </c>
+      <c r="G201" t="s">
+        <v>82</v>
+      </c>
+      <c r="H201" s="3"/>
+      <c r="J201" s="3"/>
+      <c r="L201" s="3"/>
+      <c r="N201" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>345</v>
+      </c>
+      <c r="B202" t="s">
+        <v>84</v>
+      </c>
+      <c r="C202" t="s">
+        <v>328</v>
+      </c>
+      <c r="D202" t="s">
+        <v>346</v>
+      </c>
+      <c r="E202" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="F202" t="s">
+        <v>81</v>
+      </c>
+      <c r="G202" t="s">
+        <v>82</v>
+      </c>
+      <c r="H202" s="3"/>
+      <c r="J202" s="3"/>
+      <c r="L202" s="3"/>
+      <c r="N202" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>347</v>
+      </c>
+      <c r="B203" t="s">
+        <v>84</v>
+      </c>
+      <c r="C203" t="s">
+        <v>328</v>
+      </c>
+      <c r="D203" t="s">
+        <v>348</v>
+      </c>
+      <c r="E203" s="3">
+        <v>2015</v>
+      </c>
+      <c r="F203" t="s">
+        <v>81</v>
+      </c>
+      <c r="G203" t="s">
+        <v>82</v>
+      </c>
+      <c r="H203" s="3"/>
+      <c r="J203" s="3"/>
+      <c r="L203" s="3"/>
+      <c r="N203" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>349</v>
+      </c>
+      <c r="B204" t="s">
+        <v>84</v>
+      </c>
+      <c r="C204" t="s">
+        <v>350</v>
+      </c>
+      <c r="D204" t="s">
+        <v>351</v>
+      </c>
+      <c r="E204" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F204" t="s">
+        <v>81</v>
+      </c>
+      <c r="G204" t="s">
+        <v>82</v>
+      </c>
+      <c r="H204" s="3"/>
+      <c r="J204" s="3"/>
+      <c r="L204" s="3"/>
+      <c r="N204" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>353</v>
+      </c>
+      <c r="B205" t="s">
+        <v>84</v>
+      </c>
+      <c r="C205" t="s">
+        <v>350</v>
+      </c>
+      <c r="D205" t="s">
+        <v>354</v>
+      </c>
+      <c r="E205" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F205" t="s">
+        <v>81</v>
+      </c>
+      <c r="G205" t="s">
+        <v>82</v>
+      </c>
+      <c r="H205" s="3"/>
+      <c r="J205" s="3"/>
+      <c r="L205" s="3"/>
+      <c r="N205" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>356</v>
+      </c>
+      <c r="B206" t="s">
+        <v>84</v>
+      </c>
+      <c r="C206" t="s">
+        <v>350</v>
+      </c>
+      <c r="D206" t="s">
+        <v>357</v>
+      </c>
+      <c r="E206" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F206" t="s">
+        <v>81</v>
+      </c>
+      <c r="G206" t="s">
+        <v>82</v>
+      </c>
+      <c r="H206" s="3"/>
+      <c r="J206" s="3"/>
+      <c r="L206" s="3"/>
+      <c r="N206" t="s">
         <v>358</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated missing cameroon dataset from whisp_columns.xlsx
</commit_message>
<xml_diff>
--- a/whisp_columns.xlsx
+++ b/whisp_columns.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CAFD05-62BA-4718-B43D-46F81171967B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DDF8C9-FFFF-4F96-A986-405CD27793AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="whisp outputs global" sheetId="1" r:id="rId1"/>
+    <sheet name="whisp outputs standard" sheetId="1" r:id="rId1"/>
     <sheet name="whisp outputs national" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="399">
   <si>
     <t>Column name</t>
   </si>
@@ -1094,9 +1094,6 @@
     <t>nCO_ideam_eufo_commission_2020</t>
   </si>
   <si>
-    <t>Area of Treecover outside EUFO</t>
-  </si>
-  <si>
     <t>nBR_INPE_TC_primary_forest_Amazon_2020</t>
   </si>
   <si>
@@ -1212,6 +1209,15 @@
   </si>
   <si>
     <t>BNETD 2020.</t>
+  </si>
+  <si>
+    <t>Area of Tree cover outside EUFO</t>
+  </si>
+  <si>
+    <t>nCM_Treecover_2020</t>
+  </si>
+  <si>
+    <t>Area of Treecover</t>
   </si>
 </sst>
 </file>
@@ -1233,14 +1239,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1309,26 +1315,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8311,1115 +8315,1202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C9A24C-67E0-477E-A2C1-2524EF892E56}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>2020</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="5">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>356</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="L3" s="6">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="4">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="5">
         <v>2020</v>
       </c>
-      <c r="F3" t="s">
-        <v>355</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="F4" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="6">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="6">
+        <v>1</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="L15" s="6">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="J16" s="6">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="L16" s="6">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L17" s="6">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J18" s="6">
+        <v>1</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L18" s="6">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="5">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="J19" s="6">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="5">
-        <v>1</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="L19" s="6">
+        <v>1</v>
+      </c>
+      <c r="M19" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="4">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="5">
         <v>2020</v>
       </c>
-      <c r="F4" t="s">
-        <v>359</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="F20" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="6">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="6">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J21" s="6">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="6">
+        <v>1</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="6">
+        <v>1</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" s="6">
+        <v>1</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="6">
+        <v>1</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E23" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="6">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="6">
+        <v>1</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L24" s="6">
+        <v>1</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E25" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="6">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" s="6">
+        <v>1</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="6">
+        <v>1</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E26" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="6">
+        <v>1</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L26" s="6">
+        <v>1</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E27" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L27" s="6">
+        <v>1</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E28" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="6">
+        <v>1</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="6">
+        <v>1</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L28" s="6">
+        <v>1</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L29" s="6">
+        <v>1</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E30" s="5">
+        <v>2020</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="6">
+        <v>1</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="5">
-        <v>1</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="J30" s="6">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="5">
-        <v>1</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F5" t="s">
-        <v>359</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="L30" s="6">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L5" s="5">
-        <v>1</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>361</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F6" t="s">
-        <v>362</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>363</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F7" t="s">
-        <v>362</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>364</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F8" t="s">
-        <v>362</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="5">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>365</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F9" t="s">
-        <v>362</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>366</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F10" t="s">
-        <v>362</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>367</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F11" t="s">
-        <v>368</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="5">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>369</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F12" t="s">
-        <v>370</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="5">
-        <v>1</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>371</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F13" t="s">
-        <v>372</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="5">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="5">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>373</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F14" t="s">
-        <v>368</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="5">
-        <v>1</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14" s="5">
-        <v>1</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>374</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="F15" t="s">
-        <v>359</v>
-      </c>
-      <c r="H15" s="5">
-        <v>1</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="L15" s="5">
-        <v>1</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>376</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="F16" t="s">
-        <v>378</v>
-      </c>
-      <c r="H16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="J16" s="5">
-        <v>1</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>379</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F17" t="s">
-        <v>359</v>
-      </c>
-      <c r="H17" s="5">
-        <v>1</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="J17" s="5">
-        <v>1</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>381</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="F18" t="s">
-        <v>378</v>
-      </c>
-      <c r="H18" s="5">
-        <v>1</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="J18" s="5">
-        <v>1</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="L18" s="5">
-        <v>1</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>382</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>383</v>
-      </c>
-      <c r="E19" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F19" t="s">
-        <v>370</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19" s="5">
-        <v>1</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>384</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F20" t="s">
-        <v>368</v>
-      </c>
-      <c r="H20" s="5">
-        <v>1</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J20" s="5">
-        <v>1</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>385</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F21" t="s">
-        <v>368</v>
-      </c>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J21" s="5">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>386</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
-        <v>383</v>
-      </c>
-      <c r="E22" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F22" t="s">
-        <v>368</v>
-      </c>
-      <c r="H22" s="5">
-        <v>1</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J22" s="5">
-        <v>1</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>387</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>388</v>
-      </c>
-      <c r="E23" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F23" t="s">
-        <v>370</v>
-      </c>
-      <c r="H23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J23" s="5">
-        <v>1</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>389</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H24" s="5">
-        <v>1</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J24" s="5">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>390</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>388</v>
-      </c>
-      <c r="E25" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F25" t="s">
-        <v>368</v>
-      </c>
-      <c r="H25" s="5">
-        <v>1</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="5">
-        <v>1</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>391</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
-        <v>392</v>
-      </c>
-      <c r="E26" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F26" t="s">
-        <v>370</v>
-      </c>
-      <c r="H26" s="5">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" s="5">
-        <v>1</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>393</v>
-      </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>392</v>
-      </c>
-      <c r="E27" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F27" t="s">
-        <v>372</v>
-      </c>
-      <c r="H27" s="5">
-        <v>1</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J27" s="5">
-        <v>1</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>394</v>
-      </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>392</v>
-      </c>
-      <c r="E28" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F28" t="s">
-        <v>368</v>
-      </c>
-      <c r="H28" s="5">
-        <v>1</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J28" s="5">
-        <v>1</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L28" s="5">
-        <v>1</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>395</v>
-      </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="4">
-        <v>2020</v>
-      </c>
-      <c r="F29" t="s">
-        <v>396</v>
-      </c>
-      <c r="H29" s="5">
-        <v>1</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J29" s="5">
-        <v>1</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L29" s="5">
-        <v>1</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>